<commit_message>
Created list of profiles to fix
</commit_message>
<xml_diff>
--- a/resources/db/Profiles.xlsx
+++ b/resources/db/Profiles.xlsx
@@ -5,16 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ing-my.sharepoint.com/personal/torsten_wiederkehr_ing_com/Documents/Documents/Eigene Dateien/learnING/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IN57KC\data\Projekte\csharp\ArmyBuilder\resources\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="127" documentId="8_{0CC64012-35A4-4744-B15A-B962C9CF06E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CA8EE6D-9014-433C-8971-5F4285C73C7D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699E714F-1860-42C4-A77B-2AFCDA228FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{72821A2A-92BA-4C26-854D-A2ECB76DE865}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="2" xr2:uid="{72821A2A-92BA-4C26-854D-A2ECB76DE865}"/>
   </bookViews>
   <sheets>
     <sheet name="High Elf Profiles" sheetId="1" r:id="rId1"/>
-    <sheet name="High Elf Points" sheetId="2" r:id="rId2"/>
+    <sheet name="High Elf Fixed Profiles" sheetId="3" r:id="rId2"/>
+    <sheet name="High Elf Wrong Profiles" sheetId="4" r:id="rId3"/>
+    <sheet name="High Elf Points" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="123">
   <si>
     <t>Hochelfen</t>
   </si>
@@ -787,13 +789,14 @@
   <dimension ref="A1:H84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="42.28515625" customWidth="1"/>
+    <col min="6" max="6" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2989,10 +2992,1499 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A1C7FE9-57C8-4B20-B5A5-F2082127AA84}">
+  <dimension ref="A1:E33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11693</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2">
+        <v>46368</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2">
+        <v>11693</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>11692</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3">
+        <v>46367</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3">
+        <v>11692</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>11507</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>46492</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>11507</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>12243</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5">
+        <v>47180</v>
+      </c>
+      <c r="D5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5">
+        <v>12415</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>11694</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6">
+        <v>46369</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6">
+        <v>11694</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>11906</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7">
+        <v>46816</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7">
+        <v>11906</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>11696</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8">
+        <v>46371</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8">
+        <v>11696</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>11509</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>46494</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9">
+        <v>11509</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>12236</v>
+      </c>
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10">
+        <v>47173</v>
+      </c>
+      <c r="D10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10">
+        <v>12414</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>12286</v>
+      </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11">
+        <v>47223</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11">
+        <v>12416</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12163</v>
+      </c>
+      <c r="B12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12">
+        <v>46730</v>
+      </c>
+      <c r="D12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12">
+        <v>12163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11506</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>46491</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>11506</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12269</v>
+      </c>
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14">
+        <v>47206</v>
+      </c>
+      <c r="D14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14">
+        <v>12419</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>12294</v>
+      </c>
+      <c r="B15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15">
+        <v>47321</v>
+      </c>
+      <c r="D15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15">
+        <v>12417</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>11512</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>46497</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16">
+        <v>11512</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>11508</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>46493</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>11508</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>12278</v>
+      </c>
+      <c r="B18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18">
+        <v>47215</v>
+      </c>
+      <c r="D18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18">
+        <v>12420</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>11980</v>
+      </c>
+      <c r="B19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19">
+        <v>46946</v>
+      </c>
+      <c r="D19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19">
+        <v>11980</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>12302</v>
+      </c>
+      <c r="B20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20">
+        <v>47329</v>
+      </c>
+      <c r="D20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20">
+        <v>12418</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>11695</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21">
+        <v>46370</v>
+      </c>
+      <c r="D21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21">
+        <v>11695</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>12250</v>
+      </c>
+      <c r="B22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22">
+        <v>47187</v>
+      </c>
+      <c r="D22" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22">
+        <v>12422</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>11513</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23">
+        <v>46498</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23">
+        <v>11513</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>11511</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>46496</v>
+      </c>
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24">
+        <v>11511</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>12167</v>
+      </c>
+      <c r="B25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25">
+        <v>46734</v>
+      </c>
+      <c r="D25" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25">
+        <v>12336</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>11902</v>
+      </c>
+      <c r="B26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26">
+        <v>46812</v>
+      </c>
+      <c r="D26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26">
+        <v>11902</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>11517</v>
+      </c>
+      <c r="B27" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27">
+        <v>46502</v>
+      </c>
+      <c r="D27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27">
+        <v>11517</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>12162</v>
+      </c>
+      <c r="B28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28">
+        <v>46729</v>
+      </c>
+      <c r="D28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28">
+        <v>12162</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>11907</v>
+      </c>
+      <c r="B29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29">
+        <v>46817</v>
+      </c>
+      <c r="D29" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29">
+        <v>11907</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>11905</v>
+      </c>
+      <c r="B30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30">
+        <v>46815</v>
+      </c>
+      <c r="D30" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30">
+        <v>11905</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>11904</v>
+      </c>
+      <c r="B31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31">
+        <v>46814</v>
+      </c>
+      <c r="D31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31">
+        <v>11904</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>11515</v>
+      </c>
+      <c r="B32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32">
+        <v>46500</v>
+      </c>
+      <c r="D32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32">
+        <v>11515</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>11510</v>
+      </c>
+      <c r="B33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33">
+        <v>46495</v>
+      </c>
+      <c r="D33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33">
+        <v>11510</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E36">
+    <sortCondition ref="B2:B36"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B274CE33-7099-4094-9D9A-29DF4F468E02}">
+  <dimension ref="A1:E53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="45.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11516</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2">
+        <v>46501</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2">
+        <v>11516</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>11516</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>46839</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3">
+        <v>11804</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>11514</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>46499</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>11514</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>11514</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>46838</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>11803</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>11900</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6">
+        <v>46710</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6">
+        <v>12036</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>11900</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7">
+        <v>46810</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7">
+        <v>11900</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>12585</v>
+      </c>
+      <c r="B8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8">
+        <v>47556</v>
+      </c>
+      <c r="D8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8">
+        <v>12585</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>12585</v>
+      </c>
+      <c r="B9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9">
+        <v>47603</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9">
+        <v>12034</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>12466</v>
+      </c>
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10">
+        <v>47437</v>
+      </c>
+      <c r="D10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10">
+        <v>12466</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>12466</v>
+      </c>
+      <c r="B11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11">
+        <v>47604</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11">
+        <v>12034</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11898</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12">
+        <v>46708</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12">
+        <v>12034</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11898</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13">
+        <v>46808</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13">
+        <v>11898</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12583</v>
+      </c>
+      <c r="B14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14">
+        <v>47554</v>
+      </c>
+      <c r="D14" t="s">
+        <v>93</v>
+      </c>
+      <c r="E14">
+        <v>12583</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>12583</v>
+      </c>
+      <c r="B15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15">
+        <v>47600</v>
+      </c>
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15">
+        <v>12034</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>12464</v>
+      </c>
+      <c r="B16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16">
+        <v>47435</v>
+      </c>
+      <c r="D16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16">
+        <v>12464</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>12464</v>
+      </c>
+      <c r="B17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17">
+        <v>47599</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17">
+        <v>12034</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>11901</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18">
+        <v>46811</v>
+      </c>
+      <c r="D18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18">
+        <v>11901</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>12586</v>
+      </c>
+      <c r="B19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19">
+        <v>47557</v>
+      </c>
+      <c r="D19" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19">
+        <v>12586</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>12467</v>
+      </c>
+      <c r="B20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20">
+        <v>47438</v>
+      </c>
+      <c r="D20" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20">
+        <v>12467</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>11899</v>
+      </c>
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21">
+        <v>46709</v>
+      </c>
+      <c r="D21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21">
+        <v>12034</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>11899</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22">
+        <v>46809</v>
+      </c>
+      <c r="D22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22">
+        <v>11899</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>12584</v>
+      </c>
+      <c r="B23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23">
+        <v>47555</v>
+      </c>
+      <c r="D23" t="s">
+        <v>95</v>
+      </c>
+      <c r="E23">
+        <v>12584</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>12584</v>
+      </c>
+      <c r="B24" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24">
+        <v>47601</v>
+      </c>
+      <c r="D24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24">
+        <v>12034</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>12465</v>
+      </c>
+      <c r="B25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25">
+        <v>47436</v>
+      </c>
+      <c r="D25" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25">
+        <v>12465</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>12465</v>
+      </c>
+      <c r="B26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26">
+        <v>47602</v>
+      </c>
+      <c r="D26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26">
+        <v>12034</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>11903</v>
+      </c>
+      <c r="B27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27">
+        <v>46813</v>
+      </c>
+      <c r="D27" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27">
+        <v>11903</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>12588</v>
+      </c>
+      <c r="B28" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28">
+        <v>47559</v>
+      </c>
+      <c r="D28" t="s">
+        <v>102</v>
+      </c>
+      <c r="E28">
+        <v>12588</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>12469</v>
+      </c>
+      <c r="B29" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29">
+        <v>47440</v>
+      </c>
+      <c r="D29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E29">
+        <v>12469</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>11997</v>
+      </c>
+      <c r="B30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30">
+        <v>46963</v>
+      </c>
+      <c r="D30" t="s">
+        <v>52</v>
+      </c>
+      <c r="E30">
+        <v>11997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>12652</v>
+      </c>
+      <c r="B31" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31">
+        <v>47390</v>
+      </c>
+      <c r="D31" t="s">
+        <v>111</v>
+      </c>
+      <c r="E31">
+        <v>12652</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>12533</v>
+      </c>
+      <c r="B32" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32">
+        <v>47504</v>
+      </c>
+      <c r="D32" t="s">
+        <v>91</v>
+      </c>
+      <c r="E32">
+        <v>12533</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>12113</v>
+      </c>
+      <c r="B33" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33">
+        <v>46726</v>
+      </c>
+      <c r="D33" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33">
+        <v>12159</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>12113</v>
+      </c>
+      <c r="B34" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34">
+        <v>47064</v>
+      </c>
+      <c r="D34" t="s">
+        <v>57</v>
+      </c>
+      <c r="E34">
+        <v>12113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>12113</v>
+      </c>
+      <c r="B35" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35">
+        <v>47127</v>
+      </c>
+      <c r="D35" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35">
+        <v>12034</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>12118</v>
+      </c>
+      <c r="B36" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36">
+        <v>46727</v>
+      </c>
+      <c r="D36" t="s">
+        <v>58</v>
+      </c>
+      <c r="E36">
+        <v>12160</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>12118</v>
+      </c>
+      <c r="B37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37">
+        <v>47069</v>
+      </c>
+      <c r="D37" t="s">
+        <v>57</v>
+      </c>
+      <c r="E37">
+        <v>12113</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>12118</v>
+      </c>
+      <c r="B38" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38">
+        <v>47131</v>
+      </c>
+      <c r="D38" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38">
+        <v>12034</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>12091</v>
+      </c>
+      <c r="B39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39">
+        <v>47014</v>
+      </c>
+      <c r="D39" t="s">
+        <v>54</v>
+      </c>
+      <c r="E39">
+        <v>12091</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>12091</v>
+      </c>
+      <c r="B40" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40">
+        <v>47116</v>
+      </c>
+      <c r="D40" t="s">
+        <v>55</v>
+      </c>
+      <c r="E40">
+        <v>12138</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>12591</v>
+      </c>
+      <c r="B42" t="s">
+        <v>106</v>
+      </c>
+      <c r="C42">
+        <v>47562</v>
+      </c>
+      <c r="D42" t="s">
+        <v>107</v>
+      </c>
+      <c r="E42">
+        <v>12591</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>12472</v>
+      </c>
+      <c r="B43" t="s">
+        <v>86</v>
+      </c>
+      <c r="C43">
+        <v>47443</v>
+      </c>
+      <c r="D43" t="s">
+        <v>87</v>
+      </c>
+      <c r="E43">
+        <v>12472</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>12637</v>
+      </c>
+      <c r="B44" t="s">
+        <v>109</v>
+      </c>
+      <c r="C44">
+        <v>47375</v>
+      </c>
+      <c r="D44" t="s">
+        <v>110</v>
+      </c>
+      <c r="E44">
+        <v>12637</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>12518</v>
+      </c>
+      <c r="B45" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45">
+        <v>47489</v>
+      </c>
+      <c r="D45" t="s">
+        <v>90</v>
+      </c>
+      <c r="E45">
+        <v>12518</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>12587</v>
+      </c>
+      <c r="B46" t="s">
+        <v>100</v>
+      </c>
+      <c r="C46">
+        <v>47558</v>
+      </c>
+      <c r="D46" t="s">
+        <v>100</v>
+      </c>
+      <c r="E46">
+        <v>12587</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>12468</v>
+      </c>
+      <c r="B47" t="s">
+        <v>80</v>
+      </c>
+      <c r="C47">
+        <v>47439</v>
+      </c>
+      <c r="D47" t="s">
+        <v>80</v>
+      </c>
+      <c r="E47">
+        <v>12468</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>12592</v>
+      </c>
+      <c r="B48" t="s">
+        <v>108</v>
+      </c>
+      <c r="C48">
+        <v>47563</v>
+      </c>
+      <c r="D48" t="s">
+        <v>108</v>
+      </c>
+      <c r="E48">
+        <v>12592</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>12473</v>
+      </c>
+      <c r="B49" t="s">
+        <v>88</v>
+      </c>
+      <c r="C49">
+        <v>47444</v>
+      </c>
+      <c r="D49" t="s">
+        <v>88</v>
+      </c>
+      <c r="E49">
+        <v>12473</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>12590</v>
+      </c>
+      <c r="B50" t="s">
+        <v>104</v>
+      </c>
+      <c r="C50">
+        <v>47561</v>
+      </c>
+      <c r="D50" t="s">
+        <v>105</v>
+      </c>
+      <c r="E50">
+        <v>12590</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>12471</v>
+      </c>
+      <c r="B51" t="s">
+        <v>84</v>
+      </c>
+      <c r="C51">
+        <v>47442</v>
+      </c>
+      <c r="D51" t="s">
+        <v>85</v>
+      </c>
+      <c r="E51">
+        <v>12471</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>12589</v>
+      </c>
+      <c r="B52" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52">
+        <v>47560</v>
+      </c>
+      <c r="D52" t="s">
+        <v>103</v>
+      </c>
+      <c r="E52">
+        <v>12589</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>12470</v>
+      </c>
+      <c r="B53" t="s">
+        <v>83</v>
+      </c>
+      <c r="C53">
+        <v>47441</v>
+      </c>
+      <c r="D53" t="s">
+        <v>83</v>
+      </c>
+      <c r="E53">
+        <v>12470</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC3B880E-F91A-4006-A89E-3EF61A46384C}">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J2" sqref="J2:J54"/>
     </sheetView>

</xml_diff>

<commit_message>
Updated profile of Eltharion and Tyrion
</commit_message>
<xml_diff>
--- a/resources/db/Profiles.xlsx
+++ b/resources/db/Profiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IN57KC\data\Projekte\csharp\ArmyBuilder\resources\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699E714F-1860-42C4-A77B-2AFCDA228FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3C3014-CE62-4AFB-8091-5B7B62B17A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="2" xr2:uid="{72821A2A-92BA-4C26-854D-A2ECB76DE865}"/>
   </bookViews>
@@ -3580,10 +3580,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B274CE33-7099-4094-9D9A-29DF4F468E02}">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3591,7 +3591,7 @@
     <col min="2" max="2" width="45.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>114</v>
       </c>
@@ -3608,7 +3608,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11516</v>
       </c>
@@ -3624,8 +3624,18 @@
       <c r="E2">
         <v>11516</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>467</v>
+      </c>
+      <c r="G2">
+        <v>301</v>
+      </c>
+      <c r="H2">
+        <f>F2-G2</f>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>11516</v>
       </c>
@@ -3642,7 +3652,7 @@
         <v>11804</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>11514</v>
       </c>
@@ -3658,8 +3668,18 @@
       <c r="E4">
         <v>11514</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>425</v>
+      </c>
+      <c r="G4">
+        <v>250</v>
+      </c>
+      <c r="H4">
+        <f>F4-G4</f>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>11514</v>
       </c>
@@ -3676,7 +3696,7 @@
         <v>11803</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>11900</v>
       </c>
@@ -3692,8 +3712,14 @@
       <c r="E6">
         <v>12036</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>43</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>11900</v>
       </c>
@@ -3710,7 +3736,7 @@
         <v>11900</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>12585</v>
       </c>
@@ -3727,7 +3753,7 @@
         <v>12585</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>12585</v>
       </c>
@@ -3744,7 +3770,7 @@
         <v>12034</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>12466</v>
       </c>
@@ -3761,7 +3787,7 @@
         <v>12466</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>12466</v>
       </c>
@@ -3778,7 +3804,7 @@
         <v>12034</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11898</v>
       </c>
@@ -3794,8 +3820,14 @@
       <c r="E12">
         <v>12034</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>25</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11898</v>
       </c>
@@ -3812,7 +3844,7 @@
         <v>11898</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12583</v>
       </c>
@@ -3829,7 +3861,7 @@
         <v>12583</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12583</v>
       </c>
@@ -3846,7 +3878,7 @@
         <v>12034</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12464</v>
       </c>
@@ -3863,7 +3895,7 @@
         <v>12464</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>12464</v>
       </c>
@@ -3880,7 +3912,7 @@
         <v>12034</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>11901</v>
       </c>
@@ -3896,8 +3928,14 @@
       <c r="E18">
         <v>11901</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>16</v>
+      </c>
+      <c r="G18">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>12586</v>
       </c>
@@ -3914,7 +3952,7 @@
         <v>12586</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>12467</v>
       </c>
@@ -3931,7 +3969,7 @@
         <v>12467</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>11899</v>
       </c>
@@ -3947,8 +3985,14 @@
       <c r="E21">
         <v>12034</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>31</v>
+      </c>
+      <c r="G21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>11899</v>
       </c>
@@ -3965,7 +4009,7 @@
         <v>11899</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>12584</v>
       </c>
@@ -3982,7 +4026,7 @@
         <v>12584</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>12584</v>
       </c>
@@ -3999,7 +4043,7 @@
         <v>12034</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>12465</v>
       </c>
@@ -4016,7 +4060,7 @@
         <v>12465</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>12465</v>
       </c>
@@ -4033,7 +4077,7 @@
         <v>12034</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>11903</v>
       </c>
@@ -4049,8 +4093,14 @@
       <c r="E27">
         <v>11903</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>16</v>
+      </c>
+      <c r="G27">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>12588</v>
       </c>
@@ -4067,7 +4117,7 @@
         <v>12588</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>12469</v>
       </c>
@@ -4084,7 +4134,7 @@
         <v>12469</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>11997</v>
       </c>
@@ -4100,8 +4150,14 @@
       <c r="E30">
         <v>11997</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>9</v>
+      </c>
+      <c r="G30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>12652</v>
       </c>
@@ -4118,7 +4174,7 @@
         <v>12652</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>12533</v>
       </c>
@@ -4135,7 +4191,7 @@
         <v>12533</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>12113</v>
       </c>
@@ -4151,8 +4207,14 @@
       <c r="E33">
         <v>12159</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>72</v>
+      </c>
+      <c r="G33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>12113</v>
       </c>
@@ -4169,7 +4231,7 @@
         <v>12113</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>12113</v>
       </c>
@@ -4186,7 +4248,7 @@
         <v>12034</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>12118</v>
       </c>
@@ -4202,8 +4264,14 @@
       <c r="E36">
         <v>12160</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>84</v>
+      </c>
+      <c r="G36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>12118</v>
       </c>
@@ -4220,7 +4288,7 @@
         <v>12113</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>12118</v>
       </c>
@@ -4237,7 +4305,7 @@
         <v>12034</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>12091</v>
       </c>
@@ -4253,8 +4321,14 @@
       <c r="E39">
         <v>12091</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>100</v>
+      </c>
+      <c r="G39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>12091</v>
       </c>
@@ -4271,7 +4345,7 @@
         <v>12138</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>12591</v>
       </c>
@@ -4288,7 +4362,7 @@
         <v>12591</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>12472</v>
       </c>
@@ -4305,7 +4379,7 @@
         <v>12472</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>12637</v>
       </c>
@@ -4322,7 +4396,7 @@
         <v>12637</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>12518</v>
       </c>
@@ -4339,7 +4413,7 @@
         <v>12518</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>12587</v>
       </c>
@@ -4356,7 +4430,7 @@
         <v>12587</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>12468</v>
       </c>
@@ -4373,7 +4447,7 @@
         <v>12468</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>12592</v>
       </c>

</xml_diff>

<commit_message>
Filled names of high elf army profiles
</commit_message>
<xml_diff>
--- a/resources/db/Profiles.xlsx
+++ b/resources/db/Profiles.xlsx
@@ -8,16 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IN57KC\data\Projekte\csharp\ArmyBuilder\resources\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66ED7E4F-B72A-4BD4-A6B8-599EBD4A3A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E23472A-D0BA-4842-BC62-0B7C6C4E223D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="2" xr2:uid="{72821A2A-92BA-4C26-854D-A2ECB76DE865}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{72821A2A-92BA-4C26-854D-A2ECB76DE865}"/>
   </bookViews>
   <sheets>
     <sheet name="High Elf Profiles" sheetId="1" r:id="rId1"/>
     <sheet name="High Elf Fixed Profiles" sheetId="3" r:id="rId2"/>
-    <sheet name="High Elf Wrong Profiles" sheetId="4" r:id="rId3"/>
-    <sheet name="High Elf Points" sheetId="2" r:id="rId4"/>
+    <sheet name="Tabelle1" sheetId="5" r:id="rId3"/>
+    <sheet name="High Elf Wrong Profiles" sheetId="4" r:id="rId4"/>
+    <sheet name="High Elf Points" sheetId="2" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Tabelle1!$B$1:$F$73</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="134">
   <si>
     <t>Hochelfen</t>
   </si>
@@ -408,6 +412,39 @@
   </si>
   <si>
     <t>equipment_points</t>
+  </si>
+  <si>
+    <t>profile_name</t>
+  </si>
+  <si>
+    <t>Hochelfen Basis</t>
+  </si>
+  <si>
+    <t>Hochelfen Champion</t>
+  </si>
+  <si>
+    <t>Hochelfen Elite</t>
+  </si>
+  <si>
+    <t>Hochelfen General</t>
+  </si>
+  <si>
+    <t>Hochelfen Großzauberer</t>
+  </si>
+  <si>
+    <t>Hochelfen Held</t>
+  </si>
+  <si>
+    <t>Hochelfen Meisterzauberer</t>
+  </si>
+  <si>
+    <t>Hochelfen Oberzauberer</t>
+  </si>
+  <si>
+    <t>Hochelfen Zauberer</t>
+  </si>
+  <si>
+    <t>Immerkönigin</t>
   </si>
 </sst>
 </file>
@@ -2996,8 +3033,8 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A34" sqref="A34:E43"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3749,10 +3786,1784 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50ABEE1B-A043-4FB5-8D78-6CD44D39B2E7}">
+  <dimension ref="A1:G73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2:G73"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11693</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2">
+        <v>46368</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2">
+        <v>11693</v>
+      </c>
+      <c r="F2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G2" t="str">
+        <f>CONCATENATE("UPDATE profile SET name = '",F2,"' WHERE id = '",E2,"';")</f>
+        <v>UPDATE profile SET name = 'Immerkönigin' WHERE id = '11693';</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>11692</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3">
+        <v>46367</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3">
+        <v>11692</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G66" si="0">CONCATENATE("UPDATE profile SET name = '",F3,"' WHERE id = '",E3,"';")</f>
+        <v>UPDATE profile SET name = 'General' WHERE id = '11692';</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>11507</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>46492</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>11507</v>
+      </c>
+      <c r="F4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Champion' WHERE id = '11507';</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>12243</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5">
+        <v>47180</v>
+      </c>
+      <c r="D5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5">
+        <v>12415</v>
+      </c>
+      <c r="F5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Basilisk' WHERE id = '12415';</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>11694</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6">
+        <v>46369</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6">
+        <v>11694</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Belannaer' WHERE id = '11694';</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>11906</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7">
+        <v>46816</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7">
+        <v>11906</v>
+      </c>
+      <c r="F7" t="s">
+        <v>124</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '11906';</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>12591</v>
+      </c>
+      <c r="B8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8">
+        <v>47562</v>
+      </c>
+      <c r="D8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8">
+        <v>12591</v>
+      </c>
+      <c r="F8" t="s">
+        <v>124</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12591';</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>12472</v>
+      </c>
+      <c r="B9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9">
+        <v>47443</v>
+      </c>
+      <c r="D9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9">
+        <v>12472</v>
+      </c>
+      <c r="F9" t="s">
+        <v>124</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12472';</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>11696</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10">
+        <v>46371</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10">
+        <v>11696</v>
+      </c>
+      <c r="F10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Caradryan' WHERE id = '11696';</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11509</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>46494</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>11509</v>
+      </c>
+      <c r="F11" t="s">
+        <v>125</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Champion' WHERE id = '11509';</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12236</v>
+      </c>
+      <c r="B12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12">
+        <v>47173</v>
+      </c>
+      <c r="D12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12">
+        <v>12414</v>
+      </c>
+      <c r="F12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Chimäre' WHERE id = '12414';</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12286</v>
+      </c>
+      <c r="B13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13">
+        <v>47223</v>
+      </c>
+      <c r="D13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13">
+        <v>12416</v>
+      </c>
+      <c r="F13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Drache' WHERE id = '12416';</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11900</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14">
+        <v>46810</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14">
+        <v>11900</v>
+      </c>
+      <c r="F14" t="s">
+        <v>126</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '11900';</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>12585</v>
+      </c>
+      <c r="B15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15">
+        <v>47556</v>
+      </c>
+      <c r="D15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E15">
+        <v>12585</v>
+      </c>
+      <c r="F15" t="s">
+        <v>126</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '12585';</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>12466</v>
+      </c>
+      <c r="B16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16">
+        <v>47437</v>
+      </c>
+      <c r="D16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16">
+        <v>12466</v>
+      </c>
+      <c r="F16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '12466';</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>12163</v>
+      </c>
+      <c r="B17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17">
+        <v>46730</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17">
+        <v>12163</v>
+      </c>
+      <c r="F17" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Einhorn' WHERE id = '12163';</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>11898</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18">
+        <v>46808</v>
+      </c>
+      <c r="D18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18">
+        <v>11898</v>
+      </c>
+      <c r="F18" t="s">
+        <v>124</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '11898';</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>12583</v>
+      </c>
+      <c r="B19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19">
+        <v>47554</v>
+      </c>
+      <c r="D19" t="s">
+        <v>93</v>
+      </c>
+      <c r="E19">
+        <v>12583</v>
+      </c>
+      <c r="F19" t="s">
+        <v>124</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12583';</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>12464</v>
+      </c>
+      <c r="B20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20">
+        <v>47435</v>
+      </c>
+      <c r="D20" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20">
+        <v>12464</v>
+      </c>
+      <c r="F20" t="s">
+        <v>124</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12464';</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>11516</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21">
+        <v>46501</v>
+      </c>
+      <c r="D21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21">
+        <v>11516</v>
+      </c>
+      <c r="F21" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Greif' WHERE id = '11516';</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>11516</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22">
+        <v>46839</v>
+      </c>
+      <c r="D22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22">
+        <v>11804</v>
+      </c>
+      <c r="F22" t="s">
+        <v>127</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen General' WHERE id = '11804';</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>11506</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>46491</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>11506</v>
+      </c>
+      <c r="F23" t="s">
+        <v>127</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen General' WHERE id = '11506';</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>12269</v>
+      </c>
+      <c r="B24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24">
+        <v>47206</v>
+      </c>
+      <c r="D24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24">
+        <v>12419</v>
+      </c>
+      <c r="F24" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Greif' WHERE id = '12419';</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>12294</v>
+      </c>
+      <c r="B25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25">
+        <v>47321</v>
+      </c>
+      <c r="D25" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25">
+        <v>12417</v>
+      </c>
+      <c r="F25" t="s">
+        <v>70</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Großer Drache' WHERE id = '12417';</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>11512</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26">
+        <v>46497</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26">
+        <v>11512</v>
+      </c>
+      <c r="F26" t="s">
+        <v>128</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Großzauberer' WHERE id = '11512';</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>11508</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27">
+        <v>46493</v>
+      </c>
+      <c r="D27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27">
+        <v>11508</v>
+      </c>
+      <c r="F27" t="s">
+        <v>129</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Held' WHERE id = '11508';</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>12278</v>
+      </c>
+      <c r="B28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28">
+        <v>47215</v>
+      </c>
+      <c r="D28" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28">
+        <v>12420</v>
+      </c>
+      <c r="F28" t="s">
+        <v>68</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hippogreif' WHERE id = '12420';</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>11980</v>
+      </c>
+      <c r="B29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29">
+        <v>46946</v>
+      </c>
+      <c r="D29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29">
+        <v>11980</v>
+      </c>
+      <c r="F29" t="s">
+        <v>51</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Jungferngarde' WHERE id = '11980';</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>12637</v>
+      </c>
+      <c r="B30" t="s">
+        <v>109</v>
+      </c>
+      <c r="C30">
+        <v>47375</v>
+      </c>
+      <c r="D30" t="s">
+        <v>110</v>
+      </c>
+      <c r="E30">
+        <v>12637</v>
+      </c>
+      <c r="F30" t="s">
+        <v>51</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Jungferngarde' WHERE id = '12637';</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>12518</v>
+      </c>
+      <c r="B31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31">
+        <v>47489</v>
+      </c>
+      <c r="D31" t="s">
+        <v>90</v>
+      </c>
+      <c r="E31">
+        <v>12518</v>
+      </c>
+      <c r="F31" t="s">
+        <v>51</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Jungferngarde' WHERE id = '12518';</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>12302</v>
+      </c>
+      <c r="B32" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32">
+        <v>47329</v>
+      </c>
+      <c r="D32" t="s">
+        <v>71</v>
+      </c>
+      <c r="E32">
+        <v>12418</v>
+      </c>
+      <c r="F32" t="s">
+        <v>71</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Kaiserdrache' WHERE id = '12418';</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>11695</v>
+      </c>
+      <c r="B33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33">
+        <v>46370</v>
+      </c>
+      <c r="D33" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33">
+        <v>11695</v>
+      </c>
+      <c r="F33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Korhil' WHERE id = '11695';</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>12250</v>
+      </c>
+      <c r="B34" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34">
+        <v>47187</v>
+      </c>
+      <c r="D34" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34">
+        <v>12422</v>
+      </c>
+      <c r="F34" t="s">
+        <v>65</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Mantikor' WHERE id = '12422';</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>11513</v>
+      </c>
+      <c r="B35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35">
+        <v>46498</v>
+      </c>
+      <c r="D35" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35">
+        <v>11513</v>
+      </c>
+      <c r="F35" t="s">
+        <v>130</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Meisterzauberer' WHERE id = '11513';</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>11511</v>
+      </c>
+      <c r="B36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36">
+        <v>46496</v>
+      </c>
+      <c r="D36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36">
+        <v>11511</v>
+      </c>
+      <c r="F36" t="s">
+        <v>131</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Oberzauberer' WHERE id = '11511';</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>12167</v>
+      </c>
+      <c r="B37" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37">
+        <v>46734</v>
+      </c>
+      <c r="D37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E37">
+        <v>12336</v>
+      </c>
+      <c r="F37" t="s">
+        <v>62</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Pegasus' WHERE id = '12336';</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>11902</v>
+      </c>
+      <c r="B38" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38">
+        <v>46812</v>
+      </c>
+      <c r="D38" t="s">
+        <v>41</v>
+      </c>
+      <c r="E38">
+        <v>11902</v>
+      </c>
+      <c r="F38" t="s">
+        <v>126</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '11902';</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>12587</v>
+      </c>
+      <c r="B39" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39">
+        <v>47558</v>
+      </c>
+      <c r="D39" t="s">
+        <v>100</v>
+      </c>
+      <c r="E39">
+        <v>12587</v>
+      </c>
+      <c r="F39" t="s">
+        <v>126</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '12587';</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>12468</v>
+      </c>
+      <c r="B40" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40">
+        <v>47439</v>
+      </c>
+      <c r="D40" t="s">
+        <v>80</v>
+      </c>
+      <c r="E40">
+        <v>12468</v>
+      </c>
+      <c r="F40" t="s">
+        <v>126</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '12468';</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>11517</v>
+      </c>
+      <c r="B41" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41">
+        <v>46502</v>
+      </c>
+      <c r="D41" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41">
+        <v>11517</v>
+      </c>
+      <c r="F41" t="s">
+        <v>20</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Prinz Imrik' WHERE id = '11517';</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>12091</v>
+      </c>
+      <c r="B42" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42">
+        <v>47014</v>
+      </c>
+      <c r="D42" t="s">
+        <v>54</v>
+      </c>
+      <c r="E42">
+        <v>12091</v>
+      </c>
+      <c r="F42" t="s">
+        <v>124</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12091';</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>12091</v>
+      </c>
+      <c r="B43" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43">
+        <v>47116</v>
+      </c>
+      <c r="D43" t="s">
+        <v>55</v>
+      </c>
+      <c r="E43">
+        <v>12138</v>
+      </c>
+      <c r="F43" t="s">
+        <v>55</v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Speerschleuder' WHERE id = '12138';</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>12162</v>
+      </c>
+      <c r="B44" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44">
+        <v>46729</v>
+      </c>
+      <c r="D44" t="s">
+        <v>60</v>
+      </c>
+      <c r="E44">
+        <v>12162</v>
+      </c>
+      <c r="F44" t="s">
+        <v>60</v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Riesenadler' WHERE id = '12162';</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>11907</v>
+      </c>
+      <c r="B45" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45">
+        <v>46817</v>
+      </c>
+      <c r="D45" t="s">
+        <v>49</v>
+      </c>
+      <c r="E45">
+        <v>11907</v>
+      </c>
+      <c r="F45" t="s">
+        <v>124</v>
+      </c>
+      <c r="G45" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '11907';</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>12592</v>
+      </c>
+      <c r="B46" t="s">
+        <v>108</v>
+      </c>
+      <c r="C46">
+        <v>47563</v>
+      </c>
+      <c r="D46" t="s">
+        <v>108</v>
+      </c>
+      <c r="E46">
+        <v>12592</v>
+      </c>
+      <c r="F46" t="s">
+        <v>124</v>
+      </c>
+      <c r="G46" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12592';</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>12473</v>
+      </c>
+      <c r="B47" t="s">
+        <v>88</v>
+      </c>
+      <c r="C47">
+        <v>47444</v>
+      </c>
+      <c r="D47" t="s">
+        <v>88</v>
+      </c>
+      <c r="E47">
+        <v>12473</v>
+      </c>
+      <c r="F47" t="s">
+        <v>124</v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12473';</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>11901</v>
+      </c>
+      <c r="B48" t="s">
+        <v>38</v>
+      </c>
+      <c r="C48">
+        <v>46811</v>
+      </c>
+      <c r="D48" t="s">
+        <v>39</v>
+      </c>
+      <c r="E48">
+        <v>11901</v>
+      </c>
+      <c r="F48" t="s">
+        <v>126</v>
+      </c>
+      <c r="G48" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '11901';</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>12586</v>
+      </c>
+      <c r="B49" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49">
+        <v>47557</v>
+      </c>
+      <c r="D49" t="s">
+        <v>99</v>
+      </c>
+      <c r="E49">
+        <v>12586</v>
+      </c>
+      <c r="F49" t="s">
+        <v>126</v>
+      </c>
+      <c r="G49" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '12586';</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>12467</v>
+      </c>
+      <c r="B50" t="s">
+        <v>78</v>
+      </c>
+      <c r="C50">
+        <v>47438</v>
+      </c>
+      <c r="D50" t="s">
+        <v>79</v>
+      </c>
+      <c r="E50">
+        <v>12467</v>
+      </c>
+      <c r="F50" t="s">
+        <v>126</v>
+      </c>
+      <c r="G50" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '12467';</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>11905</v>
+      </c>
+      <c r="B51" t="s">
+        <v>45</v>
+      </c>
+      <c r="C51">
+        <v>46815</v>
+      </c>
+      <c r="D51" t="s">
+        <v>46</v>
+      </c>
+      <c r="E51">
+        <v>11905</v>
+      </c>
+      <c r="F51" t="s">
+        <v>124</v>
+      </c>
+      <c r="G51" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '11905';</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>12590</v>
+      </c>
+      <c r="B52" t="s">
+        <v>104</v>
+      </c>
+      <c r="C52">
+        <v>47561</v>
+      </c>
+      <c r="D52" t="s">
+        <v>105</v>
+      </c>
+      <c r="E52">
+        <v>12590</v>
+      </c>
+      <c r="F52" t="s">
+        <v>124</v>
+      </c>
+      <c r="G52" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12590';</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>12471</v>
+      </c>
+      <c r="B53" t="s">
+        <v>84</v>
+      </c>
+      <c r="C53">
+        <v>47442</v>
+      </c>
+      <c r="D53" t="s">
+        <v>85</v>
+      </c>
+      <c r="E53">
+        <v>12471</v>
+      </c>
+      <c r="F53" t="s">
+        <v>124</v>
+      </c>
+      <c r="G53" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12471';</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>11899</v>
+      </c>
+      <c r="B54" t="s">
+        <v>34</v>
+      </c>
+      <c r="C54">
+        <v>46809</v>
+      </c>
+      <c r="D54" t="s">
+        <v>35</v>
+      </c>
+      <c r="E54">
+        <v>11899</v>
+      </c>
+      <c r="F54" t="s">
+        <v>126</v>
+      </c>
+      <c r="G54" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '11899';</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>12584</v>
+      </c>
+      <c r="B55" t="s">
+        <v>94</v>
+      </c>
+      <c r="C55">
+        <v>47555</v>
+      </c>
+      <c r="D55" t="s">
+        <v>95</v>
+      </c>
+      <c r="E55">
+        <v>12584</v>
+      </c>
+      <c r="F55" t="s">
+        <v>126</v>
+      </c>
+      <c r="G55" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '12584';</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>12465</v>
+      </c>
+      <c r="B56" t="s">
+        <v>74</v>
+      </c>
+      <c r="C56">
+        <v>47436</v>
+      </c>
+      <c r="D56" t="s">
+        <v>75</v>
+      </c>
+      <c r="E56">
+        <v>12465</v>
+      </c>
+      <c r="F56" t="s">
+        <v>126</v>
+      </c>
+      <c r="G56" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '12465';</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>11904</v>
+      </c>
+      <c r="B57" t="s">
+        <v>44</v>
+      </c>
+      <c r="C57">
+        <v>46814</v>
+      </c>
+      <c r="D57" t="s">
+        <v>44</v>
+      </c>
+      <c r="E57">
+        <v>11904</v>
+      </c>
+      <c r="F57" t="s">
+        <v>124</v>
+      </c>
+      <c r="G57" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '11904';</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>12589</v>
+      </c>
+      <c r="B58" t="s">
+        <v>103</v>
+      </c>
+      <c r="C58">
+        <v>47560</v>
+      </c>
+      <c r="D58" t="s">
+        <v>103</v>
+      </c>
+      <c r="E58">
+        <v>12589</v>
+      </c>
+      <c r="F58" t="s">
+        <v>124</v>
+      </c>
+      <c r="G58" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12589';</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>12470</v>
+      </c>
+      <c r="B59" t="s">
+        <v>83</v>
+      </c>
+      <c r="C59">
+        <v>47441</v>
+      </c>
+      <c r="D59" t="s">
+        <v>83</v>
+      </c>
+      <c r="E59">
+        <v>12470</v>
+      </c>
+      <c r="F59" t="s">
+        <v>124</v>
+      </c>
+      <c r="G59" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12470';</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>11515</v>
+      </c>
+      <c r="B60" t="s">
+        <v>14</v>
+      </c>
+      <c r="C60">
+        <v>46500</v>
+      </c>
+      <c r="D60" t="s">
+        <v>15</v>
+      </c>
+      <c r="E60">
+        <v>11515</v>
+      </c>
+      <c r="F60" t="s">
+        <v>15</v>
+      </c>
+      <c r="G60" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Teclis' WHERE id = '11515';</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>12113</v>
+      </c>
+      <c r="B61" t="s">
+        <v>56</v>
+      </c>
+      <c r="C61">
+        <v>46726</v>
+      </c>
+      <c r="D61" t="s">
+        <v>58</v>
+      </c>
+      <c r="E61">
+        <v>12159</v>
+      </c>
+      <c r="F61" t="s">
+        <v>58</v>
+      </c>
+      <c r="G61" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Streitwagen' WHERE id = '12159';</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>12113</v>
+      </c>
+      <c r="B62" t="s">
+        <v>56</v>
+      </c>
+      <c r="C62">
+        <v>47064</v>
+      </c>
+      <c r="D62" t="s">
+        <v>57</v>
+      </c>
+      <c r="E62">
+        <v>12113</v>
+      </c>
+      <c r="F62" t="s">
+        <v>58</v>
+      </c>
+      <c r="G62" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Streitwagen' WHERE id = '12113';</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>12118</v>
+      </c>
+      <c r="B63" t="s">
+        <v>59</v>
+      </c>
+      <c r="C63">
+        <v>46727</v>
+      </c>
+      <c r="D63" t="s">
+        <v>58</v>
+      </c>
+      <c r="E63">
+        <v>12160</v>
+      </c>
+      <c r="F63" t="s">
+        <v>58</v>
+      </c>
+      <c r="G63" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Streitwagen' WHERE id = '12160';</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>12118</v>
+      </c>
+      <c r="B64" t="s">
+        <v>59</v>
+      </c>
+      <c r="C64">
+        <v>47069</v>
+      </c>
+      <c r="D64" t="s">
+        <v>57</v>
+      </c>
+      <c r="E64">
+        <v>12113</v>
+      </c>
+      <c r="F64" t="s">
+        <v>124</v>
+      </c>
+      <c r="G64" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12113';</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>11514</v>
+      </c>
+      <c r="B65" t="s">
+        <v>11</v>
+      </c>
+      <c r="C65">
+        <v>46838</v>
+      </c>
+      <c r="D65" t="s">
+        <v>13</v>
+      </c>
+      <c r="E65">
+        <v>11803</v>
+      </c>
+      <c r="F65" t="s">
+        <v>13</v>
+      </c>
+      <c r="G65" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Malhandir' WHERE id = '11803';</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>11514</v>
+      </c>
+      <c r="B66" t="s">
+        <v>11</v>
+      </c>
+      <c r="C66">
+        <v>46499</v>
+      </c>
+      <c r="D66" t="s">
+        <v>12</v>
+      </c>
+      <c r="E66">
+        <v>11514</v>
+      </c>
+      <c r="F66" t="s">
+        <v>12</v>
+      </c>
+      <c r="G66" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Tyrion' WHERE id = '11514';</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>11903</v>
+      </c>
+      <c r="B67" t="s">
+        <v>42</v>
+      </c>
+      <c r="C67">
+        <v>46813</v>
+      </c>
+      <c r="D67" t="s">
+        <v>43</v>
+      </c>
+      <c r="E67">
+        <v>11903</v>
+      </c>
+      <c r="F67" t="s">
+        <v>126</v>
+      </c>
+      <c r="G67" t="str">
+        <f t="shared" ref="G67:G73" si="1">CONCATENATE("UPDATE profile SET name = '",F67,"' WHERE id = '",E67,"';")</f>
+        <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '11903';</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>12588</v>
+      </c>
+      <c r="B68" t="s">
+        <v>101</v>
+      </c>
+      <c r="C68">
+        <v>47559</v>
+      </c>
+      <c r="D68" t="s">
+        <v>102</v>
+      </c>
+      <c r="E68">
+        <v>12588</v>
+      </c>
+      <c r="F68" t="s">
+        <v>126</v>
+      </c>
+      <c r="G68" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '12588';</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>12469</v>
+      </c>
+      <c r="B69" t="s">
+        <v>81</v>
+      </c>
+      <c r="C69">
+        <v>47440</v>
+      </c>
+      <c r="D69" t="s">
+        <v>82</v>
+      </c>
+      <c r="E69">
+        <v>12469</v>
+      </c>
+      <c r="F69" t="s">
+        <v>126</v>
+      </c>
+      <c r="G69" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '12469';</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>11510</v>
+      </c>
+      <c r="B70" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70">
+        <v>46495</v>
+      </c>
+      <c r="D70" t="s">
+        <v>7</v>
+      </c>
+      <c r="E70">
+        <v>11510</v>
+      </c>
+      <c r="F70" t="s">
+        <v>132</v>
+      </c>
+      <c r="G70" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = 'Hochelfen Zauberer' WHERE id = '11510';</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>11997</v>
+      </c>
+      <c r="B71" t="s">
+        <v>52</v>
+      </c>
+      <c r="C71">
+        <v>46963</v>
+      </c>
+      <c r="D71" t="s">
+        <v>52</v>
+      </c>
+      <c r="E71">
+        <v>11997</v>
+      </c>
+      <c r="F71" t="s">
+        <v>124</v>
+      </c>
+      <c r="G71" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '11997';</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>12652</v>
+      </c>
+      <c r="B72" t="s">
+        <v>111</v>
+      </c>
+      <c r="C72">
+        <v>47390</v>
+      </c>
+      <c r="D72" t="s">
+        <v>111</v>
+      </c>
+      <c r="E72">
+        <v>12652</v>
+      </c>
+      <c r="F72" t="s">
+        <v>124</v>
+      </c>
+      <c r="G72" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12652';</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>12533</v>
+      </c>
+      <c r="B73" t="s">
+        <v>91</v>
+      </c>
+      <c r="C73">
+        <v>47504</v>
+      </c>
+      <c r="D73" t="s">
+        <v>91</v>
+      </c>
+      <c r="E73">
+        <v>12533</v>
+      </c>
+      <c r="F73" t="s">
+        <v>124</v>
+      </c>
+      <c r="G73" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12533';</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:F73" xr:uid="{50ABEE1B-A043-4FB5-8D78-6CD44D39B2E7}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F73">
+    <sortCondition ref="B2:B73"/>
+    <sortCondition ref="D2:D73"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B274CE33-7099-4094-9D9A-29DF4F468E02}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -4480,7 +6291,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC3B880E-F91A-4006-A89E-3EF61A46384C}">
   <dimension ref="A1:J54"/>
   <sheetViews>

</xml_diff>

<commit_message>
Compare old and new points in excel
</commit_message>
<xml_diff>
--- a/resources/db/Profiles.xlsx
+++ b/resources/db/Profiles.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IN57KC\data\Projekte\csharp\ArmyBuilder\resources\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\projects\ArmyBuilder\sourcecode\resources\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E23472A-D0BA-4842-BC62-0B7C6C4E223D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83DA700-B884-4358-AFA8-9DB4DD434C79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{72821A2A-92BA-4C26-854D-A2ECB76DE865}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{72821A2A-92BA-4C26-854D-A2ECB76DE865}"/>
   </bookViews>
   <sheets>
     <sheet name="High Elf Profiles" sheetId="1" r:id="rId1"/>
     <sheet name="High Elf Fixed Profiles" sheetId="3" r:id="rId2"/>
-    <sheet name="Tabelle1" sheetId="5" r:id="rId3"/>
-    <sheet name="High Elf Wrong Profiles" sheetId="4" r:id="rId4"/>
-    <sheet name="High Elf Points" sheetId="2" r:id="rId5"/>
+    <sheet name="High Elf Profile Names" sheetId="5" r:id="rId3"/>
+    <sheet name="Tabelle1" sheetId="6" r:id="rId4"/>
+    <sheet name="High Elf Wrong Profiles" sheetId="4" r:id="rId5"/>
+    <sheet name="High Elf Points" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Tabelle1!$B$1:$F$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'High Elf Profile Names'!$B$1:$F$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Tabelle1!$A$1:$G$68</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,8 +36,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="154">
   <si>
     <t>Hochelfen</t>
   </si>
@@ -445,13 +445,73 @@
   </si>
   <si>
     <t>Immerkönigin</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>Character</t>
+  </si>
+  <si>
+    <t>Trooper</t>
+  </si>
+  <si>
+    <t>War Machine</t>
+  </si>
+  <si>
+    <t>Monster</t>
+  </si>
+  <si>
+    <t>old_points</t>
+  </si>
+  <si>
+    <t>new_points</t>
+  </si>
+  <si>
+    <t>Horn von Ish (25)</t>
+  </si>
+  <si>
+    <t>Banner von Avelorn (25)</t>
+  </si>
+  <si>
+    <t>difference</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>new points are correct, because auf light armor</t>
+  </si>
+  <si>
+    <t>check profile.points</t>
+  </si>
+  <si>
+    <t>double points of mount</t>
+  </si>
+  <si>
+    <t>add Löwenumhang</t>
+  </si>
+  <si>
+    <t>profile.points 90</t>
+  </si>
+  <si>
+    <t>profile.points 57</t>
+  </si>
+  <si>
+    <t>delete main model</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -460,7 +520,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -470,6 +530,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -486,9 +552,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -830,13 +897,13 @@
       <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="4" max="4" width="42.28515625" customWidth="1"/>
-    <col min="6" max="6" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.25" customWidth="1"/>
+    <col min="6" max="6" width="31.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>112</v>
       </c>
@@ -862,7 +929,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>7</v>
       </c>
@@ -888,7 +955,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>7</v>
       </c>
@@ -914,7 +981,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>7</v>
       </c>
@@ -940,7 +1007,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>7</v>
       </c>
@@ -966,7 +1033,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>7</v>
       </c>
@@ -992,7 +1059,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>7</v>
       </c>
@@ -1018,7 +1085,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1044,7 +1111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1070,7 +1137,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1096,7 +1163,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1122,7 +1189,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>7</v>
       </c>
@@ -1148,7 +1215,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13">
         <v>7</v>
       </c>
@@ -1174,7 +1241,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>7</v>
       </c>
@@ -1200,7 +1267,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>7</v>
       </c>
@@ -1226,7 +1293,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16">
         <v>7</v>
       </c>
@@ -1252,7 +1319,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>7</v>
       </c>
@@ -1278,7 +1345,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18">
         <v>7</v>
       </c>
@@ -1304,7 +1371,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19">
         <v>7</v>
       </c>
@@ -1330,7 +1397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20">
         <v>7</v>
       </c>
@@ -1356,7 +1423,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21">
         <v>7</v>
       </c>
@@ -1382,7 +1449,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22">
         <v>7</v>
       </c>
@@ -1408,7 +1475,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23">
         <v>7</v>
       </c>
@@ -1434,7 +1501,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24">
         <v>7</v>
       </c>
@@ -1460,7 +1527,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25">
         <v>7</v>
       </c>
@@ -1486,7 +1553,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26">
         <v>7</v>
       </c>
@@ -1512,7 +1579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27">
         <v>7</v>
       </c>
@@ -1538,7 +1605,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28">
         <v>7</v>
       </c>
@@ -1564,7 +1631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29">
         <v>7</v>
       </c>
@@ -1590,7 +1657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30">
         <v>7</v>
       </c>
@@ -1616,7 +1683,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31">
         <v>7</v>
       </c>
@@ -1642,7 +1709,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32">
         <v>7</v>
       </c>
@@ -1668,7 +1735,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33">
         <v>7</v>
       </c>
@@ -1694,7 +1761,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34">
         <v>7</v>
       </c>
@@ -1720,7 +1787,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35">
         <v>7</v>
       </c>
@@ -1746,7 +1813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36">
         <v>7</v>
       </c>
@@ -1772,7 +1839,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37">
         <v>7</v>
       </c>
@@ -1798,7 +1865,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38">
         <v>7</v>
       </c>
@@ -1824,7 +1891,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39">
         <v>7</v>
       </c>
@@ -1850,7 +1917,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40">
         <v>7</v>
       </c>
@@ -1876,7 +1943,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41">
         <v>7</v>
       </c>
@@ -1902,7 +1969,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42">
         <v>7</v>
       </c>
@@ -1928,7 +1995,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43">
         <v>7</v>
       </c>
@@ -1954,7 +2021,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44">
         <v>7</v>
       </c>
@@ -1980,7 +2047,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45">
         <v>7</v>
       </c>
@@ -2006,7 +2073,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46">
         <v>7</v>
       </c>
@@ -2032,7 +2099,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47">
         <v>7</v>
       </c>
@@ -2058,7 +2125,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48">
         <v>7</v>
       </c>
@@ -2084,7 +2151,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49">
         <v>7</v>
       </c>
@@ -2110,7 +2177,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50">
         <v>7</v>
       </c>
@@ -2136,7 +2203,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51">
         <v>7</v>
       </c>
@@ -2162,7 +2229,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52">
         <v>7</v>
       </c>
@@ -2188,7 +2255,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53">
         <v>7</v>
       </c>
@@ -2214,7 +2281,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="A54">
         <v>7</v>
       </c>
@@ -2240,7 +2307,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="A55">
         <v>7</v>
       </c>
@@ -2266,7 +2333,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8">
       <c r="A56">
         <v>7</v>
       </c>
@@ -2292,7 +2359,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8">
       <c r="A57">
         <v>7</v>
       </c>
@@ -2318,7 +2385,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8">
       <c r="A58">
         <v>7</v>
       </c>
@@ -2344,7 +2411,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8">
       <c r="A59">
         <v>7</v>
       </c>
@@ -2370,7 +2437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8">
       <c r="A60">
         <v>7</v>
       </c>
@@ -2396,7 +2463,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8">
       <c r="A61">
         <v>7</v>
       </c>
@@ -2422,7 +2489,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8">
       <c r="A62">
         <v>7</v>
       </c>
@@ -2448,7 +2515,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8">
       <c r="A63">
         <v>7</v>
       </c>
@@ -2474,7 +2541,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8">
       <c r="A64">
         <v>7</v>
       </c>
@@ -2500,7 +2567,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8">
       <c r="A65">
         <v>7</v>
       </c>
@@ -2526,7 +2593,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8">
       <c r="A66">
         <v>7</v>
       </c>
@@ -2552,7 +2619,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8">
       <c r="A67">
         <v>7</v>
       </c>
@@ -2578,7 +2645,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8">
       <c r="A68">
         <v>7</v>
       </c>
@@ -2604,7 +2671,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8">
       <c r="A69">
         <v>7</v>
       </c>
@@ -2630,7 +2697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8">
       <c r="A70">
         <v>7</v>
       </c>
@@ -2656,7 +2723,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8">
       <c r="A71">
         <v>7</v>
       </c>
@@ -2682,7 +2749,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8">
       <c r="A72">
         <v>7</v>
       </c>
@@ -2708,7 +2775,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8">
       <c r="A73">
         <v>7</v>
       </c>
@@ -2734,7 +2801,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8">
       <c r="A74">
         <v>7</v>
       </c>
@@ -2760,7 +2827,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8">
       <c r="A75">
         <v>7</v>
       </c>
@@ -2786,7 +2853,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8">
       <c r="A76">
         <v>7</v>
       </c>
@@ -2812,7 +2879,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8">
       <c r="A77">
         <v>7</v>
       </c>
@@ -2838,7 +2905,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8">
       <c r="A78">
         <v>7</v>
       </c>
@@ -2864,7 +2931,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8">
       <c r="A79">
         <v>7</v>
       </c>
@@ -2890,7 +2957,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8">
       <c r="A80">
         <v>7</v>
       </c>
@@ -2916,7 +2983,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8">
       <c r="A81">
         <v>7</v>
       </c>
@@ -2942,7 +3009,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8">
       <c r="A82">
         <v>7</v>
       </c>
@@ -2968,7 +3035,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8">
       <c r="A83">
         <v>7</v>
       </c>
@@ -2994,7 +3061,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8">
       <c r="A84">
         <v>7</v>
       </c>
@@ -3037,16 +3104,16 @@
       <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>114</v>
       </c>
@@ -3063,7 +3130,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>11693</v>
       </c>
@@ -3080,7 +3147,7 @@
         <v>11693</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>11692</v>
       </c>
@@ -3097,7 +3164,7 @@
         <v>11692</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>11507</v>
       </c>
@@ -3114,7 +3181,7 @@
         <v>11507</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>12243</v>
       </c>
@@ -3131,7 +3198,7 @@
         <v>12415</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>11694</v>
       </c>
@@ -3148,7 +3215,7 @@
         <v>11694</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>11906</v>
       </c>
@@ -3165,7 +3232,7 @@
         <v>11906</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>11696</v>
       </c>
@@ -3182,7 +3249,7 @@
         <v>11696</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>11509</v>
       </c>
@@ -3199,7 +3266,7 @@
         <v>11509</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>12236</v>
       </c>
@@ -3216,7 +3283,7 @@
         <v>12414</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>12286</v>
       </c>
@@ -3233,7 +3300,7 @@
         <v>12416</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>12163</v>
       </c>
@@ -3250,7 +3317,7 @@
         <v>12163</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>11506</v>
       </c>
@@ -3267,7 +3334,7 @@
         <v>11506</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>12269</v>
       </c>
@@ -3284,7 +3351,7 @@
         <v>12419</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>12294</v>
       </c>
@@ -3301,7 +3368,7 @@
         <v>12417</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>11512</v>
       </c>
@@ -3318,7 +3385,7 @@
         <v>11512</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>11508</v>
       </c>
@@ -3335,7 +3402,7 @@
         <v>11508</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>12278</v>
       </c>
@@ -3352,7 +3419,7 @@
         <v>12420</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>11980</v>
       </c>
@@ -3369,7 +3436,7 @@
         <v>11980</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>12302</v>
       </c>
@@ -3386,7 +3453,7 @@
         <v>12418</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>11695</v>
       </c>
@@ -3403,7 +3470,7 @@
         <v>11695</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>12250</v>
       </c>
@@ -3420,7 +3487,7 @@
         <v>12422</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>11513</v>
       </c>
@@ -3437,7 +3504,7 @@
         <v>11513</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>11511</v>
       </c>
@@ -3454,7 +3521,7 @@
         <v>11511</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>12167</v>
       </c>
@@ -3471,7 +3538,7 @@
         <v>12336</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>11902</v>
       </c>
@@ -3488,7 +3555,7 @@
         <v>11902</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>11517</v>
       </c>
@@ -3505,7 +3572,7 @@
         <v>11517</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>12162</v>
       </c>
@@ -3522,7 +3589,7 @@
         <v>12162</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>11907</v>
       </c>
@@ -3539,7 +3606,7 @@
         <v>11907</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>11905</v>
       </c>
@@ -3556,7 +3623,7 @@
         <v>11905</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>11904</v>
       </c>
@@ -3573,7 +3640,7 @@
         <v>11904</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>11515</v>
       </c>
@@ -3590,7 +3657,7 @@
         <v>11515</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>11510</v>
       </c>
@@ -3607,7 +3674,7 @@
         <v>11510</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>11516</v>
       </c>
@@ -3624,7 +3691,7 @@
         <v>11516</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>11516</v>
       </c>
@@ -3641,7 +3708,7 @@
         <v>11804</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>11514</v>
       </c>
@@ -3658,7 +3725,7 @@
         <v>11514</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>11514</v>
       </c>
@@ -3675,7 +3742,7 @@
         <v>11803</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>11900</v>
       </c>
@@ -3692,7 +3759,7 @@
         <v>12036</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39">
         <v>11900</v>
       </c>
@@ -3709,7 +3776,7 @@
         <v>11900</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40">
         <v>12585</v>
       </c>
@@ -3726,7 +3793,7 @@
         <v>12585</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41">
         <v>12585</v>
       </c>
@@ -3743,7 +3810,7 @@
         <v>12034</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42">
         <v>12466</v>
       </c>
@@ -3760,7 +3827,7 @@
         <v>12466</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43">
         <v>12466</v>
       </c>
@@ -3789,19 +3856,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50ABEE1B-A043-4FB5-8D78-6CD44D39B2E7}">
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G2" sqref="G2:G73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="45.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="45.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>114</v>
       </c>
@@ -3821,7 +3888,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>11693</v>
       </c>
@@ -3845,7 +3912,7 @@
         <v>UPDATE profile SET name = 'Immerkönigin' WHERE id = '11693';</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>11692</v>
       </c>
@@ -3869,7 +3936,7 @@
         <v>UPDATE profile SET name = 'General' WHERE id = '11692';</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>11507</v>
       </c>
@@ -3893,7 +3960,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Champion' WHERE id = '11507';</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>12243</v>
       </c>
@@ -3917,7 +3984,7 @@
         <v>UPDATE profile SET name = 'Basilisk' WHERE id = '12415';</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>11694</v>
       </c>
@@ -3941,7 +4008,7 @@
         <v>UPDATE profile SET name = 'Belannaer' WHERE id = '11694';</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>11906</v>
       </c>
@@ -3965,7 +4032,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '11906';</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>12591</v>
       </c>
@@ -3989,7 +4056,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12591';</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>12472</v>
       </c>
@@ -4013,7 +4080,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12472';</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>11696</v>
       </c>
@@ -4037,7 +4104,7 @@
         <v>UPDATE profile SET name = 'Caradryan' WHERE id = '11696';</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>11509</v>
       </c>
@@ -4061,7 +4128,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Champion' WHERE id = '11509';</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>12236</v>
       </c>
@@ -4085,7 +4152,7 @@
         <v>UPDATE profile SET name = 'Chimäre' WHERE id = '12414';</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>12286</v>
       </c>
@@ -4109,7 +4176,7 @@
         <v>UPDATE profile SET name = 'Drache' WHERE id = '12416';</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>11900</v>
       </c>
@@ -4133,7 +4200,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '11900';</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>12585</v>
       </c>
@@ -4157,7 +4224,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '12585';</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>12466</v>
       </c>
@@ -4181,7 +4248,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '12466';</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>12163</v>
       </c>
@@ -4205,7 +4272,7 @@
         <v>UPDATE profile SET name = 'Einhorn' WHERE id = '12163';</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>11898</v>
       </c>
@@ -4229,7 +4296,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '11898';</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19">
         <v>12583</v>
       </c>
@@ -4253,7 +4320,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12583';</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20">
         <v>12464</v>
       </c>
@@ -4277,7 +4344,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12464';</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21">
         <v>11516</v>
       </c>
@@ -4301,7 +4368,7 @@
         <v>UPDATE profile SET name = 'Greif' WHERE id = '11516';</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22">
         <v>11516</v>
       </c>
@@ -4325,7 +4392,7 @@
         <v>UPDATE profile SET name = 'Hochelfen General' WHERE id = '11804';</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23">
         <v>11506</v>
       </c>
@@ -4349,7 +4416,7 @@
         <v>UPDATE profile SET name = 'Hochelfen General' WHERE id = '11506';</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24">
         <v>12269</v>
       </c>
@@ -4373,7 +4440,7 @@
         <v>UPDATE profile SET name = 'Greif' WHERE id = '12419';</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25">
         <v>12294</v>
       </c>
@@ -4397,7 +4464,7 @@
         <v>UPDATE profile SET name = 'Großer Drache' WHERE id = '12417';</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26">
         <v>11512</v>
       </c>
@@ -4421,7 +4488,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Großzauberer' WHERE id = '11512';</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27">
         <v>11508</v>
       </c>
@@ -4445,7 +4512,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Held' WHERE id = '11508';</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28">
         <v>12278</v>
       </c>
@@ -4469,7 +4536,7 @@
         <v>UPDATE profile SET name = 'Hippogreif' WHERE id = '12420';</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29">
         <v>11980</v>
       </c>
@@ -4493,7 +4560,7 @@
         <v>UPDATE profile SET name = 'Jungferngarde' WHERE id = '11980';</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30">
         <v>12637</v>
       </c>
@@ -4517,7 +4584,7 @@
         <v>UPDATE profile SET name = 'Jungferngarde' WHERE id = '12637';</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31">
         <v>12518</v>
       </c>
@@ -4541,7 +4608,7 @@
         <v>UPDATE profile SET name = 'Jungferngarde' WHERE id = '12518';</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="A32">
         <v>12302</v>
       </c>
@@ -4565,7 +4632,7 @@
         <v>UPDATE profile SET name = 'Kaiserdrache' WHERE id = '12418';</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33">
         <v>11695</v>
       </c>
@@ -4589,7 +4656,7 @@
         <v>UPDATE profile SET name = 'Korhil' WHERE id = '11695';</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34">
         <v>12250</v>
       </c>
@@ -4613,7 +4680,7 @@
         <v>UPDATE profile SET name = 'Mantikor' WHERE id = '12422';</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35">
         <v>11513</v>
       </c>
@@ -4637,7 +4704,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Meisterzauberer' WHERE id = '11513';</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7">
       <c r="A36">
         <v>11511</v>
       </c>
@@ -4661,7 +4728,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Oberzauberer' WHERE id = '11511';</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7">
       <c r="A37">
         <v>12167</v>
       </c>
@@ -4685,7 +4752,7 @@
         <v>UPDATE profile SET name = 'Pegasus' WHERE id = '12336';</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7">
       <c r="A38">
         <v>11902</v>
       </c>
@@ -4709,7 +4776,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '11902';</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7">
       <c r="A39">
         <v>12587</v>
       </c>
@@ -4733,7 +4800,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '12587';</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7">
       <c r="A40">
         <v>12468</v>
       </c>
@@ -4757,7 +4824,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '12468';</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7">
       <c r="A41">
         <v>11517</v>
       </c>
@@ -4781,7 +4848,7 @@
         <v>UPDATE profile SET name = 'Prinz Imrik' WHERE id = '11517';</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7">
       <c r="A42">
         <v>12091</v>
       </c>
@@ -4805,7 +4872,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12091';</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7">
       <c r="A43">
         <v>12091</v>
       </c>
@@ -4829,7 +4896,7 @@
         <v>UPDATE profile SET name = 'Speerschleuder' WHERE id = '12138';</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7">
       <c r="A44">
         <v>12162</v>
       </c>
@@ -4853,7 +4920,7 @@
         <v>UPDATE profile SET name = 'Riesenadler' WHERE id = '12162';</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7">
       <c r="A45">
         <v>11907</v>
       </c>
@@ -4877,7 +4944,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '11907';</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7">
       <c r="A46">
         <v>12592</v>
       </c>
@@ -4901,7 +4968,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12592';</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7">
       <c r="A47">
         <v>12473</v>
       </c>
@@ -4925,7 +4992,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12473';</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7">
       <c r="A48">
         <v>11901</v>
       </c>
@@ -4949,7 +5016,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '11901';</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7">
       <c r="A49">
         <v>12586</v>
       </c>
@@ -4973,7 +5040,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '12586';</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7">
       <c r="A50">
         <v>12467</v>
       </c>
@@ -4997,7 +5064,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '12467';</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7">
       <c r="A51">
         <v>11905</v>
       </c>
@@ -5021,7 +5088,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '11905';</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7">
       <c r="A52">
         <v>12590</v>
       </c>
@@ -5045,7 +5112,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12590';</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7">
       <c r="A53">
         <v>12471</v>
       </c>
@@ -5069,7 +5136,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12471';</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7">
       <c r="A54">
         <v>11899</v>
       </c>
@@ -5093,7 +5160,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '11899';</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7">
       <c r="A55">
         <v>12584</v>
       </c>
@@ -5117,7 +5184,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '12584';</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7">
       <c r="A56">
         <v>12465</v>
       </c>
@@ -5141,7 +5208,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '12465';</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7">
       <c r="A57">
         <v>11904</v>
       </c>
@@ -5165,7 +5232,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '11904';</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7">
       <c r="A58">
         <v>12589</v>
       </c>
@@ -5189,7 +5256,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12589';</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7">
       <c r="A59">
         <v>12470</v>
       </c>
@@ -5213,7 +5280,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12470';</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7">
       <c r="A60">
         <v>11515</v>
       </c>
@@ -5237,7 +5304,7 @@
         <v>UPDATE profile SET name = 'Teclis' WHERE id = '11515';</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7">
       <c r="A61">
         <v>12113</v>
       </c>
@@ -5261,7 +5328,7 @@
         <v>UPDATE profile SET name = 'Streitwagen' WHERE id = '12159';</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7">
       <c r="A62">
         <v>12113</v>
       </c>
@@ -5285,7 +5352,7 @@
         <v>UPDATE profile SET name = 'Streitwagen' WHERE id = '12113';</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7">
       <c r="A63">
         <v>12118</v>
       </c>
@@ -5309,7 +5376,7 @@
         <v>UPDATE profile SET name = 'Streitwagen' WHERE id = '12160';</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7">
       <c r="A64">
         <v>12118</v>
       </c>
@@ -5333,7 +5400,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12113';</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7">
       <c r="A65">
         <v>11514</v>
       </c>
@@ -5357,7 +5424,7 @@
         <v>UPDATE profile SET name = 'Malhandir' WHERE id = '11803';</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7">
       <c r="A66">
         <v>11514</v>
       </c>
@@ -5381,7 +5448,7 @@
         <v>UPDATE profile SET name = 'Tyrion' WHERE id = '11514';</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7">
       <c r="A67">
         <v>11903</v>
       </c>
@@ -5405,7 +5472,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '11903';</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7">
       <c r="A68">
         <v>12588</v>
       </c>
@@ -5429,7 +5496,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '12588';</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7">
       <c r="A69">
         <v>12469</v>
       </c>
@@ -5453,7 +5520,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '12469';</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7">
       <c r="A70">
         <v>11510</v>
       </c>
@@ -5477,7 +5544,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Zauberer' WHERE id = '11510';</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7">
       <c r="A71">
         <v>11997</v>
       </c>
@@ -5501,7 +5568,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '11997';</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7">
       <c r="A72">
         <v>12652</v>
       </c>
@@ -5525,7 +5592,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12652';</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7">
       <c r="A73">
         <v>12533</v>
       </c>
@@ -5560,6 +5627,1527 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2547C117-82C3-4BEF-8EA7-BDB626B12945}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:G68"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G56" sqref="G56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="2" width="14.75" customWidth="1"/>
+    <col min="3" max="3" width="43" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" hidden="1">
+      <c r="A2">
+        <v>11693</v>
+      </c>
+      <c r="B2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2">
+        <v>475</v>
+      </c>
+      <c r="E2">
+        <v>475</v>
+      </c>
+      <c r="F2">
+        <f>D2-E2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" hidden="1">
+      <c r="A3">
+        <v>11692</v>
+      </c>
+      <c r="B3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3">
+        <v>285</v>
+      </c>
+      <c r="E3">
+        <v>285</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F66" si="0">D3-E3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>11507</v>
+      </c>
+      <c r="B4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>98</v>
+      </c>
+      <c r="E4">
+        <v>96</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" hidden="1">
+      <c r="A5">
+        <v>11694</v>
+      </c>
+      <c r="B5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5">
+        <v>555</v>
+      </c>
+      <c r="E5">
+        <v>555</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" hidden="1">
+      <c r="A6">
+        <v>11696</v>
+      </c>
+      <c r="B6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6">
+        <v>73</v>
+      </c>
+      <c r="E6">
+        <v>73</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" hidden="1">
+      <c r="A7">
+        <v>11509</v>
+      </c>
+      <c r="B7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>48</v>
+      </c>
+      <c r="E7">
+        <v>48</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>11516</v>
+      </c>
+      <c r="B8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8">
+        <v>467</v>
+      </c>
+      <c r="E8">
+        <v>471</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" hidden="1">
+      <c r="A9">
+        <v>11506</v>
+      </c>
+      <c r="B9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>160</v>
+      </c>
+      <c r="E9">
+        <v>160</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" hidden="1">
+      <c r="A10">
+        <v>11512</v>
+      </c>
+      <c r="B10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>219</v>
+      </c>
+      <c r="E10">
+        <v>219</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" hidden="1">
+      <c r="A11">
+        <v>11508</v>
+      </c>
+      <c r="B11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>104</v>
+      </c>
+      <c r="E11">
+        <v>104</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" hidden="1">
+      <c r="A12">
+        <v>11695</v>
+      </c>
+      <c r="B12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12">
+        <v>198</v>
+      </c>
+      <c r="E12">
+        <v>198</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" hidden="1">
+      <c r="A13">
+        <v>11513</v>
+      </c>
+      <c r="B13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>328</v>
+      </c>
+      <c r="E13">
+        <v>328</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" hidden="1">
+      <c r="A14">
+        <v>11511</v>
+      </c>
+      <c r="B14" t="s">
+        <v>137</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14">
+        <v>121</v>
+      </c>
+      <c r="E14">
+        <v>121</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" hidden="1">
+      <c r="A15">
+        <v>11517</v>
+      </c>
+      <c r="B15" t="s">
+        <v>137</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15">
+        <v>275</v>
+      </c>
+      <c r="E15">
+        <v>275</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" hidden="1">
+      <c r="A16">
+        <v>11515</v>
+      </c>
+      <c r="B16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <v>630</v>
+      </c>
+      <c r="E16">
+        <v>630</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" hidden="1">
+      <c r="A17">
+        <v>11514</v>
+      </c>
+      <c r="B17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17">
+        <v>425</v>
+      </c>
+      <c r="E17">
+        <v>425</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" hidden="1">
+      <c r="A18">
+        <v>11510</v>
+      </c>
+      <c r="B18" t="s">
+        <v>137</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18">
+        <v>59</v>
+      </c>
+      <c r="E18">
+        <v>59</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" hidden="1">
+      <c r="A19">
+        <v>11906</v>
+      </c>
+      <c r="B19" t="s">
+        <v>138</v>
+      </c>
+      <c r="C19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
+      </c>
+      <c r="E19">
+        <v>10</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" hidden="1">
+      <c r="A20">
+        <v>12591</v>
+      </c>
+      <c r="B20" t="s">
+        <v>138</v>
+      </c>
+      <c r="C20" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20">
+        <v>20</v>
+      </c>
+      <c r="E20">
+        <v>20</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" hidden="1">
+      <c r="A21">
+        <v>12472</v>
+      </c>
+      <c r="B21" t="s">
+        <v>138</v>
+      </c>
+      <c r="C21" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21">
+        <v>20</v>
+      </c>
+      <c r="E21">
+        <v>20</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" hidden="1">
+      <c r="A22">
+        <v>11900</v>
+      </c>
+      <c r="B22" t="s">
+        <v>138</v>
+      </c>
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22">
+        <v>43</v>
+      </c>
+      <c r="E22">
+        <v>43</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23">
+        <v>12585</v>
+      </c>
+      <c r="B23" t="s">
+        <v>138</v>
+      </c>
+      <c r="C23" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23">
+        <v>86</v>
+      </c>
+      <c r="E23">
+        <v>83</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G23" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24">
+        <v>12466</v>
+      </c>
+      <c r="B24" t="s">
+        <v>138</v>
+      </c>
+      <c r="C24" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24">
+        <v>86</v>
+      </c>
+      <c r="E24">
+        <v>83</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
+        <v>11898</v>
+      </c>
+      <c r="B25" t="s">
+        <v>138</v>
+      </c>
+      <c r="C25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25">
+        <v>25</v>
+      </c>
+      <c r="E25">
+        <v>23</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26">
+        <v>12583</v>
+      </c>
+      <c r="B26" t="s">
+        <v>138</v>
+      </c>
+      <c r="C26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26">
+        <v>50</v>
+      </c>
+      <c r="E26">
+        <v>43</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="G26" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27">
+        <v>12464</v>
+      </c>
+      <c r="B27" t="s">
+        <v>138</v>
+      </c>
+      <c r="C27" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27">
+        <v>50</v>
+      </c>
+      <c r="E27">
+        <v>43</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="G27" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" hidden="1">
+      <c r="A28">
+        <v>11980</v>
+      </c>
+      <c r="B28" t="s">
+        <v>138</v>
+      </c>
+      <c r="C28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28">
+        <v>16</v>
+      </c>
+      <c r="E28">
+        <v>16</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29">
+        <v>12637</v>
+      </c>
+      <c r="B29" t="s">
+        <v>138</v>
+      </c>
+      <c r="C29" t="s">
+        <v>109</v>
+      </c>
+      <c r="D29">
+        <v>32</v>
+      </c>
+      <c r="E29">
+        <v>82</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>-50</v>
+      </c>
+      <c r="G29" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30">
+        <v>12518</v>
+      </c>
+      <c r="B30" t="s">
+        <v>138</v>
+      </c>
+      <c r="C30" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30">
+        <v>32</v>
+      </c>
+      <c r="E30">
+        <v>82</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>-50</v>
+      </c>
+      <c r="G30" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" hidden="1">
+      <c r="A31">
+        <v>11902</v>
+      </c>
+      <c r="B31" t="s">
+        <v>138</v>
+      </c>
+      <c r="C31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31">
+        <v>14</v>
+      </c>
+      <c r="E31">
+        <v>14</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" hidden="1">
+      <c r="A32">
+        <v>12587</v>
+      </c>
+      <c r="B32" t="s">
+        <v>138</v>
+      </c>
+      <c r="C32" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32">
+        <v>28</v>
+      </c>
+      <c r="E32">
+        <v>28</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" hidden="1">
+      <c r="A33">
+        <v>12468</v>
+      </c>
+      <c r="B33" t="s">
+        <v>138</v>
+      </c>
+      <c r="C33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33">
+        <v>28</v>
+      </c>
+      <c r="E33">
+        <v>28</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34">
+        <v>11907</v>
+      </c>
+      <c r="B34" t="s">
+        <v>138</v>
+      </c>
+      <c r="C34" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34">
+        <v>12</v>
+      </c>
+      <c r="E34">
+        <v>11</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35">
+        <v>12592</v>
+      </c>
+      <c r="B35" t="s">
+        <v>138</v>
+      </c>
+      <c r="C35" t="s">
+        <v>108</v>
+      </c>
+      <c r="D35">
+        <v>24</v>
+      </c>
+      <c r="E35">
+        <v>22</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36">
+        <v>12473</v>
+      </c>
+      <c r="B36" t="s">
+        <v>138</v>
+      </c>
+      <c r="C36" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36">
+        <v>24</v>
+      </c>
+      <c r="E36">
+        <v>22</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37">
+        <v>11901</v>
+      </c>
+      <c r="B37" t="s">
+        <v>138</v>
+      </c>
+      <c r="C37" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37">
+        <v>16</v>
+      </c>
+      <c r="E37">
+        <v>15</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38">
+        <v>12586</v>
+      </c>
+      <c r="B38" t="s">
+        <v>138</v>
+      </c>
+      <c r="C38" t="s">
+        <v>98</v>
+      </c>
+      <c r="D38">
+        <v>32</v>
+      </c>
+      <c r="E38">
+        <v>30</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39">
+        <v>12467</v>
+      </c>
+      <c r="B39" t="s">
+        <v>138</v>
+      </c>
+      <c r="C39" t="s">
+        <v>78</v>
+      </c>
+      <c r="D39">
+        <v>32</v>
+      </c>
+      <c r="E39">
+        <v>30</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" hidden="1">
+      <c r="A40">
+        <v>11905</v>
+      </c>
+      <c r="B40" t="s">
+        <v>138</v>
+      </c>
+      <c r="C40" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40">
+        <v>14</v>
+      </c>
+      <c r="E40">
+        <v>14</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" hidden="1">
+      <c r="A41">
+        <v>12590</v>
+      </c>
+      <c r="B41" t="s">
+        <v>138</v>
+      </c>
+      <c r="C41" t="s">
+        <v>104</v>
+      </c>
+      <c r="D41">
+        <v>28</v>
+      </c>
+      <c r="E41">
+        <v>28</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" hidden="1">
+      <c r="A42">
+        <v>12471</v>
+      </c>
+      <c r="B42" t="s">
+        <v>138</v>
+      </c>
+      <c r="C42" t="s">
+        <v>84</v>
+      </c>
+      <c r="D42">
+        <v>28</v>
+      </c>
+      <c r="E42">
+        <v>28</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" hidden="1">
+      <c r="A43">
+        <v>11899</v>
+      </c>
+      <c r="B43" t="s">
+        <v>138</v>
+      </c>
+      <c r="C43" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43">
+        <v>31</v>
+      </c>
+      <c r="E43">
+        <v>31</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44">
+        <v>12584</v>
+      </c>
+      <c r="B44" t="s">
+        <v>138</v>
+      </c>
+      <c r="C44" t="s">
+        <v>94</v>
+      </c>
+      <c r="D44">
+        <v>62</v>
+      </c>
+      <c r="E44">
+        <v>59</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G44" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45">
+        <v>12465</v>
+      </c>
+      <c r="B45" t="s">
+        <v>138</v>
+      </c>
+      <c r="C45" t="s">
+        <v>74</v>
+      </c>
+      <c r="D45">
+        <v>62</v>
+      </c>
+      <c r="E45">
+        <v>59</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G45" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" hidden="1">
+      <c r="A46">
+        <v>11904</v>
+      </c>
+      <c r="B46" t="s">
+        <v>138</v>
+      </c>
+      <c r="C46" t="s">
+        <v>44</v>
+      </c>
+      <c r="D46">
+        <v>12</v>
+      </c>
+      <c r="E46">
+        <v>12</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" hidden="1">
+      <c r="A47">
+        <v>12589</v>
+      </c>
+      <c r="B47" t="s">
+        <v>138</v>
+      </c>
+      <c r="C47" t="s">
+        <v>103</v>
+      </c>
+      <c r="D47">
+        <v>24</v>
+      </c>
+      <c r="E47">
+        <v>24</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" hidden="1">
+      <c r="A48">
+        <v>12470</v>
+      </c>
+      <c r="B48" t="s">
+        <v>138</v>
+      </c>
+      <c r="C48" t="s">
+        <v>83</v>
+      </c>
+      <c r="D48">
+        <v>24</v>
+      </c>
+      <c r="E48">
+        <v>24</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49">
+        <v>11903</v>
+      </c>
+      <c r="B49" t="s">
+        <v>138</v>
+      </c>
+      <c r="C49" t="s">
+        <v>42</v>
+      </c>
+      <c r="D49">
+        <v>16</v>
+      </c>
+      <c r="E49">
+        <v>15</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G49" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50">
+        <v>12588</v>
+      </c>
+      <c r="B50" t="s">
+        <v>138</v>
+      </c>
+      <c r="C50" t="s">
+        <v>101</v>
+      </c>
+      <c r="D50">
+        <v>32</v>
+      </c>
+      <c r="E50">
+        <v>30</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G50" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51">
+        <v>12469</v>
+      </c>
+      <c r="B51" t="s">
+        <v>138</v>
+      </c>
+      <c r="C51" t="s">
+        <v>81</v>
+      </c>
+      <c r="D51">
+        <v>32</v>
+      </c>
+      <c r="E51">
+        <v>30</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G51" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52">
+        <v>11997</v>
+      </c>
+      <c r="B52" t="s">
+        <v>138</v>
+      </c>
+      <c r="C52" t="s">
+        <v>52</v>
+      </c>
+      <c r="D52">
+        <v>9</v>
+      </c>
+      <c r="E52">
+        <v>11</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="G52" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53">
+        <v>12652</v>
+      </c>
+      <c r="B53" t="s">
+        <v>138</v>
+      </c>
+      <c r="C53" t="s">
+        <v>111</v>
+      </c>
+      <c r="D53">
+        <v>18</v>
+      </c>
+      <c r="E53">
+        <v>22</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="G53" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54">
+        <v>12533</v>
+      </c>
+      <c r="B54" t="s">
+        <v>138</v>
+      </c>
+      <c r="C54" t="s">
+        <v>91</v>
+      </c>
+      <c r="D54">
+        <v>18</v>
+      </c>
+      <c r="E54">
+        <v>22</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="G54" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55">
+        <v>12091</v>
+      </c>
+      <c r="B55" t="s">
+        <v>139</v>
+      </c>
+      <c r="C55" t="s">
+        <v>53</v>
+      </c>
+      <c r="D55">
+        <v>100</v>
+      </c>
+      <c r="E55">
+        <v>10</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="G55" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56">
+        <v>12113</v>
+      </c>
+      <c r="B56" t="s">
+        <v>139</v>
+      </c>
+      <c r="C56" t="s">
+        <v>56</v>
+      </c>
+      <c r="D56">
+        <v>72</v>
+      </c>
+      <c r="E56">
+        <v>15</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="G56" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57">
+        <v>12118</v>
+      </c>
+      <c r="B57" t="s">
+        <v>139</v>
+      </c>
+      <c r="C57" t="s">
+        <v>59</v>
+      </c>
+      <c r="D57">
+        <v>84</v>
+      </c>
+      <c r="E57">
+        <v>13</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+      <c r="G57" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" hidden="1">
+      <c r="A58">
+        <v>12243</v>
+      </c>
+      <c r="B58" t="s">
+        <v>140</v>
+      </c>
+      <c r="C58" t="s">
+        <v>64</v>
+      </c>
+      <c r="D58">
+        <v>150</v>
+      </c>
+      <c r="E58">
+        <v>150</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" hidden="1">
+      <c r="A59">
+        <v>12236</v>
+      </c>
+      <c r="B59" t="s">
+        <v>140</v>
+      </c>
+      <c r="C59" t="s">
+        <v>63</v>
+      </c>
+      <c r="D59">
+        <v>250</v>
+      </c>
+      <c r="E59">
+        <v>250</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" hidden="1">
+      <c r="A60">
+        <v>12286</v>
+      </c>
+      <c r="B60" t="s">
+        <v>140</v>
+      </c>
+      <c r="C60" t="s">
+        <v>69</v>
+      </c>
+      <c r="D60">
+        <v>450</v>
+      </c>
+      <c r="E60">
+        <v>450</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" hidden="1">
+      <c r="A61">
+        <v>12163</v>
+      </c>
+      <c r="B61" t="s">
+        <v>140</v>
+      </c>
+      <c r="C61" t="s">
+        <v>61</v>
+      </c>
+      <c r="D61">
+        <v>90</v>
+      </c>
+      <c r="E61">
+        <v>90</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" hidden="1">
+      <c r="A62">
+        <v>12269</v>
+      </c>
+      <c r="B62" t="s">
+        <v>140</v>
+      </c>
+      <c r="C62" t="s">
+        <v>67</v>
+      </c>
+      <c r="D62">
+        <v>150</v>
+      </c>
+      <c r="E62">
+        <v>150</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" hidden="1">
+      <c r="A63">
+        <v>12294</v>
+      </c>
+      <c r="B63" t="s">
+        <v>140</v>
+      </c>
+      <c r="C63" t="s">
+        <v>70</v>
+      </c>
+      <c r="D63">
+        <v>600</v>
+      </c>
+      <c r="E63">
+        <v>600</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" hidden="1">
+      <c r="A64">
+        <v>12278</v>
+      </c>
+      <c r="B64" t="s">
+        <v>140</v>
+      </c>
+      <c r="C64" t="s">
+        <v>68</v>
+      </c>
+      <c r="D64">
+        <v>145</v>
+      </c>
+      <c r="E64">
+        <v>145</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" hidden="1">
+      <c r="A65">
+        <v>12302</v>
+      </c>
+      <c r="B65" t="s">
+        <v>140</v>
+      </c>
+      <c r="C65" t="s">
+        <v>71</v>
+      </c>
+      <c r="D65">
+        <v>750</v>
+      </c>
+      <c r="E65">
+        <v>750</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" hidden="1">
+      <c r="A66">
+        <v>12250</v>
+      </c>
+      <c r="B66" t="s">
+        <v>140</v>
+      </c>
+      <c r="C66" t="s">
+        <v>65</v>
+      </c>
+      <c r="D66">
+        <v>200</v>
+      </c>
+      <c r="E66">
+        <v>200</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" hidden="1">
+      <c r="A67">
+        <v>12167</v>
+      </c>
+      <c r="B67" t="s">
+        <v>140</v>
+      </c>
+      <c r="C67" t="s">
+        <v>62</v>
+      </c>
+      <c r="D67">
+        <v>50</v>
+      </c>
+      <c r="E67">
+        <v>50</v>
+      </c>
+      <c r="F67">
+        <f t="shared" ref="F67:F68" si="1">D67-E67</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" hidden="1">
+      <c r="A68">
+        <v>12162</v>
+      </c>
+      <c r="B68" t="s">
+        <v>140</v>
+      </c>
+      <c r="C68" t="s">
+        <v>60</v>
+      </c>
+      <c r="D68">
+        <v>75</v>
+      </c>
+      <c r="E68">
+        <v>75</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:G68" xr:uid="{2547C117-82C3-4BEF-8EA7-BDB626B12945}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="1"/>
+        <filter val="2"/>
+        <filter val="-2"/>
+        <filter val="3"/>
+        <filter val="-4"/>
+        <filter val="-50"/>
+        <filter val="57"/>
+        <filter val="7"/>
+        <filter val="71"/>
+        <filter val="90"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B274CE33-7099-4094-9D9A-29DF4F468E02}">
   <dimension ref="A1:E43"/>
   <sheetViews>
@@ -5567,12 +7155,12 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>114</v>
       </c>
@@ -5589,7 +7177,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>11898</v>
       </c>
@@ -5606,7 +7194,7 @@
         <v>12034</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>11898</v>
       </c>
@@ -5623,7 +7211,7 @@
         <v>11898</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>12583</v>
       </c>
@@ -5640,7 +7228,7 @@
         <v>12583</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>12583</v>
       </c>
@@ -5657,7 +7245,7 @@
         <v>12034</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>12464</v>
       </c>
@@ -5674,7 +7262,7 @@
         <v>12464</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>12464</v>
       </c>
@@ -5691,7 +7279,7 @@
         <v>12034</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>11901</v>
       </c>
@@ -5708,7 +7296,7 @@
         <v>11901</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>12586</v>
       </c>
@@ -5725,7 +7313,7 @@
         <v>12586</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>12467</v>
       </c>
@@ -5742,7 +7330,7 @@
         <v>12467</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>11899</v>
       </c>
@@ -5759,7 +7347,7 @@
         <v>12034</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>11899</v>
       </c>
@@ -5776,7 +7364,7 @@
         <v>11899</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>12584</v>
       </c>
@@ -5793,7 +7381,7 @@
         <v>12584</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>12584</v>
       </c>
@@ -5810,7 +7398,7 @@
         <v>12034</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>12465</v>
       </c>
@@ -5827,7 +7415,7 @@
         <v>12465</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>12465</v>
       </c>
@@ -5844,7 +7432,7 @@
         <v>12034</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>11903</v>
       </c>
@@ -5861,7 +7449,7 @@
         <v>11903</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>12588</v>
       </c>
@@ -5878,7 +7466,7 @@
         <v>12588</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>12469</v>
       </c>
@@ -5895,7 +7483,7 @@
         <v>12469</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>11997</v>
       </c>
@@ -5912,7 +7500,7 @@
         <v>11997</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>12652</v>
       </c>
@@ -5929,7 +7517,7 @@
         <v>12652</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>12533</v>
       </c>
@@ -5946,7 +7534,7 @@
         <v>12533</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>12113</v>
       </c>
@@ -5963,7 +7551,7 @@
         <v>12159</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>12113</v>
       </c>
@@ -5980,7 +7568,7 @@
         <v>12113</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>12113</v>
       </c>
@@ -5997,7 +7585,7 @@
         <v>12034</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>12118</v>
       </c>
@@ -6014,7 +7602,7 @@
         <v>12160</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>12118</v>
       </c>
@@ -6031,7 +7619,7 @@
         <v>12113</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>12118</v>
       </c>
@@ -6048,7 +7636,7 @@
         <v>12034</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>12091</v>
       </c>
@@ -6065,7 +7653,7 @@
         <v>12091</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>12091</v>
       </c>
@@ -6082,7 +7670,7 @@
         <v>12138</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>12591</v>
       </c>
@@ -6099,7 +7687,7 @@
         <v>12591</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>12472</v>
       </c>
@@ -6116,7 +7704,7 @@
         <v>12472</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>12637</v>
       </c>
@@ -6133,7 +7721,7 @@
         <v>12637</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>12518</v>
       </c>
@@ -6150,7 +7738,7 @@
         <v>12518</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>12587</v>
       </c>
@@ -6167,7 +7755,7 @@
         <v>12587</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>12468</v>
       </c>
@@ -6184,7 +7772,7 @@
         <v>12468</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>12592</v>
       </c>
@@ -6201,7 +7789,7 @@
         <v>12592</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39">
         <v>12473</v>
       </c>
@@ -6218,7 +7806,7 @@
         <v>12473</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40">
         <v>12590</v>
       </c>
@@ -6235,7 +7823,7 @@
         <v>12590</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41">
         <v>12471</v>
       </c>
@@ -6252,7 +7840,7 @@
         <v>12471</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42">
         <v>12589</v>
       </c>
@@ -6269,7 +7857,7 @@
         <v>12589</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43">
         <v>12470</v>
       </c>
@@ -6291,7 +7879,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC3B880E-F91A-4006-A89E-3EF61A46384C}">
   <dimension ref="A1:J54"/>
   <sheetViews>
@@ -6300,14 +7888,14 @@
       <selection pane="bottomLeft" activeCell="J2" sqref="J2:J54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="38.85546875" customWidth="1"/>
-    <col min="4" max="4" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.875" customWidth="1"/>
+    <col min="4" max="4" width="31.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>114</v>
       </c>
@@ -6336,7 +7924,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>11693</v>
       </c>
@@ -6370,7 +7958,7 @@
         <v>UPDATE profile SET points = 330 WHERE id = 11693;</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>11692</v>
       </c>
@@ -6404,7 +7992,7 @@
         <v>UPDATE profile SET points = 167 WHERE id = 11692;</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>11507</v>
       </c>
@@ -6437,7 +8025,7 @@
         <v>UPDATE profile SET points = 98 WHERE id = 11507;</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>12243</v>
       </c>
@@ -6467,7 +8055,7 @@
         <v>UPDATE profile SET points = 150 WHERE id = 12415;</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>11694</v>
       </c>
@@ -6501,7 +8089,7 @@
         <v>UPDATE profile SET points = 400 WHERE id = 11694;</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>11906</v>
       </c>
@@ -6534,7 +8122,7 @@
         <v>UPDATE profile SET points = 8 WHERE id = 11906;</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>12591</v>
       </c>
@@ -6567,7 +8155,7 @@
         <v>UPDATE profile SET points = 16 WHERE id = 12591;</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>12472</v>
       </c>
@@ -6600,7 +8188,7 @@
         <v>UPDATE profile SET points = 16 WHERE id = 12472;</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>11696</v>
       </c>
@@ -6634,7 +8222,7 @@
         <v>UPDATE profile SET points = 68 WHERE id = 11696;</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>11509</v>
       </c>
@@ -6667,7 +8255,7 @@
         <v>UPDATE profile SET points = 48 WHERE id = 11509;</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>12236</v>
       </c>
@@ -6697,7 +8285,7 @@
         <v>UPDATE profile SET points = 250 WHERE id = 12414;</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>12286</v>
       </c>
@@ -6727,7 +8315,7 @@
         <v>UPDATE profile SET points = 450 WHERE id = 12416;</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>12163</v>
       </c>
@@ -6757,7 +8345,7 @@
         <v>UPDATE profile SET points = 90 WHERE id = 12163;</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>11506</v>
       </c>
@@ -6791,7 +8379,7 @@
         <v>UPDATE profile SET points = 160 WHERE id = 11506;</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>12269</v>
       </c>
@@ -6821,7 +8409,7 @@
         <v>UPDATE profile SET points = 150 WHERE id = 12419;</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>12294</v>
       </c>
@@ -6851,7 +8439,7 @@
         <v>UPDATE profile SET points = 600 WHERE id = 12417;</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>11512</v>
       </c>
@@ -6884,7 +8472,7 @@
         <v>UPDATE profile SET points = 219 WHERE id = 11512;</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>11508</v>
       </c>
@@ -6917,7 +8505,7 @@
         <v>UPDATE profile SET points = 104 WHERE id = 11508;</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>12278</v>
       </c>
@@ -6947,7 +8535,7 @@
         <v>UPDATE profile SET points = 145 WHERE id = 12420;</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>11980</v>
       </c>
@@ -6980,7 +8568,7 @@
         <v>UPDATE profile SET points = 10 WHERE id = 11980;</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>12637</v>
       </c>
@@ -7013,7 +8601,7 @@
         <v>UPDATE profile SET points = 20 WHERE id = 12637;</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>12518</v>
       </c>
@@ -7046,7 +8634,7 @@
         <v>UPDATE profile SET points = 20 WHERE id = 12518;</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>12302</v>
       </c>
@@ -7076,7 +8664,7 @@
         <v>UPDATE profile SET points = 750 WHERE id = 12418;</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>11695</v>
       </c>
@@ -7110,7 +8698,7 @@
         <v>UPDATE profile SET points = 123 WHERE id = 11695;</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>12250</v>
       </c>
@@ -7140,7 +8728,7 @@
         <v>UPDATE profile SET points = 200 WHERE id = 12422;</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>11513</v>
       </c>
@@ -7173,7 +8761,7 @@
         <v>UPDATE profile SET points = 328 WHERE id = 11513;</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>11511</v>
       </c>
@@ -7206,7 +8794,7 @@
         <v>UPDATE profile SET points = 121 WHERE id = 11511;</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>12167</v>
       </c>
@@ -7236,7 +8824,7 @@
         <v>UPDATE profile SET points = 50 WHERE id = 12336;</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>11902</v>
       </c>
@@ -7269,7 +8857,7 @@
         <v>UPDATE profile SET points = 10 WHERE id = 11902;</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>12587</v>
       </c>
@@ -7302,7 +8890,7 @@
         <v>UPDATE profile SET points = 20 WHERE id = 12587;</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>12468</v>
       </c>
@@ -7335,7 +8923,7 @@
         <v>UPDATE profile SET points = 20 WHERE id = 12468;</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33">
         <v>11517</v>
       </c>
@@ -7369,7 +8957,7 @@
         <v>UPDATE profile SET points = 170 WHERE id = 11517;</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34">
         <v>12162</v>
       </c>
@@ -7399,7 +8987,7 @@
         <v>UPDATE profile SET points = 75 WHERE id = 12162;</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35">
         <v>11907</v>
       </c>
@@ -7432,7 +9020,7 @@
         <v>UPDATE profile SET points = 9 WHERE id = 11907;</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36">
         <v>12592</v>
       </c>
@@ -7465,7 +9053,7 @@
         <v>UPDATE profile SET points = 18 WHERE id = 12592;</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37">
         <v>12473</v>
       </c>
@@ -7498,7 +9086,7 @@
         <v>UPDATE profile SET points = 18 WHERE id = 12473;</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38">
         <v>11901</v>
       </c>
@@ -7531,7 +9119,7 @@
         <v>UPDATE profile SET points = 9 WHERE id = 11901;</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39">
         <v>12586</v>
       </c>
@@ -7564,7 +9152,7 @@
         <v>UPDATE profile SET points = 18 WHERE id = 12586;</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40">
         <v>12467</v>
       </c>
@@ -7597,7 +9185,7 @@
         <v>UPDATE profile SET points = 18 WHERE id = 12467;</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41">
         <v>11905</v>
       </c>
@@ -7630,7 +9218,7 @@
         <v>UPDATE profile SET points = 8 WHERE id = 11905;</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42">
         <v>12590</v>
       </c>
@@ -7663,7 +9251,7 @@
         <v>UPDATE profile SET points = 16 WHERE id = 12590;</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43">
         <v>12471</v>
       </c>
@@ -7696,7 +9284,7 @@
         <v>UPDATE profile SET points = 16 WHERE id = 12471;</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44">
         <v>11904</v>
       </c>
@@ -7729,7 +9317,7 @@
         <v>UPDATE profile SET points = 8 WHERE id = 11904;</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45">
         <v>12589</v>
       </c>
@@ -7762,7 +9350,7 @@
         <v>UPDATE profile SET points = 16 WHERE id = 12589;</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46">
         <v>12470</v>
       </c>
@@ -7795,7 +9383,7 @@
         <v>UPDATE profile SET points = 16 WHERE id = 12470;</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47">
         <v>11515</v>
       </c>
@@ -7829,7 +9417,7 @@
         <v>UPDATE profile SET points = 330 WHERE id = 11515;</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48">
         <v>11903</v>
       </c>
@@ -7862,7 +9450,7 @@
         <v>UPDATE profile SET points = 9 WHERE id = 11903;</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10">
       <c r="A49">
         <v>12588</v>
       </c>
@@ -7895,7 +9483,7 @@
         <v>UPDATE profile SET points = 18 WHERE id = 12588;</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50">
         <v>12469</v>
       </c>
@@ -7928,7 +9516,7 @@
         <v>UPDATE profile SET points = 18 WHERE id = 12469;</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51">
         <v>11510</v>
       </c>
@@ -7961,7 +9549,7 @@
         <v>UPDATE profile SET points = 59 WHERE id = 11510;</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10">
       <c r="A52">
         <v>11997</v>
       </c>
@@ -7994,7 +9582,7 @@
         <v>UPDATE profile SET points = 8 WHERE id = 11997;</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53">
         <v>12652</v>
       </c>
@@ -8027,7 +9615,7 @@
         <v>UPDATE profile SET points = 16 WHERE id = 12652;</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54">
         <v>12533</v>
       </c>

</xml_diff>

<commit_message>
Fixed points of Speerschleuder, Streitwagen and Zwillingskämpfer
</commit_message>
<xml_diff>
--- a/resources/db/Profiles.xlsx
+++ b/resources/db/Profiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\projects\ArmyBuilder\sourcecode\resources\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83DA700-B884-4358-AFA8-9DB4DD434C79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C726752A-74C8-4089-97AD-FF86DCFE8621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{72821A2A-92BA-4C26-854D-A2ECB76DE865}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="152">
   <si>
     <t>Hochelfen</t>
   </si>
@@ -496,12 +496,6 @@
   </si>
   <si>
     <t>add Löwenumhang</t>
-  </si>
-  <si>
-    <t>profile.points 90</t>
-  </si>
-  <si>
-    <t>profile.points 57</t>
   </si>
   <si>
     <t>delete main model</t>
@@ -5633,7 +5627,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G56" sqref="G56"/>
+      <selection pane="bottomLeft" activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -6751,7 +6745,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" hidden="1">
       <c r="A52">
         <v>11997</v>
       </c>
@@ -6762,20 +6756,20 @@
         <v>52</v>
       </c>
       <c r="D52">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E52">
         <v>11</v>
       </c>
       <c r="F52">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="G52" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" hidden="1">
       <c r="A53">
         <v>12652</v>
       </c>
@@ -6786,20 +6780,20 @@
         <v>111</v>
       </c>
       <c r="D53">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E53">
         <v>22</v>
       </c>
       <c r="F53">
         <f t="shared" si="0"/>
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="G53" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" hidden="1">
       <c r="A54">
         <v>12533</v>
       </c>
@@ -6810,20 +6804,20 @@
         <v>91</v>
       </c>
       <c r="D54">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E54">
         <v>22</v>
       </c>
       <c r="F54">
         <f t="shared" si="0"/>
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="G54" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" hidden="1">
       <c r="A55">
         <v>12091</v>
       </c>
@@ -6837,17 +6831,14 @@
         <v>100</v>
       </c>
       <c r="E55">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="F55">
         <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-      <c r="G55" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" hidden="1">
       <c r="A56">
         <v>12113</v>
       </c>
@@ -6861,14 +6852,11 @@
         <v>72</v>
       </c>
       <c r="E56">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="F56">
         <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="G56" t="s">
-        <v>152</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -6885,14 +6873,14 @@
         <v>84</v>
       </c>
       <c r="E57">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="F57">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="G57" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="58" spans="1:7" hidden="1">
@@ -7131,15 +7119,12 @@
     <filterColumn colId="5">
       <filters>
         <filter val="1"/>
+        <filter val="14"/>
         <filter val="2"/>
-        <filter val="-2"/>
         <filter val="3"/>
         <filter val="-4"/>
         <filter val="-50"/>
-        <filter val="57"/>
         <filter val="7"/>
-        <filter val="71"/>
-        <filter val="90"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Fixed points of standard bearer and musician
</commit_message>
<xml_diff>
--- a/resources/db/Profiles.xlsx
+++ b/resources/db/Profiles.xlsx
@@ -8,21 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\projects\ArmyBuilder\sourcecode\resources\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2AC30A-4B03-44D3-A56B-D082A8040F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1C09D6-2A27-4C05-8572-1A5D77A6F1B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{72821A2A-92BA-4C26-854D-A2ECB76DE865}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{72821A2A-92BA-4C26-854D-A2ECB76DE865}"/>
   </bookViews>
   <sheets>
     <sheet name="High Elf Profiles" sheetId="1" r:id="rId1"/>
     <sheet name="High Elf Fixed Profiles" sheetId="3" r:id="rId2"/>
     <sheet name="High Elf Profile Names" sheetId="5" r:id="rId3"/>
-    <sheet name="Tabelle1" sheetId="6" r:id="rId4"/>
+    <sheet name="High Elf Points Difference" sheetId="6" r:id="rId4"/>
     <sheet name="High Elf Wrong Profiles" sheetId="4" r:id="rId5"/>
     <sheet name="High Elf Points" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'High Elf Points Difference'!$A$1:$G$67</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'High Elf Profile Names'!$B$1:$F$73</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Tabelle1!$A$1:$G$68</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="148">
   <si>
     <t>Hochelfen</t>
   </si>
@@ -487,21 +487,6 @@
   </si>
   <si>
     <t>new points are correct, because auf light armor</t>
-  </si>
-  <si>
-    <t>add Löwenumhang</t>
-  </si>
-  <si>
-    <t>delete main model</t>
-  </si>
-  <si>
-    <t>add Zweihänder von Hoeth</t>
-  </si>
-  <si>
-    <t>add Schattenumhang</t>
-  </si>
-  <si>
-    <t>create extra Armeestandard profile</t>
   </si>
 </sst>
 </file>
@@ -5626,11 +5611,11 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2547C117-82C3-4BEF-8EA7-BDB626B12945}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G44" sqref="G44"/>
+      <selection pane="bottomLeft" activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -5700,11 +5685,11 @@
         <v>285</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F66" si="0">D3-E3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <f t="shared" ref="F3:F65" si="0">D3-E3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" hidden="1">
       <c r="A4">
         <v>11507</v>
       </c>
@@ -5718,14 +5703,11 @@
         <v>98</v>
       </c>
       <c r="E4">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G4" t="s">
-        <v>152</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" hidden="1">
@@ -6106,7 +6088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" hidden="1">
       <c r="A23">
         <v>12585</v>
       </c>
@@ -6120,14 +6102,14 @@
         <v>86</v>
       </c>
       <c r="E23">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" hidden="1">
       <c r="A24">
         <v>12466</v>
       </c>
@@ -6141,11 +6123,11 @@
         <v>86</v>
       </c>
       <c r="E24">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F24">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -6183,11 +6165,11 @@
         <v>50</v>
       </c>
       <c r="E26">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -6204,11 +6186,11 @@
         <v>50</v>
       </c>
       <c r="E27">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F27">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:7" hidden="1">
@@ -6322,7 +6304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" hidden="1">
+    <row r="33" spans="1:6" hidden="1">
       <c r="A33">
         <v>12468</v>
       </c>
@@ -6343,7 +6325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:6" hidden="1">
       <c r="A34">
         <v>11907</v>
       </c>
@@ -6357,17 +6339,14 @@
         <v>12</v>
       </c>
       <c r="E34">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F34">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G34" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" hidden="1">
       <c r="A35">
         <v>12592</v>
       </c>
@@ -6381,17 +6360,14 @@
         <v>24</v>
       </c>
       <c r="E35">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F35">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G35" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" hidden="1">
       <c r="A36">
         <v>12473</v>
       </c>
@@ -6405,17 +6381,14 @@
         <v>24</v>
       </c>
       <c r="E36">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F36">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G36" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" hidden="1">
       <c r="A37">
         <v>11901</v>
       </c>
@@ -6429,17 +6402,14 @@
         <v>16</v>
       </c>
       <c r="E37">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F37">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G37" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" hidden="1">
       <c r="A38">
         <v>12586</v>
       </c>
@@ -6453,17 +6423,14 @@
         <v>32</v>
       </c>
       <c r="E38">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F38">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G38" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" hidden="1">
       <c r="A39">
         <v>12467</v>
       </c>
@@ -6477,17 +6444,14 @@
         <v>32</v>
       </c>
       <c r="E39">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F39">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G39" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" hidden="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" hidden="1">
       <c r="A40">
         <v>11905</v>
       </c>
@@ -6508,7 +6472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" hidden="1">
+    <row r="41" spans="1:6" hidden="1">
       <c r="A41">
         <v>12590</v>
       </c>
@@ -6529,7 +6493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7" hidden="1">
+    <row r="42" spans="1:6" hidden="1">
       <c r="A42">
         <v>12471</v>
       </c>
@@ -6550,7 +6514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" hidden="1">
+    <row r="43" spans="1:6" hidden="1">
       <c r="A43">
         <v>11899</v>
       </c>
@@ -6571,7 +6535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:6" hidden="1">
       <c r="A44">
         <v>12584</v>
       </c>
@@ -6585,14 +6549,14 @@
         <v>62</v>
       </c>
       <c r="E44">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F44">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" hidden="1">
       <c r="A45">
         <v>12465</v>
       </c>
@@ -6606,14 +6570,14 @@
         <v>62</v>
       </c>
       <c r="E45">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F45">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" hidden="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" hidden="1">
       <c r="A46">
         <v>11904</v>
       </c>
@@ -6634,7 +6598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" hidden="1">
+    <row r="47" spans="1:6" hidden="1">
       <c r="A47">
         <v>12589</v>
       </c>
@@ -6655,7 +6619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7" hidden="1">
+    <row r="48" spans="1:6" hidden="1">
       <c r="A48">
         <v>12470</v>
       </c>
@@ -6676,7 +6640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" hidden="1">
       <c r="A49">
         <v>11903</v>
       </c>
@@ -6690,17 +6654,14 @@
         <v>16</v>
       </c>
       <c r="E49">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F49">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G49" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" hidden="1">
       <c r="A50">
         <v>12588</v>
       </c>
@@ -6714,17 +6675,14 @@
         <v>32</v>
       </c>
       <c r="E50">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F50">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G50" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" hidden="1">
       <c r="A51">
         <v>12469</v>
       </c>
@@ -6738,14 +6696,11 @@
         <v>32</v>
       </c>
       <c r="E51">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F51">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G51" t="s">
-        <v>148</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:7" hidden="1">
@@ -6862,45 +6817,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" hidden="1">
       <c r="A57">
-        <v>12118</v>
+        <v>12243</v>
       </c>
       <c r="B57" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C57" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D57">
-        <v>84</v>
+        <v>150</v>
       </c>
       <c r="E57">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="F57">
         <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="G57" t="s">
-        <v>149</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:7" hidden="1">
       <c r="A58">
-        <v>12243</v>
+        <v>12236</v>
       </c>
       <c r="B58" t="s">
         <v>140</v>
       </c>
       <c r="C58" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D58">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="E58">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="F58">
         <f t="shared" si="0"/>
@@ -6909,19 +6861,19 @@
     </row>
     <row r="59" spans="1:7" hidden="1">
       <c r="A59">
-        <v>12236</v>
+        <v>12286</v>
       </c>
       <c r="B59" t="s">
         <v>140</v>
       </c>
       <c r="C59" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D59">
-        <v>250</v>
+        <v>450</v>
       </c>
       <c r="E59">
-        <v>250</v>
+        <v>450</v>
       </c>
       <c r="F59">
         <f t="shared" si="0"/>
@@ -6930,19 +6882,19 @@
     </row>
     <row r="60" spans="1:7" hidden="1">
       <c r="A60">
-        <v>12286</v>
+        <v>12163</v>
       </c>
       <c r="B60" t="s">
         <v>140</v>
       </c>
       <c r="C60" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D60">
-        <v>450</v>
+        <v>90</v>
       </c>
       <c r="E60">
-        <v>450</v>
+        <v>90</v>
       </c>
       <c r="F60">
         <f t="shared" si="0"/>
@@ -6951,19 +6903,19 @@
     </row>
     <row r="61" spans="1:7" hidden="1">
       <c r="A61">
-        <v>12163</v>
+        <v>12269</v>
       </c>
       <c r="B61" t="s">
         <v>140</v>
       </c>
       <c r="C61" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D61">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="E61">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="F61">
         <f t="shared" si="0"/>
@@ -6972,19 +6924,19 @@
     </row>
     <row r="62" spans="1:7" hidden="1">
       <c r="A62">
-        <v>12269</v>
+        <v>12294</v>
       </c>
       <c r="B62" t="s">
         <v>140</v>
       </c>
       <c r="C62" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D62">
-        <v>150</v>
+        <v>600</v>
       </c>
       <c r="E62">
-        <v>150</v>
+        <v>600</v>
       </c>
       <c r="F62">
         <f t="shared" si="0"/>
@@ -6993,19 +6945,19 @@
     </row>
     <row r="63" spans="1:7" hidden="1">
       <c r="A63">
-        <v>12294</v>
+        <v>12278</v>
       </c>
       <c r="B63" t="s">
         <v>140</v>
       </c>
       <c r="C63" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D63">
-        <v>600</v>
+        <v>145</v>
       </c>
       <c r="E63">
-        <v>600</v>
+        <v>145</v>
       </c>
       <c r="F63">
         <f t="shared" si="0"/>
@@ -7014,19 +6966,19 @@
     </row>
     <row r="64" spans="1:7" hidden="1">
       <c r="A64">
-        <v>12278</v>
+        <v>12302</v>
       </c>
       <c r="B64" t="s">
         <v>140</v>
       </c>
       <c r="C64" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D64">
-        <v>145</v>
+        <v>750</v>
       </c>
       <c r="E64">
-        <v>145</v>
+        <v>750</v>
       </c>
       <c r="F64">
         <f t="shared" si="0"/>
@@ -7035,19 +6987,19 @@
     </row>
     <row r="65" spans="1:6" hidden="1">
       <c r="A65">
-        <v>12302</v>
+        <v>12250</v>
       </c>
       <c r="B65" t="s">
         <v>140</v>
       </c>
       <c r="C65" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D65">
-        <v>750</v>
+        <v>200</v>
       </c>
       <c r="E65">
-        <v>750</v>
+        <v>200</v>
       </c>
       <c r="F65">
         <f t="shared" si="0"/>
@@ -7056,78 +7008,54 @@
     </row>
     <row r="66" spans="1:6" hidden="1">
       <c r="A66">
-        <v>12250</v>
+        <v>12167</v>
       </c>
       <c r="B66" t="s">
         <v>140</v>
       </c>
       <c r="C66" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D66">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="E66">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="F66">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F66:F67" si="1">D66-E66</f>
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:6" hidden="1">
       <c r="A67">
-        <v>12167</v>
+        <v>12162</v>
       </c>
       <c r="B67" t="s">
         <v>140</v>
       </c>
       <c r="C67" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D67">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="E67">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="F67">
-        <f t="shared" ref="F67:F68" si="1">D67-E67</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" hidden="1">
-      <c r="A68">
-        <v>12162</v>
-      </c>
-      <c r="B68" t="s">
-        <v>140</v>
-      </c>
-      <c r="C68" t="s">
-        <v>60</v>
-      </c>
-      <c r="D68">
-        <v>75</v>
-      </c>
-      <c r="E68">
-        <v>75</v>
-      </c>
-      <c r="F68">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G68" xr:uid="{2547C117-82C3-4BEF-8EA7-BDB626B12945}">
+  <autoFilter ref="A1:G67" xr:uid="{2547C117-82C3-4BEF-8EA7-BDB626B12945}">
     <filterColumn colId="5">
       <filters>
-        <filter val="1"/>
-        <filter val="14"/>
         <filter val="2"/>
-        <filter val="3"/>
+        <filter val="4"/>
         <filter val="-4"/>
         <filter val="-50"/>
-        <filter val="7"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Fixed profile points of dark elf army list
</commit_message>
<xml_diff>
--- a/resources/db/Profiles.xlsx
+++ b/resources/db/Profiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simone\projects\ArmyBuilder\resources\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5BA895-CAB8-4692-8ED3-E84A3E4246F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CFB923-4FC0-4D4C-A072-68338FBFF9E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{72821A2A-92BA-4C26-854D-A2ECB76DE865}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="330">
   <si>
     <t>General</t>
   </si>
@@ -1020,9 +1020,6 @@
   </si>
   <si>
     <t>Elfen Elite</t>
-  </si>
-  <si>
-    <t>Elfen Armeestandarte</t>
   </si>
 </sst>
 </file>
@@ -3647,7 +3644,8 @@
   <dimension ref="A1:J62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -3742,14 +3740,14 @@
         <v>11509</v>
       </c>
       <c r="H3" t="s">
-        <v>330</v>
+        <v>305</v>
       </c>
       <c r="I3">
-        <v>98</v>
+        <v>48</v>
       </c>
       <c r="J3" t="str">
         <f t="shared" ref="J3:J44" si="0">CONCATENATE("UPDATE profile SET name = '",H3,"', points = ",I3," WHERE id =",G3,";")</f>
-        <v>UPDATE profile SET name = 'Elfen Armeestandarte', points = 98 WHERE id =11509;</v>
+        <v>UPDATE profile SET name = 'Elfen Champion', points = 48 WHERE id =11509;</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -5637,8 +5635,8 @@
   <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D66" sqref="D66"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>

</xml_diff>

<commit_message>
Started assigning points to profiles of Orc & Goblin army list
</commit_message>
<xml_diff>
--- a/resources/db/Profiles.xlsx
+++ b/resources/db/Profiles.xlsx
@@ -1,36 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simone\projects\ArmyBuilder\resources\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\projects\ArmyBuilder\sourcecode\resources\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CFB923-4FC0-4D4C-A072-68338FBFF9E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE0D7CB-8B54-4793-993D-6B9713B79FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{72821A2A-92BA-4C26-854D-A2ECB76DE865}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{72821A2A-92BA-4C26-854D-A2ECB76DE865}"/>
   </bookViews>
   <sheets>
-    <sheet name="Dwarven Profiles" sheetId="7" r:id="rId1"/>
-    <sheet name="Dark Elf Profiles" sheetId="8" r:id="rId2"/>
-    <sheet name="High Elf Profiles" sheetId="5" r:id="rId3"/>
+    <sheet name="Orcs &amp; Goblins Profiles" sheetId="9" r:id="rId1"/>
+    <sheet name="Dwarven Profiles" sheetId="7" r:id="rId2"/>
+    <sheet name="Dark Elf Profiles" sheetId="8" r:id="rId3"/>
+    <sheet name="High Elf Profiles" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'High Elf Profiles'!$B$1:$F$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'High Elf Profiles'!$B$1:$F$73</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1375" uniqueCount="487">
   <si>
     <t>General</t>
   </si>
@@ -1020,6 +1030,477 @@
   </si>
   <si>
     <t>Elfen Elite</t>
+  </si>
+  <si>
+    <t>Orks &amp; Goblins</t>
+  </si>
+  <si>
+    <t>Grom der Fettsack vom Nebelberg</t>
+  </si>
+  <si>
+    <t>Grom</t>
+  </si>
+  <si>
+    <t>Niblit</t>
+  </si>
+  <si>
+    <t>Riesenwolf</t>
+  </si>
+  <si>
+    <t>Gorbad Eisenfaust</t>
+  </si>
+  <si>
+    <t>Gorbad</t>
+  </si>
+  <si>
+    <t>Morglum Knochenbrecher</t>
+  </si>
+  <si>
+    <t>Morglum</t>
+  </si>
+  <si>
+    <t>Oglok der Fürchtaliche</t>
+  </si>
+  <si>
+    <t>Oglok</t>
+  </si>
+  <si>
+    <t>Skarsnik, Herrscher der Acht Gipfel</t>
+  </si>
+  <si>
+    <t>Skarsnik</t>
+  </si>
+  <si>
+    <t>Gobbla</t>
+  </si>
+  <si>
+    <t>Ork Chefoberboss</t>
+  </si>
+  <si>
+    <t>Schwarzork Chefoberboss</t>
+  </si>
+  <si>
+    <t>Wildork Chefoberboss</t>
+  </si>
+  <si>
+    <t>Goblin Chefoberboss</t>
+  </si>
+  <si>
+    <t>Waldgoblin Chefoberboss</t>
+  </si>
+  <si>
+    <t>Nachtgoblin Chefoberboss</t>
+  </si>
+  <si>
+    <t>Schwarzork Armeestandarte</t>
+  </si>
+  <si>
+    <t>Ork Armeestandarte</t>
+  </si>
+  <si>
+    <t>Wildork Armeestandarte</t>
+  </si>
+  <si>
+    <t>Goblin Armeestandarte</t>
+  </si>
+  <si>
+    <t>Waldgoblin Armeestandarte</t>
+  </si>
+  <si>
+    <t>Nachtgoblin Armeestandarte</t>
+  </si>
+  <si>
+    <t>Schwarzork Oberboss</t>
+  </si>
+  <si>
+    <t>Ork Oberboss</t>
+  </si>
+  <si>
+    <t>Wildork Oberboss</t>
+  </si>
+  <si>
+    <t>Goblin Oberboss</t>
+  </si>
+  <si>
+    <t>Waldgoblin Oberboss</t>
+  </si>
+  <si>
+    <t>Nachtgoblin Oberboss</t>
+  </si>
+  <si>
+    <t>Schwarzork Boss</t>
+  </si>
+  <si>
+    <t>Ork Boss</t>
+  </si>
+  <si>
+    <t>Wildork Boss</t>
+  </si>
+  <si>
+    <t>Goblin Boss</t>
+  </si>
+  <si>
+    <t>Waldgoblin Boss</t>
+  </si>
+  <si>
+    <t>Nachtgoblin Boss</t>
+  </si>
+  <si>
+    <t>Ork Schamane</t>
+  </si>
+  <si>
+    <t>Wildork Schamane</t>
+  </si>
+  <si>
+    <t>Goblin Schamane</t>
+  </si>
+  <si>
+    <t>Nachtgoblin Schamane</t>
+  </si>
+  <si>
+    <t>Waldgoblin Schamane</t>
+  </si>
+  <si>
+    <t>Ork Oberschamane</t>
+  </si>
+  <si>
+    <t>Wildork Oberschamane</t>
+  </si>
+  <si>
+    <t>Goblin Oberschamane</t>
+  </si>
+  <si>
+    <t>Nachtgoblin Oberschamane</t>
+  </si>
+  <si>
+    <t>Waldgoblin Oberschamane</t>
+  </si>
+  <si>
+    <t>Ork Großschamane</t>
+  </si>
+  <si>
+    <t>Wildork Großschamane</t>
+  </si>
+  <si>
+    <t>Goblin Großschamane</t>
+  </si>
+  <si>
+    <t>Nachtgoblin Großschamane</t>
+  </si>
+  <si>
+    <t>Waldgoblin Großschamane</t>
+  </si>
+  <si>
+    <t>Ork Meisterschamane</t>
+  </si>
+  <si>
+    <t>Wildork Meisterschamane</t>
+  </si>
+  <si>
+    <t>Goblin Meisterschamane</t>
+  </si>
+  <si>
+    <t>Nachtgoblin Meisterschamane</t>
+  </si>
+  <si>
+    <t>Waldgoblin Meisterschamane</t>
+  </si>
+  <si>
+    <t>Gorfang Rotzahn</t>
+  </si>
+  <si>
+    <t>Azhag der Vernichter</t>
+  </si>
+  <si>
+    <t>Wildork Schweinereiter</t>
+  </si>
+  <si>
+    <t>Wildork</t>
+  </si>
+  <si>
+    <t>Wildschwein</t>
+  </si>
+  <si>
+    <t>Ork Schweinereiter</t>
+  </si>
+  <si>
+    <t>Ork</t>
+  </si>
+  <si>
+    <t>Goblin Wolfsreiter</t>
+  </si>
+  <si>
+    <t>Goblin</t>
+  </si>
+  <si>
+    <t>Waldgoblin Spinnenreiter</t>
+  </si>
+  <si>
+    <t>Waldgoblin</t>
+  </si>
+  <si>
+    <t>Riesenspinne</t>
+  </si>
+  <si>
+    <t>Grobgitz</t>
+  </si>
+  <si>
+    <t>Grobgit</t>
+  </si>
+  <si>
+    <t>Orks</t>
+  </si>
+  <si>
+    <t>Ork Bogenschützen</t>
+  </si>
+  <si>
+    <t>Ork Bogenschütze</t>
+  </si>
+  <si>
+    <t>Schwarzorks</t>
+  </si>
+  <si>
+    <t>Schwarzork</t>
+  </si>
+  <si>
+    <t>Wildorks</t>
+  </si>
+  <si>
+    <t>Goblins</t>
+  </si>
+  <si>
+    <t>Waldgoblins</t>
+  </si>
+  <si>
+    <t>Nachtgoblins</t>
+  </si>
+  <si>
+    <t>Nachtgoblin</t>
+  </si>
+  <si>
+    <t>Squigjäger</t>
+  </si>
+  <si>
+    <t>Höhlensquig</t>
+  </si>
+  <si>
+    <t>Netzgitz</t>
+  </si>
+  <si>
+    <t>Nachtgoblin Fanatics</t>
+  </si>
+  <si>
+    <t>Fanatic</t>
+  </si>
+  <si>
+    <t>Squigreiter</t>
+  </si>
+  <si>
+    <t>Riese</t>
+  </si>
+  <si>
+    <t>Oger</t>
+  </si>
+  <si>
+    <t>Flußtrolle</t>
+  </si>
+  <si>
+    <t>Flußtroll</t>
+  </si>
+  <si>
+    <t>Steintrolle</t>
+  </si>
+  <si>
+    <t>Steintroll</t>
+  </si>
+  <si>
+    <t>Snotlings</t>
+  </si>
+  <si>
+    <t>Snotling-Base</t>
+  </si>
+  <si>
+    <t>Schädelquetscha</t>
+  </si>
+  <si>
+    <t>Besatzung</t>
+  </si>
+  <si>
+    <t>Menschenfetza</t>
+  </si>
+  <si>
+    <t>Snotling Kurbelwagen</t>
+  </si>
+  <si>
+    <t>Snotling</t>
+  </si>
+  <si>
+    <t>Kurbelwagen</t>
+  </si>
+  <si>
+    <t>Kamikaze Katapult</t>
+  </si>
+  <si>
+    <t>Kamikaze</t>
+  </si>
+  <si>
+    <t>Katapult</t>
+  </si>
+  <si>
+    <t>Ork Streitwagen</t>
+  </si>
+  <si>
+    <t>Orkbesatzung</t>
+  </si>
+  <si>
+    <t>Goblin Wolfsstreitwagen</t>
+  </si>
+  <si>
+    <t>Orks Niblit</t>
+  </si>
+  <si>
+    <t>Orks Gobbla</t>
+  </si>
+  <si>
+    <t>Orks Ork Chefoberboss</t>
+  </si>
+  <si>
+    <t>Orks Schwarzork Chefoberboss</t>
+  </si>
+  <si>
+    <t>Orks Wildork Chefoberboss</t>
+  </si>
+  <si>
+    <t>Orks Goblin Chefoberboss</t>
+  </si>
+  <si>
+    <t>Orks Waldgoblin Chefoberboss</t>
+  </si>
+  <si>
+    <t>Orks Nachtgoblin Chefoberboss</t>
+  </si>
+  <si>
+    <t>Orks Schwarzork Armeestandarte</t>
+  </si>
+  <si>
+    <t>Orks Ork Armeestandarte</t>
+  </si>
+  <si>
+    <t>Orks Wildork Armeestandarte</t>
+  </si>
+  <si>
+    <t>Orks Goblin Armeestandarte</t>
+  </si>
+  <si>
+    <t>Orks Waldgoblin Armeestandarte</t>
+  </si>
+  <si>
+    <t>Orks Nachtgoblin Armeestandarte</t>
+  </si>
+  <si>
+    <t>Orks Schwarzork Oberboss</t>
+  </si>
+  <si>
+    <t>Orks Ork Oberboss</t>
+  </si>
+  <si>
+    <t>Orks Wildork Oberboss</t>
+  </si>
+  <si>
+    <t>Orks Goblin Oberboss</t>
+  </si>
+  <si>
+    <t>Orks Waldgoblin Oberboss</t>
+  </si>
+  <si>
+    <t>Orks Nachtgoblin Oberboss</t>
+  </si>
+  <si>
+    <t>Orks Schwarzork Boss</t>
+  </si>
+  <si>
+    <t>Orks Ork Boss</t>
+  </si>
+  <si>
+    <t>Orks Wildork Boss</t>
+  </si>
+  <si>
+    <t>Orks Goblin Boss</t>
+  </si>
+  <si>
+    <t>Orks Waldgoblin Boss</t>
+  </si>
+  <si>
+    <t>Orks Nachtgoblin Boss</t>
+  </si>
+  <si>
+    <t>Orks Ork Schamane</t>
+  </si>
+  <si>
+    <t>Orks Wildork Schamane</t>
+  </si>
+  <si>
+    <t>Orks Goblin Schamane</t>
+  </si>
+  <si>
+    <t>Orks Nachtgoblin Schamane</t>
+  </si>
+  <si>
+    <t>Orks Waldgoblin Schamane</t>
+  </si>
+  <si>
+    <t>Orks Ork Oberschamane</t>
+  </si>
+  <si>
+    <t>Orks Wildork Oberschamane</t>
+  </si>
+  <si>
+    <t>Orks Grom der Fettsack vom Nebelberg</t>
+  </si>
+  <si>
+    <t>Orks Gorbad Eisenfause</t>
+  </si>
+  <si>
+    <t>Orks Skarsnik Herrscher der Acht Gipfel</t>
+  </si>
+  <si>
+    <t>Orks Goblin Oberschamane</t>
+  </si>
+  <si>
+    <t>Orks Nachtgoblin Oberschamane</t>
+  </si>
+  <si>
+    <t>Orks Waldgoblin Oberschamane</t>
+  </si>
+  <si>
+    <t>Orks Ork Großschamane</t>
+  </si>
+  <si>
+    <t>Orks Wildork Großschamane</t>
+  </si>
+  <si>
+    <t>Orks Goblin Großschamane</t>
+  </si>
+  <si>
+    <t>Orks Nachtgoblin Großschamane</t>
+  </si>
+  <si>
+    <t>Orks Waldgoblin Großschamane</t>
+  </si>
+  <si>
+    <t>Orks Ork Meisterschamane</t>
+  </si>
+  <si>
+    <t>Orks Wildork Meisterschamane</t>
+  </si>
+  <si>
+    <t>Orks Goblin Meisterschamane</t>
+  </si>
+  <si>
+    <t>Orks Nachtgoblin Meisterschamane</t>
+  </si>
+  <si>
+    <t>Orks Waldgoblin Meisterschamane</t>
   </si>
 </sst>
 </file>
@@ -1407,12 +1888,3709 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73F0926A-28CA-48B1-B472-BA874B7E1E5A}">
+  <dimension ref="A1:J118"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I22" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C2">
+        <v>11421</v>
+      </c>
+      <c r="D2" t="s">
+        <v>331</v>
+      </c>
+      <c r="E2">
+        <v>46406</v>
+      </c>
+      <c r="F2" t="s">
+        <v>332</v>
+      </c>
+      <c r="G2">
+        <v>11421</v>
+      </c>
+      <c r="H2" t="s">
+        <v>471</v>
+      </c>
+      <c r="I2">
+        <v>80</v>
+      </c>
+      <c r="J2" t="str">
+        <f t="shared" ref="J2:J65" si="0">CONCATENATE("UPDATE profile SET name = '",H2,"', points = ",I2," WHERE id =",G2,";")</f>
+        <v>UPDATE profile SET name = 'Orks Grom der Fettsack vom Nebelberg', points = 80 WHERE id =11421;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>330</v>
+      </c>
+      <c r="C3">
+        <v>11421</v>
+      </c>
+      <c r="D3" t="s">
+        <v>331</v>
+      </c>
+      <c r="E3">
+        <v>46757</v>
+      </c>
+      <c r="F3" t="s">
+        <v>333</v>
+      </c>
+      <c r="G3">
+        <v>11791</v>
+      </c>
+      <c r="H3" t="s">
+        <v>438</v>
+      </c>
+      <c r="I3">
+        <v>65</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Niblit', points = 65 WHERE id =11791;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>330</v>
+      </c>
+      <c r="C4">
+        <v>11421</v>
+      </c>
+      <c r="D4" t="s">
+        <v>331</v>
+      </c>
+      <c r="E4">
+        <v>46876</v>
+      </c>
+      <c r="F4" t="s">
+        <v>334</v>
+      </c>
+      <c r="G4">
+        <v>11841</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11841;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>330</v>
+      </c>
+      <c r="C5">
+        <v>11422</v>
+      </c>
+      <c r="D5" t="s">
+        <v>335</v>
+      </c>
+      <c r="E5">
+        <v>46407</v>
+      </c>
+      <c r="F5" t="s">
+        <v>336</v>
+      </c>
+      <c r="G5">
+        <v>11422</v>
+      </c>
+      <c r="H5" t="s">
+        <v>472</v>
+      </c>
+      <c r="I5">
+        <v>120</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Gorbad Eisenfause', points = 120 WHERE id =11422;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>330</v>
+      </c>
+      <c r="C6">
+        <v>11423</v>
+      </c>
+      <c r="D6" t="s">
+        <v>337</v>
+      </c>
+      <c r="E6">
+        <v>46408</v>
+      </c>
+      <c r="F6" t="s">
+        <v>338</v>
+      </c>
+      <c r="G6">
+        <v>11423</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11423;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>330</v>
+      </c>
+      <c r="C7">
+        <v>11424</v>
+      </c>
+      <c r="D7" t="s">
+        <v>339</v>
+      </c>
+      <c r="E7">
+        <v>46409</v>
+      </c>
+      <c r="F7" t="s">
+        <v>340</v>
+      </c>
+      <c r="G7">
+        <v>11424</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11424;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>330</v>
+      </c>
+      <c r="C8">
+        <v>11425</v>
+      </c>
+      <c r="D8" t="s">
+        <v>341</v>
+      </c>
+      <c r="E8">
+        <v>46410</v>
+      </c>
+      <c r="F8" t="s">
+        <v>342</v>
+      </c>
+      <c r="G8">
+        <v>11425</v>
+      </c>
+      <c r="H8" t="s">
+        <v>473</v>
+      </c>
+      <c r="I8">
+        <v>80</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Skarsnik Herrscher der Acht Gipfel', points = 80 WHERE id =11425;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>330</v>
+      </c>
+      <c r="C9">
+        <v>11425</v>
+      </c>
+      <c r="D9" t="s">
+        <v>341</v>
+      </c>
+      <c r="E9">
+        <v>46758</v>
+      </c>
+      <c r="F9" t="s">
+        <v>343</v>
+      </c>
+      <c r="G9">
+        <v>11792</v>
+      </c>
+      <c r="H9" t="s">
+        <v>439</v>
+      </c>
+      <c r="I9">
+        <v>50</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Gobbla', points = 50 WHERE id =11792;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>330</v>
+      </c>
+      <c r="C10">
+        <v>11426</v>
+      </c>
+      <c r="D10" t="s">
+        <v>344</v>
+      </c>
+      <c r="E10">
+        <v>46411</v>
+      </c>
+      <c r="F10" t="s">
+        <v>344</v>
+      </c>
+      <c r="G10">
+        <v>11426</v>
+      </c>
+      <c r="H10" t="s">
+        <v>440</v>
+      </c>
+      <c r="I10">
+        <v>110</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Ork Chefoberboss', points = 110 WHERE id =11426;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>330</v>
+      </c>
+      <c r="C11">
+        <v>11427</v>
+      </c>
+      <c r="D11" t="s">
+        <v>345</v>
+      </c>
+      <c r="E11">
+        <v>46412</v>
+      </c>
+      <c r="F11" t="s">
+        <v>345</v>
+      </c>
+      <c r="G11">
+        <v>11427</v>
+      </c>
+      <c r="H11" t="s">
+        <v>441</v>
+      </c>
+      <c r="I11">
+        <v>140</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Schwarzork Chefoberboss', points = 140 WHERE id =11427;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>330</v>
+      </c>
+      <c r="C12">
+        <v>11428</v>
+      </c>
+      <c r="D12" t="s">
+        <v>346</v>
+      </c>
+      <c r="E12">
+        <v>46413</v>
+      </c>
+      <c r="F12" t="s">
+        <v>346</v>
+      </c>
+      <c r="G12">
+        <v>11428</v>
+      </c>
+      <c r="H12" t="s">
+        <v>442</v>
+      </c>
+      <c r="I12">
+        <v>150</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Wildork Chefoberboss', points = 150 WHERE id =11428;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>330</v>
+      </c>
+      <c r="C13">
+        <v>11429</v>
+      </c>
+      <c r="D13" t="s">
+        <v>347</v>
+      </c>
+      <c r="E13">
+        <v>46414</v>
+      </c>
+      <c r="F13" t="s">
+        <v>347</v>
+      </c>
+      <c r="G13">
+        <v>11429</v>
+      </c>
+      <c r="H13" t="s">
+        <v>443</v>
+      </c>
+      <c r="I13">
+        <v>50</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Goblin Chefoberboss', points = 50 WHERE id =11429;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>330</v>
+      </c>
+      <c r="C14">
+        <v>11430</v>
+      </c>
+      <c r="D14" t="s">
+        <v>348</v>
+      </c>
+      <c r="E14">
+        <v>46415</v>
+      </c>
+      <c r="F14" t="s">
+        <v>348</v>
+      </c>
+      <c r="G14">
+        <v>11430</v>
+      </c>
+      <c r="H14" t="s">
+        <v>444</v>
+      </c>
+      <c r="I14">
+        <v>50</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Waldgoblin Chefoberboss', points = 50 WHERE id =11430;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>330</v>
+      </c>
+      <c r="C15">
+        <v>11431</v>
+      </c>
+      <c r="D15" t="s">
+        <v>349</v>
+      </c>
+      <c r="E15">
+        <v>46416</v>
+      </c>
+      <c r="F15" t="s">
+        <v>349</v>
+      </c>
+      <c r="G15">
+        <v>11431</v>
+      </c>
+      <c r="H15" t="s">
+        <v>445</v>
+      </c>
+      <c r="I15">
+        <v>50</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Nachtgoblin Chefoberboss', points = 50 WHERE id =11431;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>330</v>
+      </c>
+      <c r="C16">
+        <v>11432</v>
+      </c>
+      <c r="D16" t="s">
+        <v>350</v>
+      </c>
+      <c r="E16">
+        <v>46417</v>
+      </c>
+      <c r="F16" t="s">
+        <v>350</v>
+      </c>
+      <c r="G16">
+        <v>11432</v>
+      </c>
+      <c r="H16" t="s">
+        <v>446</v>
+      </c>
+      <c r="I16">
+        <v>92</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Schwarzork Armeestandarte', points = 92 WHERE id =11432;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
+        <v>330</v>
+      </c>
+      <c r="C17">
+        <v>11433</v>
+      </c>
+      <c r="D17" t="s">
+        <v>351</v>
+      </c>
+      <c r="E17">
+        <v>46418</v>
+      </c>
+      <c r="F17" t="s">
+        <v>351</v>
+      </c>
+      <c r="G17">
+        <v>11433</v>
+      </c>
+      <c r="H17" t="s">
+        <v>447</v>
+      </c>
+      <c r="I17">
+        <v>83</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Ork Armeestandarte', points = 83 WHERE id =11433;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18">
+        <v>9</v>
+      </c>
+      <c r="B18" t="s">
+        <v>330</v>
+      </c>
+      <c r="C18">
+        <v>11434</v>
+      </c>
+      <c r="D18" t="s">
+        <v>352</v>
+      </c>
+      <c r="E18">
+        <v>46419</v>
+      </c>
+      <c r="F18" t="s">
+        <v>352</v>
+      </c>
+      <c r="G18">
+        <v>11434</v>
+      </c>
+      <c r="H18" t="s">
+        <v>448</v>
+      </c>
+      <c r="I18">
+        <v>95</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Wildork Armeestandarte', points = 95 WHERE id =11434;</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
+        <v>330</v>
+      </c>
+      <c r="C19">
+        <v>11435</v>
+      </c>
+      <c r="D19" t="s">
+        <v>353</v>
+      </c>
+      <c r="E19">
+        <v>46420</v>
+      </c>
+      <c r="F19" t="s">
+        <v>353</v>
+      </c>
+      <c r="G19">
+        <v>11435</v>
+      </c>
+      <c r="H19" t="s">
+        <v>449</v>
+      </c>
+      <c r="I19">
+        <v>65</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Goblin Armeestandarte', points = 65 WHERE id =11435;</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>330</v>
+      </c>
+      <c r="C20">
+        <v>11436</v>
+      </c>
+      <c r="D20" t="s">
+        <v>354</v>
+      </c>
+      <c r="E20">
+        <v>46421</v>
+      </c>
+      <c r="F20" t="s">
+        <v>354</v>
+      </c>
+      <c r="G20">
+        <v>11436</v>
+      </c>
+      <c r="H20" t="s">
+        <v>450</v>
+      </c>
+      <c r="I20">
+        <v>65</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Waldgoblin Armeestandarte', points = 65 WHERE id =11436;</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>330</v>
+      </c>
+      <c r="C21">
+        <v>11437</v>
+      </c>
+      <c r="D21" t="s">
+        <v>355</v>
+      </c>
+      <c r="E21">
+        <v>46422</v>
+      </c>
+      <c r="F21" t="s">
+        <v>355</v>
+      </c>
+      <c r="G21">
+        <v>11437</v>
+      </c>
+      <c r="H21" t="s">
+        <v>451</v>
+      </c>
+      <c r="I21">
+        <v>65</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Nachtgoblin Armeestandarte', points = 65 WHERE id =11437;</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22">
+        <v>9</v>
+      </c>
+      <c r="B22" t="s">
+        <v>330</v>
+      </c>
+      <c r="C22">
+        <v>11438</v>
+      </c>
+      <c r="D22" t="s">
+        <v>356</v>
+      </c>
+      <c r="E22">
+        <v>46423</v>
+      </c>
+      <c r="F22" t="s">
+        <v>356</v>
+      </c>
+      <c r="G22">
+        <v>11438</v>
+      </c>
+      <c r="H22" t="s">
+        <v>452</v>
+      </c>
+      <c r="I22" t="s">
+        <v>1</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Schwarzork Oberboss', points = 0.0 WHERE id =11438;</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23">
+        <v>9</v>
+      </c>
+      <c r="B23" t="s">
+        <v>330</v>
+      </c>
+      <c r="C23">
+        <v>11439</v>
+      </c>
+      <c r="D23" t="s">
+        <v>357</v>
+      </c>
+      <c r="E23">
+        <v>46424</v>
+      </c>
+      <c r="F23" t="s">
+        <v>357</v>
+      </c>
+      <c r="G23">
+        <v>11439</v>
+      </c>
+      <c r="H23" t="s">
+        <v>453</v>
+      </c>
+      <c r="I23" t="s">
+        <v>1</v>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Ork Oberboss', points = 0.0 WHERE id =11439;</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24">
+        <v>9</v>
+      </c>
+      <c r="B24" t="s">
+        <v>330</v>
+      </c>
+      <c r="C24">
+        <v>11440</v>
+      </c>
+      <c r="D24" t="s">
+        <v>358</v>
+      </c>
+      <c r="E24">
+        <v>46425</v>
+      </c>
+      <c r="F24" t="s">
+        <v>358</v>
+      </c>
+      <c r="G24">
+        <v>11440</v>
+      </c>
+      <c r="H24" t="s">
+        <v>454</v>
+      </c>
+      <c r="I24" t="s">
+        <v>1</v>
+      </c>
+      <c r="J24" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Wildork Oberboss', points = 0.0 WHERE id =11440;</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25">
+        <v>9</v>
+      </c>
+      <c r="B25" t="s">
+        <v>330</v>
+      </c>
+      <c r="C25">
+        <v>11441</v>
+      </c>
+      <c r="D25" t="s">
+        <v>359</v>
+      </c>
+      <c r="E25">
+        <v>46426</v>
+      </c>
+      <c r="F25" t="s">
+        <v>359</v>
+      </c>
+      <c r="G25">
+        <v>11441</v>
+      </c>
+      <c r="H25" t="s">
+        <v>455</v>
+      </c>
+      <c r="I25" t="s">
+        <v>1</v>
+      </c>
+      <c r="J25" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Goblin Oberboss', points = 0.0 WHERE id =11441;</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26">
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>330</v>
+      </c>
+      <c r="C26">
+        <v>11442</v>
+      </c>
+      <c r="D26" t="s">
+        <v>360</v>
+      </c>
+      <c r="E26">
+        <v>46427</v>
+      </c>
+      <c r="F26" t="s">
+        <v>360</v>
+      </c>
+      <c r="G26">
+        <v>11442</v>
+      </c>
+      <c r="H26" t="s">
+        <v>456</v>
+      </c>
+      <c r="I26" t="s">
+        <v>1</v>
+      </c>
+      <c r="J26" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Waldgoblin Oberboss', points = 0.0 WHERE id =11442;</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27">
+        <v>9</v>
+      </c>
+      <c r="B27" t="s">
+        <v>330</v>
+      </c>
+      <c r="C27">
+        <v>11443</v>
+      </c>
+      <c r="D27" t="s">
+        <v>361</v>
+      </c>
+      <c r="E27">
+        <v>46428</v>
+      </c>
+      <c r="F27" t="s">
+        <v>361</v>
+      </c>
+      <c r="G27">
+        <v>11443</v>
+      </c>
+      <c r="H27" t="s">
+        <v>457</v>
+      </c>
+      <c r="I27" t="s">
+        <v>1</v>
+      </c>
+      <c r="J27" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Nachtgoblin Oberboss', points = 0.0 WHERE id =11443;</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28">
+        <v>9</v>
+      </c>
+      <c r="B28" t="s">
+        <v>330</v>
+      </c>
+      <c r="C28">
+        <v>11444</v>
+      </c>
+      <c r="D28" t="s">
+        <v>362</v>
+      </c>
+      <c r="E28">
+        <v>46429</v>
+      </c>
+      <c r="F28" t="s">
+        <v>362</v>
+      </c>
+      <c r="G28">
+        <v>11444</v>
+      </c>
+      <c r="H28" t="s">
+        <v>458</v>
+      </c>
+      <c r="I28" t="s">
+        <v>1</v>
+      </c>
+      <c r="J28" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Schwarzork Boss', points = 0.0 WHERE id =11444;</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29">
+        <v>9</v>
+      </c>
+      <c r="B29" t="s">
+        <v>330</v>
+      </c>
+      <c r="C29">
+        <v>11445</v>
+      </c>
+      <c r="D29" t="s">
+        <v>363</v>
+      </c>
+      <c r="E29">
+        <v>46430</v>
+      </c>
+      <c r="F29" t="s">
+        <v>363</v>
+      </c>
+      <c r="G29">
+        <v>11445</v>
+      </c>
+      <c r="H29" t="s">
+        <v>459</v>
+      </c>
+      <c r="I29" t="s">
+        <v>1</v>
+      </c>
+      <c r="J29" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Ork Boss', points = 0.0 WHERE id =11445;</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30">
+        <v>9</v>
+      </c>
+      <c r="B30" t="s">
+        <v>330</v>
+      </c>
+      <c r="C30">
+        <v>11446</v>
+      </c>
+      <c r="D30" t="s">
+        <v>364</v>
+      </c>
+      <c r="E30">
+        <v>46431</v>
+      </c>
+      <c r="F30" t="s">
+        <v>364</v>
+      </c>
+      <c r="G30">
+        <v>11446</v>
+      </c>
+      <c r="H30" t="s">
+        <v>460</v>
+      </c>
+      <c r="I30" t="s">
+        <v>1</v>
+      </c>
+      <c r="J30" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Wildork Boss', points = 0.0 WHERE id =11446;</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31">
+        <v>9</v>
+      </c>
+      <c r="B31" t="s">
+        <v>330</v>
+      </c>
+      <c r="C31">
+        <v>11447</v>
+      </c>
+      <c r="D31" t="s">
+        <v>365</v>
+      </c>
+      <c r="E31">
+        <v>46432</v>
+      </c>
+      <c r="F31" t="s">
+        <v>365</v>
+      </c>
+      <c r="G31">
+        <v>11447</v>
+      </c>
+      <c r="H31" t="s">
+        <v>461</v>
+      </c>
+      <c r="I31" t="s">
+        <v>1</v>
+      </c>
+      <c r="J31" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Goblin Boss', points = 0.0 WHERE id =11447;</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32">
+        <v>9</v>
+      </c>
+      <c r="B32" t="s">
+        <v>330</v>
+      </c>
+      <c r="C32">
+        <v>11448</v>
+      </c>
+      <c r="D32" t="s">
+        <v>366</v>
+      </c>
+      <c r="E32">
+        <v>46433</v>
+      </c>
+      <c r="F32" t="s">
+        <v>366</v>
+      </c>
+      <c r="G32">
+        <v>11448</v>
+      </c>
+      <c r="H32" t="s">
+        <v>462</v>
+      </c>
+      <c r="I32" t="s">
+        <v>1</v>
+      </c>
+      <c r="J32" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Waldgoblin Boss', points = 0.0 WHERE id =11448;</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33">
+        <v>9</v>
+      </c>
+      <c r="B33" t="s">
+        <v>330</v>
+      </c>
+      <c r="C33">
+        <v>11449</v>
+      </c>
+      <c r="D33" t="s">
+        <v>367</v>
+      </c>
+      <c r="E33">
+        <v>46434</v>
+      </c>
+      <c r="F33" t="s">
+        <v>367</v>
+      </c>
+      <c r="G33">
+        <v>11449</v>
+      </c>
+      <c r="H33" t="s">
+        <v>463</v>
+      </c>
+      <c r="I33" t="s">
+        <v>1</v>
+      </c>
+      <c r="J33" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Nachtgoblin Boss', points = 0.0 WHERE id =11449;</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34">
+        <v>9</v>
+      </c>
+      <c r="B34" t="s">
+        <v>330</v>
+      </c>
+      <c r="C34">
+        <v>11450</v>
+      </c>
+      <c r="D34" t="s">
+        <v>368</v>
+      </c>
+      <c r="E34">
+        <v>46435</v>
+      </c>
+      <c r="F34" t="s">
+        <v>368</v>
+      </c>
+      <c r="G34">
+        <v>11450</v>
+      </c>
+      <c r="H34" t="s">
+        <v>464</v>
+      </c>
+      <c r="I34" t="s">
+        <v>1</v>
+      </c>
+      <c r="J34" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Ork Schamane', points = 0.0 WHERE id =11450;</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35">
+        <v>9</v>
+      </c>
+      <c r="B35" t="s">
+        <v>330</v>
+      </c>
+      <c r="C35">
+        <v>11451</v>
+      </c>
+      <c r="D35" t="s">
+        <v>369</v>
+      </c>
+      <c r="E35">
+        <v>46436</v>
+      </c>
+      <c r="F35" t="s">
+        <v>369</v>
+      </c>
+      <c r="G35">
+        <v>11451</v>
+      </c>
+      <c r="H35" t="s">
+        <v>465</v>
+      </c>
+      <c r="I35" t="s">
+        <v>1</v>
+      </c>
+      <c r="J35" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Wildork Schamane', points = 0.0 WHERE id =11451;</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36">
+        <v>9</v>
+      </c>
+      <c r="B36" t="s">
+        <v>330</v>
+      </c>
+      <c r="C36">
+        <v>11452</v>
+      </c>
+      <c r="D36" t="s">
+        <v>370</v>
+      </c>
+      <c r="E36">
+        <v>46437</v>
+      </c>
+      <c r="F36" t="s">
+        <v>370</v>
+      </c>
+      <c r="G36">
+        <v>11452</v>
+      </c>
+      <c r="H36" t="s">
+        <v>466</v>
+      </c>
+      <c r="I36" t="s">
+        <v>1</v>
+      </c>
+      <c r="J36" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Goblin Schamane', points = 0.0 WHERE id =11452;</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37">
+        <v>9</v>
+      </c>
+      <c r="B37" t="s">
+        <v>330</v>
+      </c>
+      <c r="C37">
+        <v>11453</v>
+      </c>
+      <c r="D37" t="s">
+        <v>371</v>
+      </c>
+      <c r="E37">
+        <v>46438</v>
+      </c>
+      <c r="F37" t="s">
+        <v>371</v>
+      </c>
+      <c r="G37">
+        <v>11453</v>
+      </c>
+      <c r="H37" t="s">
+        <v>467</v>
+      </c>
+      <c r="I37" t="s">
+        <v>1</v>
+      </c>
+      <c r="J37" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Nachtgoblin Schamane', points = 0.0 WHERE id =11453;</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38">
+        <v>9</v>
+      </c>
+      <c r="B38" t="s">
+        <v>330</v>
+      </c>
+      <c r="C38">
+        <v>11454</v>
+      </c>
+      <c r="D38" t="s">
+        <v>372</v>
+      </c>
+      <c r="E38">
+        <v>46439</v>
+      </c>
+      <c r="F38" t="s">
+        <v>372</v>
+      </c>
+      <c r="G38">
+        <v>11454</v>
+      </c>
+      <c r="H38" t="s">
+        <v>468</v>
+      </c>
+      <c r="I38" t="s">
+        <v>1</v>
+      </c>
+      <c r="J38" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Waldgoblin Schamane', points = 0.0 WHERE id =11454;</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39">
+        <v>9</v>
+      </c>
+      <c r="B39" t="s">
+        <v>330</v>
+      </c>
+      <c r="C39">
+        <v>11455</v>
+      </c>
+      <c r="D39" t="s">
+        <v>373</v>
+      </c>
+      <c r="E39">
+        <v>46440</v>
+      </c>
+      <c r="F39" t="s">
+        <v>373</v>
+      </c>
+      <c r="G39">
+        <v>11455</v>
+      </c>
+      <c r="H39" t="s">
+        <v>469</v>
+      </c>
+      <c r="I39" t="s">
+        <v>1</v>
+      </c>
+      <c r="J39" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Ork Oberschamane', points = 0.0 WHERE id =11455;</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40">
+        <v>9</v>
+      </c>
+      <c r="B40" t="s">
+        <v>330</v>
+      </c>
+      <c r="C40">
+        <v>11456</v>
+      </c>
+      <c r="D40" t="s">
+        <v>374</v>
+      </c>
+      <c r="E40">
+        <v>46441</v>
+      </c>
+      <c r="F40" t="s">
+        <v>374</v>
+      </c>
+      <c r="G40">
+        <v>11456</v>
+      </c>
+      <c r="H40" t="s">
+        <v>470</v>
+      </c>
+      <c r="I40" t="s">
+        <v>1</v>
+      </c>
+      <c r="J40" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Wildork Oberschamane', points = 0.0 WHERE id =11456;</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41">
+        <v>9</v>
+      </c>
+      <c r="B41" t="s">
+        <v>330</v>
+      </c>
+      <c r="C41">
+        <v>11457</v>
+      </c>
+      <c r="D41" t="s">
+        <v>375</v>
+      </c>
+      <c r="E41">
+        <v>46442</v>
+      </c>
+      <c r="F41" t="s">
+        <v>375</v>
+      </c>
+      <c r="G41">
+        <v>11457</v>
+      </c>
+      <c r="H41" t="s">
+        <v>474</v>
+      </c>
+      <c r="I41" t="s">
+        <v>1</v>
+      </c>
+      <c r="J41" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Goblin Oberschamane', points = 0.0 WHERE id =11457;</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42">
+        <v>9</v>
+      </c>
+      <c r="B42" t="s">
+        <v>330</v>
+      </c>
+      <c r="C42">
+        <v>11458</v>
+      </c>
+      <c r="D42" t="s">
+        <v>376</v>
+      </c>
+      <c r="E42">
+        <v>46443</v>
+      </c>
+      <c r="F42" t="s">
+        <v>376</v>
+      </c>
+      <c r="G42">
+        <v>11458</v>
+      </c>
+      <c r="H42" t="s">
+        <v>475</v>
+      </c>
+      <c r="I42" t="s">
+        <v>1</v>
+      </c>
+      <c r="J42" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Nachtgoblin Oberschamane', points = 0.0 WHERE id =11458;</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43">
+        <v>9</v>
+      </c>
+      <c r="B43" t="s">
+        <v>330</v>
+      </c>
+      <c r="C43">
+        <v>11459</v>
+      </c>
+      <c r="D43" t="s">
+        <v>377</v>
+      </c>
+      <c r="E43">
+        <v>46444</v>
+      </c>
+      <c r="F43" t="s">
+        <v>377</v>
+      </c>
+      <c r="G43">
+        <v>11459</v>
+      </c>
+      <c r="H43" t="s">
+        <v>476</v>
+      </c>
+      <c r="I43" t="s">
+        <v>1</v>
+      </c>
+      <c r="J43" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Waldgoblin Oberschamane', points = 0.0 WHERE id =11459;</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44">
+        <v>9</v>
+      </c>
+      <c r="B44" t="s">
+        <v>330</v>
+      </c>
+      <c r="C44">
+        <v>11460</v>
+      </c>
+      <c r="D44" t="s">
+        <v>378</v>
+      </c>
+      <c r="E44">
+        <v>46445</v>
+      </c>
+      <c r="F44" t="s">
+        <v>378</v>
+      </c>
+      <c r="G44">
+        <v>11460</v>
+      </c>
+      <c r="H44" t="s">
+        <v>477</v>
+      </c>
+      <c r="I44" t="s">
+        <v>1</v>
+      </c>
+      <c r="J44" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Ork Großschamane', points = 0.0 WHERE id =11460;</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45">
+        <v>9</v>
+      </c>
+      <c r="B45" t="s">
+        <v>330</v>
+      </c>
+      <c r="C45">
+        <v>11461</v>
+      </c>
+      <c r="D45" t="s">
+        <v>379</v>
+      </c>
+      <c r="E45">
+        <v>46446</v>
+      </c>
+      <c r="F45" t="s">
+        <v>379</v>
+      </c>
+      <c r="G45">
+        <v>11461</v>
+      </c>
+      <c r="H45" t="s">
+        <v>478</v>
+      </c>
+      <c r="I45" t="s">
+        <v>1</v>
+      </c>
+      <c r="J45" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Wildork Großschamane', points = 0.0 WHERE id =11461;</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46">
+        <v>9</v>
+      </c>
+      <c r="B46" t="s">
+        <v>330</v>
+      </c>
+      <c r="C46">
+        <v>11462</v>
+      </c>
+      <c r="D46" t="s">
+        <v>380</v>
+      </c>
+      <c r="E46">
+        <v>46447</v>
+      </c>
+      <c r="F46" t="s">
+        <v>380</v>
+      </c>
+      <c r="G46">
+        <v>11462</v>
+      </c>
+      <c r="H46" t="s">
+        <v>479</v>
+      </c>
+      <c r="I46" t="s">
+        <v>1</v>
+      </c>
+      <c r="J46" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Goblin Großschamane', points = 0.0 WHERE id =11462;</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47">
+        <v>9</v>
+      </c>
+      <c r="B47" t="s">
+        <v>330</v>
+      </c>
+      <c r="C47">
+        <v>11463</v>
+      </c>
+      <c r="D47" t="s">
+        <v>381</v>
+      </c>
+      <c r="E47">
+        <v>46448</v>
+      </c>
+      <c r="F47" t="s">
+        <v>381</v>
+      </c>
+      <c r="G47">
+        <v>11463</v>
+      </c>
+      <c r="H47" t="s">
+        <v>480</v>
+      </c>
+      <c r="I47" t="s">
+        <v>1</v>
+      </c>
+      <c r="J47" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Nachtgoblin Großschamane', points = 0.0 WHERE id =11463;</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48">
+        <v>9</v>
+      </c>
+      <c r="B48" t="s">
+        <v>330</v>
+      </c>
+      <c r="C48">
+        <v>11464</v>
+      </c>
+      <c r="D48" t="s">
+        <v>382</v>
+      </c>
+      <c r="E48">
+        <v>46449</v>
+      </c>
+      <c r="F48" t="s">
+        <v>382</v>
+      </c>
+      <c r="G48">
+        <v>11464</v>
+      </c>
+      <c r="H48" t="s">
+        <v>481</v>
+      </c>
+      <c r="I48" t="s">
+        <v>1</v>
+      </c>
+      <c r="J48" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Waldgoblin Großschamane', points = 0.0 WHERE id =11464;</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49">
+        <v>9</v>
+      </c>
+      <c r="B49" t="s">
+        <v>330</v>
+      </c>
+      <c r="C49">
+        <v>11465</v>
+      </c>
+      <c r="D49" t="s">
+        <v>383</v>
+      </c>
+      <c r="E49">
+        <v>46450</v>
+      </c>
+      <c r="F49" t="s">
+        <v>383</v>
+      </c>
+      <c r="G49">
+        <v>11465</v>
+      </c>
+      <c r="H49" t="s">
+        <v>482</v>
+      </c>
+      <c r="I49" t="s">
+        <v>1</v>
+      </c>
+      <c r="J49" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Ork Meisterschamane', points = 0.0 WHERE id =11465;</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50">
+        <v>9</v>
+      </c>
+      <c r="B50" t="s">
+        <v>330</v>
+      </c>
+      <c r="C50">
+        <v>11466</v>
+      </c>
+      <c r="D50" t="s">
+        <v>384</v>
+      </c>
+      <c r="E50">
+        <v>46451</v>
+      </c>
+      <c r="F50" t="s">
+        <v>384</v>
+      </c>
+      <c r="G50">
+        <v>11466</v>
+      </c>
+      <c r="H50" t="s">
+        <v>483</v>
+      </c>
+      <c r="I50" t="s">
+        <v>1</v>
+      </c>
+      <c r="J50" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Wildork Meisterschamane', points = 0.0 WHERE id =11466;</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51">
+        <v>9</v>
+      </c>
+      <c r="B51" t="s">
+        <v>330</v>
+      </c>
+      <c r="C51">
+        <v>11467</v>
+      </c>
+      <c r="D51" t="s">
+        <v>385</v>
+      </c>
+      <c r="E51">
+        <v>46452</v>
+      </c>
+      <c r="F51" t="s">
+        <v>385</v>
+      </c>
+      <c r="G51">
+        <v>11467</v>
+      </c>
+      <c r="H51" t="s">
+        <v>484</v>
+      </c>
+      <c r="I51" t="s">
+        <v>1</v>
+      </c>
+      <c r="J51" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Goblin Meisterschamane', points = 0.0 WHERE id =11467;</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52">
+        <v>9</v>
+      </c>
+      <c r="B52" t="s">
+        <v>330</v>
+      </c>
+      <c r="C52">
+        <v>11468</v>
+      </c>
+      <c r="D52" t="s">
+        <v>386</v>
+      </c>
+      <c r="E52">
+        <v>46453</v>
+      </c>
+      <c r="F52" t="s">
+        <v>386</v>
+      </c>
+      <c r="G52">
+        <v>11468</v>
+      </c>
+      <c r="H52" t="s">
+        <v>485</v>
+      </c>
+      <c r="I52" t="s">
+        <v>1</v>
+      </c>
+      <c r="J52" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Nachtgoblin Meisterschamane', points = 0.0 WHERE id =11468;</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53">
+        <v>9</v>
+      </c>
+      <c r="B53" t="s">
+        <v>330</v>
+      </c>
+      <c r="C53">
+        <v>11469</v>
+      </c>
+      <c r="D53" t="s">
+        <v>387</v>
+      </c>
+      <c r="E53">
+        <v>46454</v>
+      </c>
+      <c r="F53" t="s">
+        <v>387</v>
+      </c>
+      <c r="G53">
+        <v>11469</v>
+      </c>
+      <c r="H53" t="s">
+        <v>486</v>
+      </c>
+      <c r="I53" t="s">
+        <v>1</v>
+      </c>
+      <c r="J53" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Orks Waldgoblin Meisterschamane', points = 0.0 WHERE id =11469;</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54">
+        <v>9</v>
+      </c>
+      <c r="B54" t="s">
+        <v>330</v>
+      </c>
+      <c r="C54">
+        <v>11586</v>
+      </c>
+      <c r="D54" t="s">
+        <v>388</v>
+      </c>
+      <c r="E54">
+        <v>46571</v>
+      </c>
+      <c r="F54" t="s">
+        <v>388</v>
+      </c>
+      <c r="G54">
+        <v>11586</v>
+      </c>
+      <c r="I54" t="s">
+        <v>1</v>
+      </c>
+      <c r="J54" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11586;</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55">
+        <v>9</v>
+      </c>
+      <c r="B55" t="s">
+        <v>330</v>
+      </c>
+      <c r="C55">
+        <v>11643</v>
+      </c>
+      <c r="D55" t="s">
+        <v>389</v>
+      </c>
+      <c r="E55">
+        <v>46628</v>
+      </c>
+      <c r="F55" t="s">
+        <v>389</v>
+      </c>
+      <c r="G55">
+        <v>11643</v>
+      </c>
+      <c r="I55" t="s">
+        <v>1</v>
+      </c>
+      <c r="J55" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11643;</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" s="2" customFormat="1">
+      <c r="A56" s="2">
+        <v>9</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C56" s="2">
+        <v>11643</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="E56" s="2">
+        <v>46854</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="G56" s="2">
+        <v>12423</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="J56" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = 'Lindwurm', points = 180.0 WHERE id =12423;</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57">
+        <v>9</v>
+      </c>
+      <c r="B57" t="s">
+        <v>330</v>
+      </c>
+      <c r="C57">
+        <v>11850</v>
+      </c>
+      <c r="D57" t="s">
+        <v>390</v>
+      </c>
+      <c r="E57">
+        <v>46760</v>
+      </c>
+      <c r="F57" t="s">
+        <v>391</v>
+      </c>
+      <c r="G57">
+        <v>11850</v>
+      </c>
+      <c r="I57" t="s">
+        <v>1</v>
+      </c>
+      <c r="J57" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11850;</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58">
+        <v>9</v>
+      </c>
+      <c r="B58" t="s">
+        <v>330</v>
+      </c>
+      <c r="C58">
+        <v>11850</v>
+      </c>
+      <c r="D58" t="s">
+        <v>390</v>
+      </c>
+      <c r="E58">
+        <v>46989</v>
+      </c>
+      <c r="F58" t="s">
+        <v>392</v>
+      </c>
+      <c r="G58">
+        <v>12023</v>
+      </c>
+      <c r="I58" t="s">
+        <v>1</v>
+      </c>
+      <c r="J58" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12023;</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59">
+        <v>9</v>
+      </c>
+      <c r="B59" t="s">
+        <v>330</v>
+      </c>
+      <c r="C59">
+        <v>11851</v>
+      </c>
+      <c r="D59" t="s">
+        <v>393</v>
+      </c>
+      <c r="E59">
+        <v>46761</v>
+      </c>
+      <c r="F59" t="s">
+        <v>394</v>
+      </c>
+      <c r="G59">
+        <v>11851</v>
+      </c>
+      <c r="I59" t="s">
+        <v>1</v>
+      </c>
+      <c r="J59" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11851;</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60">
+        <v>9</v>
+      </c>
+      <c r="B60" t="s">
+        <v>330</v>
+      </c>
+      <c r="C60">
+        <v>11851</v>
+      </c>
+      <c r="D60" t="s">
+        <v>393</v>
+      </c>
+      <c r="E60">
+        <v>46990</v>
+      </c>
+      <c r="F60" t="s">
+        <v>392</v>
+      </c>
+      <c r="G60">
+        <v>12023</v>
+      </c>
+      <c r="I60" t="s">
+        <v>1</v>
+      </c>
+      <c r="J60" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12023;</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61">
+        <v>9</v>
+      </c>
+      <c r="B61" t="s">
+        <v>330</v>
+      </c>
+      <c r="C61">
+        <v>11852</v>
+      </c>
+      <c r="D61" t="s">
+        <v>395</v>
+      </c>
+      <c r="E61">
+        <v>46991</v>
+      </c>
+      <c r="F61" t="s">
+        <v>334</v>
+      </c>
+      <c r="G61">
+        <v>11841</v>
+      </c>
+      <c r="I61" t="s">
+        <v>1</v>
+      </c>
+      <c r="J61" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11841;</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="A62">
+        <v>9</v>
+      </c>
+      <c r="B62" t="s">
+        <v>330</v>
+      </c>
+      <c r="C62">
+        <v>11852</v>
+      </c>
+      <c r="D62" t="s">
+        <v>395</v>
+      </c>
+      <c r="E62">
+        <v>46762</v>
+      </c>
+      <c r="F62" t="s">
+        <v>396</v>
+      </c>
+      <c r="G62">
+        <v>11852</v>
+      </c>
+      <c r="I62" t="s">
+        <v>1</v>
+      </c>
+      <c r="J62" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11852;</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63">
+        <v>9</v>
+      </c>
+      <c r="B63" t="s">
+        <v>330</v>
+      </c>
+      <c r="C63">
+        <v>11853</v>
+      </c>
+      <c r="D63" t="s">
+        <v>397</v>
+      </c>
+      <c r="E63">
+        <v>46763</v>
+      </c>
+      <c r="F63" t="s">
+        <v>398</v>
+      </c>
+      <c r="G63">
+        <v>11853</v>
+      </c>
+      <c r="I63" t="s">
+        <v>1</v>
+      </c>
+      <c r="J63" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11853;</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64">
+        <v>9</v>
+      </c>
+      <c r="B64" t="s">
+        <v>330</v>
+      </c>
+      <c r="C64">
+        <v>11853</v>
+      </c>
+      <c r="D64" t="s">
+        <v>397</v>
+      </c>
+      <c r="E64">
+        <v>46992</v>
+      </c>
+      <c r="F64" t="s">
+        <v>399</v>
+      </c>
+      <c r="G64">
+        <v>12026</v>
+      </c>
+      <c r="I64" t="s">
+        <v>1</v>
+      </c>
+      <c r="J64" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12026;</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="A65">
+        <v>9</v>
+      </c>
+      <c r="B65" t="s">
+        <v>330</v>
+      </c>
+      <c r="C65">
+        <v>11854</v>
+      </c>
+      <c r="D65" t="s">
+        <v>400</v>
+      </c>
+      <c r="E65">
+        <v>46764</v>
+      </c>
+      <c r="F65" t="s">
+        <v>401</v>
+      </c>
+      <c r="G65">
+        <v>11854</v>
+      </c>
+      <c r="I65" t="s">
+        <v>1</v>
+      </c>
+      <c r="J65" t="str">
+        <f t="shared" si="0"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11854;</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66">
+        <v>9</v>
+      </c>
+      <c r="B66" t="s">
+        <v>330</v>
+      </c>
+      <c r="C66">
+        <v>11855</v>
+      </c>
+      <c r="D66" t="s">
+        <v>402</v>
+      </c>
+      <c r="E66">
+        <v>46765</v>
+      </c>
+      <c r="F66" t="s">
+        <v>394</v>
+      </c>
+      <c r="G66">
+        <v>11855</v>
+      </c>
+      <c r="I66" t="s">
+        <v>1</v>
+      </c>
+      <c r="J66" t="str">
+        <f t="shared" ref="J66:J99" si="1">CONCATENATE("UPDATE profile SET name = '",H66,"', points = ",I66," WHERE id =",G66,";")</f>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11855;</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67">
+        <v>9</v>
+      </c>
+      <c r="B67" t="s">
+        <v>330</v>
+      </c>
+      <c r="C67">
+        <v>11856</v>
+      </c>
+      <c r="D67" t="s">
+        <v>403</v>
+      </c>
+      <c r="E67">
+        <v>46766</v>
+      </c>
+      <c r="F67" t="s">
+        <v>404</v>
+      </c>
+      <c r="G67">
+        <v>11856</v>
+      </c>
+      <c r="I67" t="s">
+        <v>1</v>
+      </c>
+      <c r="J67" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11856;</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68">
+        <v>9</v>
+      </c>
+      <c r="B68" t="s">
+        <v>330</v>
+      </c>
+      <c r="C68">
+        <v>11857</v>
+      </c>
+      <c r="D68" t="s">
+        <v>405</v>
+      </c>
+      <c r="E68">
+        <v>46767</v>
+      </c>
+      <c r="F68" t="s">
+        <v>406</v>
+      </c>
+      <c r="G68">
+        <v>11857</v>
+      </c>
+      <c r="I68" t="s">
+        <v>1</v>
+      </c>
+      <c r="J68" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11857;</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69">
+        <v>9</v>
+      </c>
+      <c r="B69" t="s">
+        <v>330</v>
+      </c>
+      <c r="C69">
+        <v>11858</v>
+      </c>
+      <c r="D69" t="s">
+        <v>407</v>
+      </c>
+      <c r="E69">
+        <v>46768</v>
+      </c>
+      <c r="F69" t="s">
+        <v>391</v>
+      </c>
+      <c r="G69">
+        <v>11858</v>
+      </c>
+      <c r="I69" t="s">
+        <v>1</v>
+      </c>
+      <c r="J69" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11858;</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70">
+        <v>9</v>
+      </c>
+      <c r="B70" t="s">
+        <v>330</v>
+      </c>
+      <c r="C70">
+        <v>11859</v>
+      </c>
+      <c r="D70" t="s">
+        <v>408</v>
+      </c>
+      <c r="E70">
+        <v>46769</v>
+      </c>
+      <c r="F70" t="s">
+        <v>396</v>
+      </c>
+      <c r="G70">
+        <v>11852</v>
+      </c>
+      <c r="I70" t="s">
+        <v>1</v>
+      </c>
+      <c r="J70" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11852;</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71">
+        <v>9</v>
+      </c>
+      <c r="B71" t="s">
+        <v>330</v>
+      </c>
+      <c r="C71">
+        <v>11860</v>
+      </c>
+      <c r="D71" t="s">
+        <v>409</v>
+      </c>
+      <c r="E71">
+        <v>46770</v>
+      </c>
+      <c r="F71" t="s">
+        <v>398</v>
+      </c>
+      <c r="G71">
+        <v>11853</v>
+      </c>
+      <c r="I71" t="s">
+        <v>1</v>
+      </c>
+      <c r="J71" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11853;</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72">
+        <v>9</v>
+      </c>
+      <c r="B72" t="s">
+        <v>330</v>
+      </c>
+      <c r="C72">
+        <v>11861</v>
+      </c>
+      <c r="D72" t="s">
+        <v>410</v>
+      </c>
+      <c r="E72">
+        <v>46771</v>
+      </c>
+      <c r="F72" t="s">
+        <v>411</v>
+      </c>
+      <c r="G72">
+        <v>11861</v>
+      </c>
+      <c r="I72" t="s">
+        <v>1</v>
+      </c>
+      <c r="J72" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11861;</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73">
+        <v>9</v>
+      </c>
+      <c r="B73" t="s">
+        <v>330</v>
+      </c>
+      <c r="C73">
+        <v>11862</v>
+      </c>
+      <c r="D73" t="s">
+        <v>412</v>
+      </c>
+      <c r="E73">
+        <v>46772</v>
+      </c>
+      <c r="F73" t="s">
+        <v>411</v>
+      </c>
+      <c r="G73">
+        <v>11862</v>
+      </c>
+      <c r="I73" t="s">
+        <v>1</v>
+      </c>
+      <c r="J73" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11862;</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="A74">
+        <v>9</v>
+      </c>
+      <c r="B74" t="s">
+        <v>330</v>
+      </c>
+      <c r="C74">
+        <v>11862</v>
+      </c>
+      <c r="D74" t="s">
+        <v>412</v>
+      </c>
+      <c r="E74">
+        <v>46993</v>
+      </c>
+      <c r="F74" t="s">
+        <v>413</v>
+      </c>
+      <c r="G74">
+        <v>12027</v>
+      </c>
+      <c r="I74" t="s">
+        <v>1</v>
+      </c>
+      <c r="J74" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12027;</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="A75">
+        <v>9</v>
+      </c>
+      <c r="B75" t="s">
+        <v>330</v>
+      </c>
+      <c r="C75">
+        <v>11863</v>
+      </c>
+      <c r="D75" t="s">
+        <v>414</v>
+      </c>
+      <c r="E75">
+        <v>46773</v>
+      </c>
+      <c r="F75" t="s">
+        <v>414</v>
+      </c>
+      <c r="G75">
+        <v>11863</v>
+      </c>
+      <c r="I75" t="s">
+        <v>1</v>
+      </c>
+      <c r="J75" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11863;</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="A76">
+        <v>9</v>
+      </c>
+      <c r="B76" t="s">
+        <v>330</v>
+      </c>
+      <c r="C76">
+        <v>11864</v>
+      </c>
+      <c r="D76" t="s">
+        <v>415</v>
+      </c>
+      <c r="E76">
+        <v>46774</v>
+      </c>
+      <c r="F76" t="s">
+        <v>416</v>
+      </c>
+      <c r="G76">
+        <v>11864</v>
+      </c>
+      <c r="I76" t="s">
+        <v>1</v>
+      </c>
+      <c r="J76" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11864;</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77">
+        <v>9</v>
+      </c>
+      <c r="B77" t="s">
+        <v>330</v>
+      </c>
+      <c r="C77">
+        <v>11865</v>
+      </c>
+      <c r="D77" t="s">
+        <v>417</v>
+      </c>
+      <c r="E77">
+        <v>46775</v>
+      </c>
+      <c r="F77" t="s">
+        <v>411</v>
+      </c>
+      <c r="G77">
+        <v>11861</v>
+      </c>
+      <c r="I77" t="s">
+        <v>1</v>
+      </c>
+      <c r="J77" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11861;</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="A78">
+        <v>9</v>
+      </c>
+      <c r="B78" t="s">
+        <v>330</v>
+      </c>
+      <c r="C78">
+        <v>11865</v>
+      </c>
+      <c r="D78" t="s">
+        <v>417</v>
+      </c>
+      <c r="E78">
+        <v>46994</v>
+      </c>
+      <c r="F78" t="s">
+        <v>413</v>
+      </c>
+      <c r="G78">
+        <v>12028</v>
+      </c>
+      <c r="I78" t="s">
+        <v>1</v>
+      </c>
+      <c r="J78" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12028;</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79">
+        <v>9</v>
+      </c>
+      <c r="B79" t="s">
+        <v>330</v>
+      </c>
+      <c r="C79">
+        <v>11866</v>
+      </c>
+      <c r="D79" t="s">
+        <v>418</v>
+      </c>
+      <c r="E79">
+        <v>46776</v>
+      </c>
+      <c r="F79" t="s">
+        <v>418</v>
+      </c>
+      <c r="G79">
+        <v>11866</v>
+      </c>
+      <c r="I79" t="s">
+        <v>1</v>
+      </c>
+      <c r="J79" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11866;</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80">
+        <v>9</v>
+      </c>
+      <c r="B80" t="s">
+        <v>330</v>
+      </c>
+      <c r="C80">
+        <v>11867</v>
+      </c>
+      <c r="D80" t="s">
+        <v>419</v>
+      </c>
+      <c r="E80">
+        <v>46777</v>
+      </c>
+      <c r="F80" t="s">
+        <v>419</v>
+      </c>
+      <c r="G80">
+        <v>11867</v>
+      </c>
+      <c r="I80" t="s">
+        <v>1</v>
+      </c>
+      <c r="J80" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11867;</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
+      <c r="A81">
+        <v>9</v>
+      </c>
+      <c r="B81" t="s">
+        <v>330</v>
+      </c>
+      <c r="C81">
+        <v>11868</v>
+      </c>
+      <c r="D81" t="s">
+        <v>420</v>
+      </c>
+      <c r="E81">
+        <v>46778</v>
+      </c>
+      <c r="F81" t="s">
+        <v>421</v>
+      </c>
+      <c r="G81">
+        <v>11868</v>
+      </c>
+      <c r="I81" t="s">
+        <v>1</v>
+      </c>
+      <c r="J81" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11868;</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="A82">
+        <v>9</v>
+      </c>
+      <c r="B82" t="s">
+        <v>330</v>
+      </c>
+      <c r="C82">
+        <v>11869</v>
+      </c>
+      <c r="D82" t="s">
+        <v>422</v>
+      </c>
+      <c r="E82">
+        <v>46779</v>
+      </c>
+      <c r="F82" t="s">
+        <v>423</v>
+      </c>
+      <c r="G82">
+        <v>11869</v>
+      </c>
+      <c r="I82" t="s">
+        <v>1</v>
+      </c>
+      <c r="J82" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11869;</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
+      <c r="A83">
+        <v>9</v>
+      </c>
+      <c r="B83" t="s">
+        <v>330</v>
+      </c>
+      <c r="C83">
+        <v>11870</v>
+      </c>
+      <c r="D83" t="s">
+        <v>424</v>
+      </c>
+      <c r="E83">
+        <v>46780</v>
+      </c>
+      <c r="F83" t="s">
+        <v>425</v>
+      </c>
+      <c r="G83">
+        <v>11870</v>
+      </c>
+      <c r="I83" t="s">
+        <v>1</v>
+      </c>
+      <c r="J83" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11870;</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
+      <c r="A84">
+        <v>9</v>
+      </c>
+      <c r="B84" t="s">
+        <v>330</v>
+      </c>
+      <c r="C84">
+        <v>12071</v>
+      </c>
+      <c r="D84" t="s">
+        <v>426</v>
+      </c>
+      <c r="E84">
+        <v>47047</v>
+      </c>
+      <c r="F84" t="s">
+        <v>427</v>
+      </c>
+      <c r="G84">
+        <v>12071</v>
+      </c>
+      <c r="I84" t="s">
+        <v>1</v>
+      </c>
+      <c r="J84" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12071;</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
+      <c r="A85">
+        <v>9</v>
+      </c>
+      <c r="B85" t="s">
+        <v>330</v>
+      </c>
+      <c r="C85">
+        <v>12071</v>
+      </c>
+      <c r="D85" t="s">
+        <v>426</v>
+      </c>
+      <c r="E85">
+        <v>47070</v>
+      </c>
+      <c r="F85" t="s">
+        <v>426</v>
+      </c>
+      <c r="G85">
+        <v>12119</v>
+      </c>
+      <c r="I85" t="s">
+        <v>1</v>
+      </c>
+      <c r="J85" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12119;</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
+      <c r="A86">
+        <v>9</v>
+      </c>
+      <c r="B86" t="s">
+        <v>330</v>
+      </c>
+      <c r="C86">
+        <v>12072</v>
+      </c>
+      <c r="D86" t="s">
+        <v>428</v>
+      </c>
+      <c r="E86">
+        <v>47048</v>
+      </c>
+      <c r="F86" t="s">
+        <v>427</v>
+      </c>
+      <c r="G86">
+        <v>12071</v>
+      </c>
+      <c r="I86" t="s">
+        <v>1</v>
+      </c>
+      <c r="J86" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12071;</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
+      <c r="A87">
+        <v>9</v>
+      </c>
+      <c r="B87" t="s">
+        <v>330</v>
+      </c>
+      <c r="C87">
+        <v>12072</v>
+      </c>
+      <c r="D87" t="s">
+        <v>428</v>
+      </c>
+      <c r="E87">
+        <v>47071</v>
+      </c>
+      <c r="F87" t="s">
+        <v>428</v>
+      </c>
+      <c r="G87">
+        <v>12120</v>
+      </c>
+      <c r="I87" t="s">
+        <v>1</v>
+      </c>
+      <c r="J87" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12120;</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
+      <c r="A88">
+        <v>9</v>
+      </c>
+      <c r="B88" t="s">
+        <v>330</v>
+      </c>
+      <c r="C88">
+        <v>12073</v>
+      </c>
+      <c r="D88" t="s">
+        <v>53</v>
+      </c>
+      <c r="E88">
+        <v>47049</v>
+      </c>
+      <c r="F88" t="s">
+        <v>427</v>
+      </c>
+      <c r="G88">
+        <v>12071</v>
+      </c>
+      <c r="I88" t="s">
+        <v>1</v>
+      </c>
+      <c r="J88" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12071;</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
+      <c r="A89">
+        <v>9</v>
+      </c>
+      <c r="B89" t="s">
+        <v>330</v>
+      </c>
+      <c r="C89">
+        <v>12073</v>
+      </c>
+      <c r="D89" t="s">
+        <v>53</v>
+      </c>
+      <c r="E89">
+        <v>47072</v>
+      </c>
+      <c r="F89" t="s">
+        <v>53</v>
+      </c>
+      <c r="G89">
+        <v>12121</v>
+      </c>
+      <c r="I89" t="s">
+        <v>1</v>
+      </c>
+      <c r="J89" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12121;</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="A90">
+        <v>9</v>
+      </c>
+      <c r="B90" t="s">
+        <v>330</v>
+      </c>
+      <c r="C90">
+        <v>12074</v>
+      </c>
+      <c r="D90" t="s">
+        <v>429</v>
+      </c>
+      <c r="E90">
+        <v>47050</v>
+      </c>
+      <c r="F90" t="s">
+        <v>430</v>
+      </c>
+      <c r="G90">
+        <v>12074</v>
+      </c>
+      <c r="I90" t="s">
+        <v>1</v>
+      </c>
+      <c r="J90" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12074;</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10">
+      <c r="A91">
+        <v>9</v>
+      </c>
+      <c r="B91" t="s">
+        <v>330</v>
+      </c>
+      <c r="C91">
+        <v>12074</v>
+      </c>
+      <c r="D91" t="s">
+        <v>429</v>
+      </c>
+      <c r="E91">
+        <v>47073</v>
+      </c>
+      <c r="F91" t="s">
+        <v>431</v>
+      </c>
+      <c r="G91">
+        <v>12122</v>
+      </c>
+      <c r="I91" t="s">
+        <v>1</v>
+      </c>
+      <c r="J91" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12122;</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
+      <c r="A92">
+        <v>9</v>
+      </c>
+      <c r="B92" t="s">
+        <v>330</v>
+      </c>
+      <c r="C92">
+        <v>12075</v>
+      </c>
+      <c r="D92" t="s">
+        <v>432</v>
+      </c>
+      <c r="E92">
+        <v>47051</v>
+      </c>
+      <c r="F92" t="s">
+        <v>433</v>
+      </c>
+      <c r="G92">
+        <v>12075</v>
+      </c>
+      <c r="I92" t="s">
+        <v>1</v>
+      </c>
+      <c r="J92" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12075;</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="A93">
+        <v>9</v>
+      </c>
+      <c r="B93" t="s">
+        <v>330</v>
+      </c>
+      <c r="C93">
+        <v>12075</v>
+      </c>
+      <c r="D93" t="s">
+        <v>432</v>
+      </c>
+      <c r="E93">
+        <v>47074</v>
+      </c>
+      <c r="F93" t="s">
+        <v>434</v>
+      </c>
+      <c r="G93">
+        <v>12123</v>
+      </c>
+      <c r="I93" t="s">
+        <v>1</v>
+      </c>
+      <c r="J93" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12123;</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
+      <c r="A94">
+        <v>9</v>
+      </c>
+      <c r="B94" t="s">
+        <v>330</v>
+      </c>
+      <c r="C94">
+        <v>12076</v>
+      </c>
+      <c r="D94" t="s">
+        <v>435</v>
+      </c>
+      <c r="E94">
+        <v>47132</v>
+      </c>
+      <c r="F94" t="s">
+        <v>392</v>
+      </c>
+      <c r="G94">
+        <v>12023</v>
+      </c>
+      <c r="I94" t="s">
+        <v>1</v>
+      </c>
+      <c r="J94" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12023;</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
+      <c r="A95">
+        <v>9</v>
+      </c>
+      <c r="B95" t="s">
+        <v>330</v>
+      </c>
+      <c r="C95">
+        <v>12076</v>
+      </c>
+      <c r="D95" t="s">
+        <v>435</v>
+      </c>
+      <c r="E95">
+        <v>47052</v>
+      </c>
+      <c r="F95" t="s">
+        <v>436</v>
+      </c>
+      <c r="G95">
+        <v>12076</v>
+      </c>
+      <c r="I95" t="s">
+        <v>1</v>
+      </c>
+      <c r="J95" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12076;</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
+      <c r="A96">
+        <v>9</v>
+      </c>
+      <c r="B96" t="s">
+        <v>330</v>
+      </c>
+      <c r="C96">
+        <v>12076</v>
+      </c>
+      <c r="D96" t="s">
+        <v>435</v>
+      </c>
+      <c r="E96">
+        <v>47075</v>
+      </c>
+      <c r="F96" t="s">
+        <v>56</v>
+      </c>
+      <c r="G96">
+        <v>12124</v>
+      </c>
+      <c r="I96" t="s">
+        <v>1</v>
+      </c>
+      <c r="J96" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12124;</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10">
+      <c r="A97">
+        <v>9</v>
+      </c>
+      <c r="B97" t="s">
+        <v>330</v>
+      </c>
+      <c r="C97">
+        <v>12077</v>
+      </c>
+      <c r="D97" t="s">
+        <v>437</v>
+      </c>
+      <c r="E97">
+        <v>47133</v>
+      </c>
+      <c r="F97" t="s">
+        <v>334</v>
+      </c>
+      <c r="G97">
+        <v>11841</v>
+      </c>
+      <c r="I97" t="s">
+        <v>1</v>
+      </c>
+      <c r="J97" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11841;</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
+      <c r="A98">
+        <v>9</v>
+      </c>
+      <c r="B98" t="s">
+        <v>330</v>
+      </c>
+      <c r="C98">
+        <v>12077</v>
+      </c>
+      <c r="D98" t="s">
+        <v>437</v>
+      </c>
+      <c r="E98">
+        <v>47000</v>
+      </c>
+      <c r="F98" t="s">
+        <v>396</v>
+      </c>
+      <c r="G98">
+        <v>11852</v>
+      </c>
+      <c r="I98" t="s">
+        <v>1</v>
+      </c>
+      <c r="J98" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11852;</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10">
+      <c r="A99">
+        <v>9</v>
+      </c>
+      <c r="B99" t="s">
+        <v>330</v>
+      </c>
+      <c r="C99">
+        <v>12077</v>
+      </c>
+      <c r="D99" t="s">
+        <v>437</v>
+      </c>
+      <c r="E99">
+        <v>47103</v>
+      </c>
+      <c r="F99" t="s">
+        <v>56</v>
+      </c>
+      <c r="G99">
+        <v>12125</v>
+      </c>
+      <c r="I99" t="s">
+        <v>1</v>
+      </c>
+      <c r="J99" t="str">
+        <f t="shared" si="1"/>
+        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12125;</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" s="2" customFormat="1">
+      <c r="A100" s="2">
+        <v>9</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C100" s="2">
+        <v>12161</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E100" s="2">
+        <v>46728</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="G100" s="2">
+        <v>12311</v>
+      </c>
+      <c r="H100" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I100" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" s="2" customFormat="1">
+      <c r="A101" s="2">
+        <v>9</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C101" s="2">
+        <v>12179</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E101" s="2">
+        <v>47085</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="G101" s="2">
+        <v>12423</v>
+      </c>
+      <c r="H101" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="I101" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" s="2" customFormat="1">
+      <c r="A102" s="2">
+        <v>9</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C102" s="2">
+        <v>12184</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E102" s="2">
+        <v>47090</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="G102" s="2">
+        <v>12421</v>
+      </c>
+      <c r="H102" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="I102" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" s="2" customFormat="1">
+      <c r="A103" s="2">
+        <v>9</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C103" s="2">
+        <v>12190</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E103" s="2">
+        <v>47096</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G103" s="2">
+        <v>12314</v>
+      </c>
+      <c r="H103" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I103" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" s="2" customFormat="1">
+      <c r="A104" s="2">
+        <v>9</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C104" s="2">
+        <v>12196</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E104" s="2">
+        <v>47102</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="G104" s="2">
+        <v>12320</v>
+      </c>
+      <c r="H104" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="I104" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" s="2" customFormat="1">
+      <c r="A105" s="2">
+        <v>9</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C105" s="2">
+        <v>12202</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E105" s="2">
+        <v>47139</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="G105" s="2">
+        <v>12315</v>
+      </c>
+      <c r="H105" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="I105" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" s="2" customFormat="1">
+      <c r="A106" s="2">
+        <v>9</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C106" s="2">
+        <v>12208</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E106" s="2">
+        <v>47145</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G106" s="2">
+        <v>12316</v>
+      </c>
+      <c r="H106" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="I106" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" s="2" customFormat="1">
+      <c r="A107" s="2">
+        <v>9</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C107" s="2">
+        <v>12214</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E107" s="2">
+        <v>47151</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="G107" s="2">
+        <v>12321</v>
+      </c>
+      <c r="H107" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="I107" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" s="2" customFormat="1">
+      <c r="A108" s="2">
+        <v>9</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C108" s="2">
+        <v>12220</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E108" s="2">
+        <v>47157</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G108" s="2">
+        <v>12410</v>
+      </c>
+      <c r="H108" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="I108" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" s="2" customFormat="1">
+      <c r="A109" s="2">
+        <v>9</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C109" s="2">
+        <v>12226</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E109" s="2">
+        <v>47163</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G109" s="2">
+        <v>12411</v>
+      </c>
+      <c r="H109" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="I109" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" s="2" customFormat="1">
+      <c r="A110" s="2">
+        <v>9</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C110" s="2">
+        <v>12232</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E110" s="2">
+        <v>47169</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G110" s="2">
+        <v>12412</v>
+      </c>
+      <c r="H110" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="I110" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" s="2" customFormat="1">
+      <c r="A111" s="2">
+        <v>9</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C111" s="2">
+        <v>12238</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E111" s="2">
+        <v>47175</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G111" s="2">
+        <v>12414</v>
+      </c>
+      <c r="H111" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I111" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" s="2" customFormat="1">
+      <c r="A112" s="2">
+        <v>9</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C112" s="2">
+        <v>12245</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E112" s="2">
+        <v>47182</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G112" s="2">
+        <v>12415</v>
+      </c>
+      <c r="H112" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I112" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" s="2" customFormat="1">
+      <c r="A113" s="2">
+        <v>9</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C113" s="2">
+        <v>12252</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E113" s="2">
+        <v>47189</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G113" s="2">
+        <v>12422</v>
+      </c>
+      <c r="H113" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I113" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" s="2" customFormat="1">
+      <c r="A114" s="2">
+        <v>9</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C114" s="2">
+        <v>12271</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E114" s="2">
+        <v>47208</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G114" s="2">
+        <v>12419</v>
+      </c>
+      <c r="H114" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I114" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" s="2" customFormat="1">
+      <c r="A115" s="2">
+        <v>9</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C115" s="2">
+        <v>12280</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E115" s="2">
+        <v>47217</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G115" s="2">
+        <v>12420</v>
+      </c>
+      <c r="H115" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I115" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" s="2" customFormat="1">
+      <c r="A116" s="2">
+        <v>9</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C116" s="2">
+        <v>12288</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E116" s="2">
+        <v>47315</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G116" s="2">
+        <v>12416</v>
+      </c>
+      <c r="H116" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I116" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" s="2" customFormat="1">
+      <c r="A117" s="2">
+        <v>9</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C117" s="2">
+        <v>12296</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E117" s="2">
+        <v>47323</v>
+      </c>
+      <c r="F117" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G117" s="2">
+        <v>12417</v>
+      </c>
+      <c r="H117" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I117" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" s="2" customFormat="1">
+      <c r="A118" s="2">
+        <v>9</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C118" s="2">
+        <v>12304</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E118" s="2">
+        <v>47331</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G118" s="2">
+        <v>12418</v>
+      </c>
+      <c r="H118" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I118" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692C0128-2874-46CB-A76B-5E564EAFF5BE}">
   <dimension ref="A1:J68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -3639,12 +7817,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF445392-2AFB-4227-8589-AE21294CCAEB}">
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -5630,7 +9808,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50ABEE1B-A043-4FB5-8D78-6CD44D39B2E7}">
   <dimension ref="A1:G73"/>
   <sheetViews>
@@ -7396,7 +11574,7 @@
     </row>
   </sheetData>
   <autoFilter ref="B1:F73" xr:uid="{50ABEE1B-A043-4FB5-8D78-6CD44D39B2E7}"/>
-  <sortState ref="A2:F73">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F73">
     <sortCondition ref="B2:B73"/>
     <sortCondition ref="D2:D73"/>
   </sortState>

</xml_diff>

<commit_message>
Added points to profiles of Orcs & Goblins army list
</commit_message>
<xml_diff>
--- a/resources/db/Profiles.xlsx
+++ b/resources/db/Profiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\projects\ArmyBuilder\sourcecode\resources\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE0D7CB-8B54-4793-993D-6B9713B79FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272E107B-E8FC-4726-A32D-9EFB475B9A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{72821A2A-92BA-4C26-854D-A2ECB76DE865}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1375" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1388" uniqueCount="530">
   <si>
     <t>General</t>
   </si>
@@ -1501,6 +1501,135 @@
   </si>
   <si>
     <t>Orks Waldgoblin Meisterschamane</t>
+  </si>
+  <si>
+    <t>Orks Gorfan Rotzahn</t>
+  </si>
+  <si>
+    <t>Orks Azhag der Vernichter</t>
+  </si>
+  <si>
+    <t>Orks Wildork Basis</t>
+  </si>
+  <si>
+    <t>Orks Wildschwein</t>
+  </si>
+  <si>
+    <t>Orks Ork Basis</t>
+  </si>
+  <si>
+    <t>6.5</t>
+  </si>
+  <si>
+    <t>5.5</t>
+  </si>
+  <si>
+    <t>Orks Riesenwolf</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Orks Goblin Basis</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>Orks Waldgoblin Basis</t>
+  </si>
+  <si>
+    <t>Orks Riesenspinne</t>
+  </si>
+  <si>
+    <t>Orks Grobgitz Basis</t>
+  </si>
+  <si>
+    <t>Orks Schwarzork Basis</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Orks Nachtgoblin Basis</t>
+  </si>
+  <si>
+    <t>Orks Höhlensquig</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Orks Fanatic</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>Orks Riese</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>Orks Oger</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>Orks Flußtroll</t>
+  </si>
+  <si>
+    <t>Orks Steintroll</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>Orks Snotling-Base</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Orks Kurbelwagen</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>Orks Kamikaze Katapult</t>
+  </si>
+  <si>
+    <t>97.5</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>Orks Morglum Knochenbrecher</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>Orks Oglock der Fürchtaliche</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>122</t>
   </si>
 </sst>
 </file>
@@ -1548,12 +1677,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1892,8 +2030,8 @@
   <dimension ref="A1:J118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I22" sqref="I22"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -1906,7 +2044,7 @@
     <col min="6" max="6" width="25.625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1934,7 +2072,7 @@
       <c r="H1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1963,7 +2101,7 @@
       <c r="H2" t="s">
         <v>471</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="5">
         <v>80</v>
       </c>
       <c r="J2" t="str">
@@ -1996,7 +2134,7 @@
       <c r="H3" t="s">
         <v>438</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="5">
         <v>65</v>
       </c>
       <c r="J3" t="str">
@@ -2026,12 +2164,15 @@
       <c r="G4">
         <v>11841</v>
       </c>
-      <c r="I4" t="s">
-        <v>1</v>
+      <c r="H4" t="s">
+        <v>494</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>495</v>
       </c>
       <c r="J4" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11841;</v>
+        <v>UPDATE profile SET name = 'Orks Riesenwolf', points = 4 WHERE id =11841;</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -2059,7 +2200,7 @@
       <c r="H5" t="s">
         <v>472</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="5">
         <v>120</v>
       </c>
       <c r="J5" t="str">
@@ -2089,12 +2230,15 @@
       <c r="G6">
         <v>11423</v>
       </c>
-      <c r="I6" t="s">
-        <v>1</v>
+      <c r="H6" t="s">
+        <v>525</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>526</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11423;</v>
+        <v>UPDATE profile SET name = 'Orks Morglum Knochenbrecher', points = 150 WHERE id =11423;</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -2119,12 +2263,15 @@
       <c r="G7">
         <v>11424</v>
       </c>
-      <c r="I7" t="s">
-        <v>1</v>
+      <c r="H7" t="s">
+        <v>527</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>528</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11424;</v>
+        <v>UPDATE profile SET name = 'Orks Oglock der Fürchtaliche', points = 90 WHERE id =11424;</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -2152,7 +2299,7 @@
       <c r="H8" t="s">
         <v>473</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="5">
         <v>80</v>
       </c>
       <c r="J8" t="str">
@@ -2185,7 +2332,7 @@
       <c r="H9" t="s">
         <v>439</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="5">
         <v>50</v>
       </c>
       <c r="J9" t="str">
@@ -2218,7 +2365,7 @@
       <c r="H10" t="s">
         <v>440</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="5">
         <v>110</v>
       </c>
       <c r="J10" t="str">
@@ -2251,7 +2398,7 @@
       <c r="H11" t="s">
         <v>441</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="5">
         <v>140</v>
       </c>
       <c r="J11" t="str">
@@ -2284,7 +2431,7 @@
       <c r="H12" t="s">
         <v>442</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="5">
         <v>150</v>
       </c>
       <c r="J12" t="str">
@@ -2317,7 +2464,7 @@
       <c r="H13" t="s">
         <v>443</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="5">
         <v>50</v>
       </c>
       <c r="J13" t="str">
@@ -2350,7 +2497,7 @@
       <c r="H14" t="s">
         <v>444</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="5">
         <v>50</v>
       </c>
       <c r="J14" t="str">
@@ -2383,7 +2530,7 @@
       <c r="H15" t="s">
         <v>445</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="5">
         <v>50</v>
       </c>
       <c r="J15" t="str">
@@ -2416,7 +2563,7 @@
       <c r="H16" t="s">
         <v>446</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="5">
         <v>92</v>
       </c>
       <c r="J16" t="str">
@@ -2449,7 +2596,7 @@
       <c r="H17" t="s">
         <v>447</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="5">
         <v>83</v>
       </c>
       <c r="J17" t="str">
@@ -2482,7 +2629,7 @@
       <c r="H18" t="s">
         <v>448</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="5">
         <v>95</v>
       </c>
       <c r="J18" t="str">
@@ -2515,7 +2662,7 @@
       <c r="H19" t="s">
         <v>449</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="5">
         <v>65</v>
       </c>
       <c r="J19" t="str">
@@ -2548,7 +2695,7 @@
       <c r="H20" t="s">
         <v>450</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="5">
         <v>65</v>
       </c>
       <c r="J20" t="str">
@@ -2581,7 +2728,7 @@
       <c r="H21" t="s">
         <v>451</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="5">
         <v>65</v>
       </c>
       <c r="J21" t="str">
@@ -2614,12 +2761,12 @@
       <c r="H22" t="s">
         <v>452</v>
       </c>
-      <c r="I22" t="s">
-        <v>1</v>
+      <c r="I22" s="5">
+        <v>91</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Schwarzork Oberboss', points = 0.0 WHERE id =11438;</v>
+        <v>UPDATE profile SET name = 'Orks Schwarzork Oberboss', points = 91 WHERE id =11438;</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -2647,12 +2794,12 @@
       <c r="H23" t="s">
         <v>453</v>
       </c>
-      <c r="I23" t="s">
-        <v>1</v>
+      <c r="I23" s="5">
+        <v>72</v>
       </c>
       <c r="J23" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Ork Oberboss', points = 0.0 WHERE id =11439;</v>
+        <v>UPDATE profile SET name = 'Orks Ork Oberboss', points = 72 WHERE id =11439;</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -2680,12 +2827,12 @@
       <c r="H24" t="s">
         <v>454</v>
       </c>
-      <c r="I24" t="s">
-        <v>1</v>
+      <c r="I24" s="5">
+        <v>98</v>
       </c>
       <c r="J24" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Wildork Oberboss', points = 0.0 WHERE id =11440;</v>
+        <v>UPDATE profile SET name = 'Orks Wildork Oberboss', points = 98 WHERE id =11440;</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -2713,12 +2860,12 @@
       <c r="H25" t="s">
         <v>455</v>
       </c>
-      <c r="I25" t="s">
-        <v>1</v>
+      <c r="I25" s="5">
+        <v>33</v>
       </c>
       <c r="J25" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Goblin Oberboss', points = 0.0 WHERE id =11441;</v>
+        <v>UPDATE profile SET name = 'Orks Goblin Oberboss', points = 33 WHERE id =11441;</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -2746,12 +2893,12 @@
       <c r="H26" t="s">
         <v>456</v>
       </c>
-      <c r="I26" t="s">
-        <v>1</v>
+      <c r="I26" s="5">
+        <v>33</v>
       </c>
       <c r="J26" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Waldgoblin Oberboss', points = 0.0 WHERE id =11442;</v>
+        <v>UPDATE profile SET name = 'Orks Waldgoblin Oberboss', points = 33 WHERE id =11442;</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -2779,12 +2926,12 @@
       <c r="H27" t="s">
         <v>457</v>
       </c>
-      <c r="I27" t="s">
-        <v>1</v>
+      <c r="I27" s="5">
+        <v>33</v>
       </c>
       <c r="J27" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Nachtgoblin Oberboss', points = 0.0 WHERE id =11443;</v>
+        <v>UPDATE profile SET name = 'Orks Nachtgoblin Oberboss', points = 33 WHERE id =11443;</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -2812,12 +2959,12 @@
       <c r="H28" t="s">
         <v>458</v>
       </c>
-      <c r="I28" t="s">
-        <v>1</v>
+      <c r="I28" s="5">
+        <v>42</v>
       </c>
       <c r="J28" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Schwarzork Boss', points = 0.0 WHERE id =11444;</v>
+        <v>UPDATE profile SET name = 'Orks Schwarzork Boss', points = 42 WHERE id =11444;</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -2845,12 +2992,12 @@
       <c r="H29" t="s">
         <v>459</v>
       </c>
-      <c r="I29" t="s">
-        <v>1</v>
+      <c r="I29" s="5">
+        <v>33</v>
       </c>
       <c r="J29" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Ork Boss', points = 0.0 WHERE id =11445;</v>
+        <v>UPDATE profile SET name = 'Orks Ork Boss', points = 33 WHERE id =11445;</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -2878,12 +3025,12 @@
       <c r="H30" t="s">
         <v>460</v>
       </c>
-      <c r="I30" t="s">
-        <v>1</v>
+      <c r="I30" s="5">
+        <v>33</v>
       </c>
       <c r="J30" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Wildork Boss', points = 0.0 WHERE id =11446;</v>
+        <v>UPDATE profile SET name = 'Orks Wildork Boss', points = 33 WHERE id =11446;</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -2911,12 +3058,12 @@
       <c r="H31" t="s">
         <v>461</v>
       </c>
-      <c r="I31" t="s">
-        <v>1</v>
+      <c r="I31" s="5">
+        <v>15</v>
       </c>
       <c r="J31" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Goblin Boss', points = 0.0 WHERE id =11447;</v>
+        <v>UPDATE profile SET name = 'Orks Goblin Boss', points = 15 WHERE id =11447;</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -2944,12 +3091,12 @@
       <c r="H32" t="s">
         <v>462</v>
       </c>
-      <c r="I32" t="s">
-        <v>1</v>
+      <c r="I32" s="5">
+        <v>15</v>
       </c>
       <c r="J32" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Waldgoblin Boss', points = 0.0 WHERE id =11448;</v>
+        <v>UPDATE profile SET name = 'Orks Waldgoblin Boss', points = 15 WHERE id =11448;</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -2977,12 +3124,12 @@
       <c r="H33" t="s">
         <v>463</v>
       </c>
-      <c r="I33" t="s">
-        <v>1</v>
+      <c r="I33" s="5">
+        <v>15</v>
       </c>
       <c r="J33" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Nachtgoblin Boss', points = 0.0 WHERE id =11449;</v>
+        <v>UPDATE profile SET name = 'Orks Nachtgoblin Boss', points = 15 WHERE id =11449;</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -3010,12 +3157,12 @@
       <c r="H34" t="s">
         <v>464</v>
       </c>
-      <c r="I34" t="s">
-        <v>1</v>
+      <c r="I34" s="5">
+        <v>56</v>
       </c>
       <c r="J34" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Ork Schamane', points = 0.0 WHERE id =11450;</v>
+        <v>UPDATE profile SET name = 'Orks Ork Schamane', points = 56 WHERE id =11450;</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -3043,12 +3190,12 @@
       <c r="H35" t="s">
         <v>465</v>
       </c>
-      <c r="I35" t="s">
-        <v>1</v>
+      <c r="I35" s="5">
+        <v>59</v>
       </c>
       <c r="J35" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Wildork Schamane', points = 0.0 WHERE id =11451;</v>
+        <v>UPDATE profile SET name = 'Orks Wildork Schamane', points = 59 WHERE id =11451;</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -3076,12 +3223,12 @@
       <c r="H36" t="s">
         <v>466</v>
       </c>
-      <c r="I36" t="s">
-        <v>1</v>
+      <c r="I36" s="5">
+        <v>28</v>
       </c>
       <c r="J36" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Goblin Schamane', points = 0.0 WHERE id =11452;</v>
+        <v>UPDATE profile SET name = 'Orks Goblin Schamane', points = 28 WHERE id =11452;</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -3109,12 +3256,12 @@
       <c r="H37" t="s">
         <v>467</v>
       </c>
-      <c r="I37" t="s">
-        <v>1</v>
+      <c r="I37" s="5">
+        <v>28</v>
       </c>
       <c r="J37" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Nachtgoblin Schamane', points = 0.0 WHERE id =11453;</v>
+        <v>UPDATE profile SET name = 'Orks Nachtgoblin Schamane', points = 28 WHERE id =11453;</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -3142,12 +3289,12 @@
       <c r="H38" t="s">
         <v>468</v>
       </c>
-      <c r="I38" t="s">
-        <v>1</v>
+      <c r="I38" s="5">
+        <v>28</v>
       </c>
       <c r="J38" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Waldgoblin Schamane', points = 0.0 WHERE id =11454;</v>
+        <v>UPDATE profile SET name = 'Orks Waldgoblin Schamane', points = 28 WHERE id =11454;</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -3175,12 +3322,12 @@
       <c r="H39" t="s">
         <v>469</v>
       </c>
-      <c r="I39" t="s">
-        <v>1</v>
+      <c r="I39" s="5">
+        <v>118</v>
       </c>
       <c r="J39" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Ork Oberschamane', points = 0.0 WHERE id =11455;</v>
+        <v>UPDATE profile SET name = 'Orks Ork Oberschamane', points = 118 WHERE id =11455;</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -3208,12 +3355,12 @@
       <c r="H40" t="s">
         <v>470</v>
       </c>
-      <c r="I40" t="s">
-        <v>1</v>
+      <c r="I40" s="5" t="s">
+        <v>529</v>
       </c>
       <c r="J40" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Wildork Oberschamane', points = 0.0 WHERE id =11456;</v>
+        <v>UPDATE profile SET name = 'Orks Wildork Oberschamane', points = 122 WHERE id =11456;</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -3241,12 +3388,12 @@
       <c r="H41" t="s">
         <v>474</v>
       </c>
-      <c r="I41" t="s">
-        <v>1</v>
+      <c r="I41" s="5">
+        <v>83</v>
       </c>
       <c r="J41" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Goblin Oberschamane', points = 0.0 WHERE id =11457;</v>
+        <v>UPDATE profile SET name = 'Orks Goblin Oberschamane', points = 83 WHERE id =11457;</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -3274,12 +3421,12 @@
       <c r="H42" t="s">
         <v>475</v>
       </c>
-      <c r="I42" t="s">
-        <v>1</v>
+      <c r="I42" s="5">
+        <v>83</v>
       </c>
       <c r="J42" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Nachtgoblin Oberschamane', points = 0.0 WHERE id =11458;</v>
+        <v>UPDATE profile SET name = 'Orks Nachtgoblin Oberschamane', points = 83 WHERE id =11458;</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -3307,12 +3454,12 @@
       <c r="H43" t="s">
         <v>476</v>
       </c>
-      <c r="I43" t="s">
-        <v>1</v>
+      <c r="I43" s="5">
+        <v>83</v>
       </c>
       <c r="J43" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Waldgoblin Oberschamane', points = 0.0 WHERE id =11459;</v>
+        <v>UPDATE profile SET name = 'Orks Waldgoblin Oberschamane', points = 83 WHERE id =11459;</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -3340,12 +3487,12 @@
       <c r="H44" t="s">
         <v>477</v>
       </c>
-      <c r="I44" t="s">
-        <v>1</v>
+      <c r="I44" s="5">
+        <v>190</v>
       </c>
       <c r="J44" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Ork Großschamane', points = 0.0 WHERE id =11460;</v>
+        <v>UPDATE profile SET name = 'Orks Ork Großschamane', points = 190 WHERE id =11460;</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -3373,12 +3520,12 @@
       <c r="H45" t="s">
         <v>478</v>
       </c>
-      <c r="I45" t="s">
-        <v>1</v>
+      <c r="I45" s="5">
+        <v>219</v>
       </c>
       <c r="J45" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Wildork Großschamane', points = 0.0 WHERE id =11461;</v>
+        <v>UPDATE profile SET name = 'Orks Wildork Großschamane', points = 219 WHERE id =11461;</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -3406,12 +3553,12 @@
       <c r="H46" t="s">
         <v>479</v>
       </c>
-      <c r="I46" t="s">
-        <v>1</v>
+      <c r="I46" s="5">
+        <v>159</v>
       </c>
       <c r="J46" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Goblin Großschamane', points = 0.0 WHERE id =11462;</v>
+        <v>UPDATE profile SET name = 'Orks Goblin Großschamane', points = 159 WHERE id =11462;</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -3439,12 +3586,12 @@
       <c r="H47" t="s">
         <v>480</v>
       </c>
-      <c r="I47" t="s">
-        <v>1</v>
+      <c r="I47" s="5">
+        <v>159</v>
       </c>
       <c r="J47" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Nachtgoblin Großschamane', points = 0.0 WHERE id =11463;</v>
+        <v>UPDATE profile SET name = 'Orks Nachtgoblin Großschamane', points = 159 WHERE id =11463;</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -3472,12 +3619,12 @@
       <c r="H48" t="s">
         <v>481</v>
       </c>
-      <c r="I48" t="s">
-        <v>1</v>
+      <c r="I48" s="5">
+        <v>159</v>
       </c>
       <c r="J48" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Waldgoblin Großschamane', points = 0.0 WHERE id =11464;</v>
+        <v>UPDATE profile SET name = 'Orks Waldgoblin Großschamane', points = 159 WHERE id =11464;</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -3505,12 +3652,12 @@
       <c r="H49" t="s">
         <v>482</v>
       </c>
-      <c r="I49" t="s">
-        <v>1</v>
+      <c r="I49" s="5">
+        <v>287</v>
       </c>
       <c r="J49" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Ork Meisterschamane', points = 0.0 WHERE id =11465;</v>
+        <v>UPDATE profile SET name = 'Orks Ork Meisterschamane', points = 287 WHERE id =11465;</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -3538,12 +3685,12 @@
       <c r="H50" t="s">
         <v>483</v>
       </c>
-      <c r="I50" t="s">
-        <v>1</v>
+      <c r="I50" s="5">
+        <v>303</v>
       </c>
       <c r="J50" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Wildork Meisterschamane', points = 0.0 WHERE id =11466;</v>
+        <v>UPDATE profile SET name = 'Orks Wildork Meisterschamane', points = 303 WHERE id =11466;</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -3571,12 +3718,12 @@
       <c r="H51" t="s">
         <v>484</v>
       </c>
-      <c r="I51" t="s">
-        <v>1</v>
+      <c r="I51" s="5">
+        <v>253</v>
       </c>
       <c r="J51" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Goblin Meisterschamane', points = 0.0 WHERE id =11467;</v>
+        <v>UPDATE profile SET name = 'Orks Goblin Meisterschamane', points = 253 WHERE id =11467;</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -3604,12 +3751,12 @@
       <c r="H52" t="s">
         <v>485</v>
       </c>
-      <c r="I52" t="s">
-        <v>1</v>
+      <c r="I52" s="5">
+        <v>253</v>
       </c>
       <c r="J52" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Nachtgoblin Meisterschamane', points = 0.0 WHERE id =11468;</v>
+        <v>UPDATE profile SET name = 'Orks Nachtgoblin Meisterschamane', points = 253 WHERE id =11468;</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -3637,12 +3784,12 @@
       <c r="H53" t="s">
         <v>486</v>
       </c>
-      <c r="I53" t="s">
-        <v>1</v>
+      <c r="I53" s="5">
+        <v>253</v>
       </c>
       <c r="J53" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Waldgoblin Meisterschamane', points = 0.0 WHERE id =11469;</v>
+        <v>UPDATE profile SET name = 'Orks Waldgoblin Meisterschamane', points = 253 WHERE id =11469;</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -3667,12 +3814,15 @@
       <c r="G54">
         <v>11586</v>
       </c>
-      <c r="I54" t="s">
-        <v>1</v>
+      <c r="H54" t="s">
+        <v>487</v>
+      </c>
+      <c r="I54" s="5">
+        <v>90</v>
       </c>
       <c r="J54" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11586;</v>
+        <v>UPDATE profile SET name = 'Orks Gorfan Rotzahn', points = 90 WHERE id =11586;</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -3697,12 +3847,15 @@
       <c r="G55">
         <v>11643</v>
       </c>
-      <c r="I55" t="s">
-        <v>1</v>
+      <c r="H55" t="s">
+        <v>488</v>
+      </c>
+      <c r="I55" s="5">
+        <v>130</v>
       </c>
       <c r="J55" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11643;</v>
+        <v>UPDATE profile SET name = 'Orks Azhag der Vernichter', points = 130 WHERE id =11643;</v>
       </c>
     </row>
     <row r="56" spans="1:10" s="2" customFormat="1">
@@ -3730,12 +3883,12 @@
       <c r="H56" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="I56" s="2" t="s">
-        <v>250</v>
+      <c r="I56" s="6">
+        <v>180</v>
       </c>
       <c r="J56" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Lindwurm', points = 180.0 WHERE id =12423;</v>
+        <v>UPDATE profile SET name = 'Lindwurm', points = 180 WHERE id =12423;</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -3760,12 +3913,15 @@
       <c r="G57">
         <v>11850</v>
       </c>
-      <c r="I57" t="s">
-        <v>1</v>
+      <c r="H57" t="s">
+        <v>489</v>
+      </c>
+      <c r="I57" s="5" t="s">
+        <v>492</v>
       </c>
       <c r="J57" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11850;</v>
+        <v>UPDATE profile SET name = 'Orks Wildork Basis', points = 6.5 WHERE id =11850;</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -3790,12 +3946,15 @@
       <c r="G58">
         <v>12023</v>
       </c>
-      <c r="I58" t="s">
-        <v>1</v>
+      <c r="H58" t="s">
+        <v>490</v>
+      </c>
+      <c r="I58" s="5">
+        <v>8</v>
       </c>
       <c r="J58" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12023;</v>
+        <v>UPDATE profile SET name = 'Orks Wildschwein', points = 8 WHERE id =12023;</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -3820,12 +3979,15 @@
       <c r="G59">
         <v>11851</v>
       </c>
-      <c r="I59" t="s">
-        <v>1</v>
+      <c r="H59" t="s">
+        <v>491</v>
+      </c>
+      <c r="I59" s="5" t="s">
+        <v>493</v>
       </c>
       <c r="J59" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11851;</v>
+        <v>UPDATE profile SET name = 'Orks Ork Basis', points = 5.5 WHERE id =11851;</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -3850,12 +4012,15 @@
       <c r="G60">
         <v>12023</v>
       </c>
-      <c r="I60" t="s">
-        <v>1</v>
+      <c r="H60" t="s">
+        <v>490</v>
+      </c>
+      <c r="I60" s="5" t="s">
+        <v>493</v>
       </c>
       <c r="J60" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12023;</v>
+        <v>UPDATE profile SET name = 'Orks Wildschwein', points = 5.5 WHERE id =12023;</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -3880,12 +4045,15 @@
       <c r="G61">
         <v>11841</v>
       </c>
-      <c r="I61" t="s">
-        <v>1</v>
+      <c r="H61" t="s">
+        <v>494</v>
+      </c>
+      <c r="I61" s="5" t="s">
+        <v>495</v>
       </c>
       <c r="J61" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11841;</v>
+        <v>UPDATE profile SET name = 'Orks Riesenwolf', points = 4 WHERE id =11841;</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -3910,12 +4078,15 @@
       <c r="G62">
         <v>11852</v>
       </c>
-      <c r="I62" t="s">
-        <v>1</v>
+      <c r="H62" t="s">
+        <v>496</v>
+      </c>
+      <c r="I62" s="5" t="s">
+        <v>497</v>
       </c>
       <c r="J62" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11852;</v>
+        <v>UPDATE profile SET name = 'Orks Goblin Basis', points = 2.5 WHERE id =11852;</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -3940,12 +4111,15 @@
       <c r="G63">
         <v>11853</v>
       </c>
-      <c r="I63" t="s">
-        <v>1</v>
+      <c r="H63" t="s">
+        <v>498</v>
+      </c>
+      <c r="I63" s="5" t="s">
+        <v>497</v>
       </c>
       <c r="J63" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11853;</v>
+        <v>UPDATE profile SET name = 'Orks Waldgoblin Basis', points = 2.5 WHERE id =11853;</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -3970,12 +4144,15 @@
       <c r="G64">
         <v>12026</v>
       </c>
-      <c r="I64" t="s">
-        <v>1</v>
+      <c r="H64" t="s">
+        <v>499</v>
+      </c>
+      <c r="I64" s="5" t="s">
+        <v>492</v>
       </c>
       <c r="J64" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12026;</v>
+        <v>UPDATE profile SET name = 'Orks Riesenspinne', points = 6.5 WHERE id =12026;</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -4000,12 +4177,15 @@
       <c r="G65">
         <v>11854</v>
       </c>
-      <c r="I65" t="s">
-        <v>1</v>
+      <c r="H65" t="s">
+        <v>500</v>
+      </c>
+      <c r="I65" s="5" t="s">
+        <v>492</v>
       </c>
       <c r="J65" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11854;</v>
+        <v>UPDATE profile SET name = 'Orks Grobgitz Basis', points = 6.5 WHERE id =11854;</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -4030,12 +4210,15 @@
       <c r="G66">
         <v>11855</v>
       </c>
-      <c r="I66" t="s">
-        <v>1</v>
+      <c r="H66" t="s">
+        <v>491</v>
+      </c>
+      <c r="I66" s="5" t="s">
+        <v>493</v>
       </c>
       <c r="J66" t="str">
         <f t="shared" ref="J66:J99" si="1">CONCATENATE("UPDATE profile SET name = '",H66,"', points = ",I66," WHERE id =",G66,";")</f>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11855;</v>
+        <v>UPDATE profile SET name = 'Orks Ork Basis', points = 5.5 WHERE id =11855;</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -4060,12 +4243,15 @@
       <c r="G67">
         <v>11856</v>
       </c>
-      <c r="I67" t="s">
-        <v>1</v>
+      <c r="H67" t="s">
+        <v>491</v>
+      </c>
+      <c r="I67" s="5" t="s">
+        <v>493</v>
       </c>
       <c r="J67" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11856;</v>
+        <v>UPDATE profile SET name = 'Orks Ork Basis', points = 5.5 WHERE id =11856;</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -4090,12 +4276,15 @@
       <c r="G68">
         <v>11857</v>
       </c>
-      <c r="I68" t="s">
-        <v>1</v>
+      <c r="H68" t="s">
+        <v>501</v>
+      </c>
+      <c r="I68" s="5" t="s">
+        <v>502</v>
       </c>
       <c r="J68" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11857;</v>
+        <v>UPDATE profile SET name = 'Orks Schwarzork Basis', points = 8 WHERE id =11857;</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -4120,12 +4309,15 @@
       <c r="G69">
         <v>11858</v>
       </c>
-      <c r="I69" t="s">
-        <v>1</v>
+      <c r="H69" t="s">
+        <v>489</v>
+      </c>
+      <c r="I69" s="5" t="s">
+        <v>492</v>
       </c>
       <c r="J69" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11858;</v>
+        <v>UPDATE profile SET name = 'Orks Wildork Basis', points = 6.5 WHERE id =11858;</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -4150,12 +4342,15 @@
       <c r="G70">
         <v>11852</v>
       </c>
-      <c r="I70" t="s">
-        <v>1</v>
+      <c r="H70" t="s">
+        <v>496</v>
+      </c>
+      <c r="I70" s="5" t="s">
+        <v>497</v>
       </c>
       <c r="J70" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11852;</v>
+        <v>UPDATE profile SET name = 'Orks Goblin Basis', points = 2.5 WHERE id =11852;</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -4180,12 +4375,15 @@
       <c r="G71">
         <v>11853</v>
       </c>
-      <c r="I71" t="s">
-        <v>1</v>
+      <c r="H71" t="s">
+        <v>498</v>
+      </c>
+      <c r="I71" s="5" t="s">
+        <v>497</v>
       </c>
       <c r="J71" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11853;</v>
+        <v>UPDATE profile SET name = 'Orks Waldgoblin Basis', points = 2.5 WHERE id =11853;</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -4210,12 +4408,15 @@
       <c r="G72">
         <v>11861</v>
       </c>
-      <c r="I72" t="s">
-        <v>1</v>
+      <c r="H72" t="s">
+        <v>503</v>
+      </c>
+      <c r="I72" s="5" t="s">
+        <v>497</v>
       </c>
       <c r="J72" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11861;</v>
+        <v>UPDATE profile SET name = 'Orks Nachtgoblin Basis', points = 2.5 WHERE id =11861;</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -4240,12 +4441,15 @@
       <c r="G73">
         <v>11862</v>
       </c>
-      <c r="I73" t="s">
-        <v>1</v>
+      <c r="H73" t="s">
+        <v>503</v>
+      </c>
+      <c r="I73" s="5" t="s">
+        <v>497</v>
       </c>
       <c r="J73" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11862;</v>
+        <v>UPDATE profile SET name = 'Orks Nachtgoblin Basis', points = 2.5 WHERE id =11862;</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -4270,12 +4474,15 @@
       <c r="G74">
         <v>12027</v>
       </c>
-      <c r="I74" t="s">
-        <v>1</v>
+      <c r="H74" t="s">
+        <v>504</v>
+      </c>
+      <c r="I74" s="5" t="s">
+        <v>505</v>
       </c>
       <c r="J74" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12027;</v>
+        <v>UPDATE profile SET name = 'Orks Höhlensquig', points = 20 WHERE id =12027;</v>
       </c>
     </row>
     <row r="75" spans="1:10">
@@ -4300,12 +4507,15 @@
       <c r="G75">
         <v>11863</v>
       </c>
-      <c r="I75" t="s">
-        <v>1</v>
+      <c r="H75" t="s">
+        <v>503</v>
+      </c>
+      <c r="I75" s="5" t="s">
+        <v>497</v>
       </c>
       <c r="J75" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11863;</v>
+        <v>UPDATE profile SET name = 'Orks Nachtgoblin Basis', points = 2.5 WHERE id =11863;</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -4330,12 +4540,15 @@
       <c r="G76">
         <v>11864</v>
       </c>
-      <c r="I76" t="s">
-        <v>1</v>
+      <c r="H76" t="s">
+        <v>506</v>
+      </c>
+      <c r="I76" s="5" t="s">
+        <v>507</v>
       </c>
       <c r="J76" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11864;</v>
+        <v>UPDATE profile SET name = 'Orks Fanatic', points = 30 WHERE id =11864;</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -4360,12 +4573,15 @@
       <c r="G77">
         <v>11861</v>
       </c>
-      <c r="I77" t="s">
-        <v>1</v>
+      <c r="H77" t="s">
+        <v>503</v>
+      </c>
+      <c r="I77" s="5" t="s">
+        <v>497</v>
       </c>
       <c r="J77" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11861;</v>
+        <v>UPDATE profile SET name = 'Orks Nachtgoblin Basis', points = 2.5 WHERE id =11861;</v>
       </c>
     </row>
     <row r="78" spans="1:10">
@@ -4390,12 +4606,15 @@
       <c r="G78">
         <v>12028</v>
       </c>
-      <c r="I78" t="s">
-        <v>1</v>
+      <c r="H78" t="s">
+        <v>504</v>
+      </c>
+      <c r="I78" s="5" t="s">
+        <v>505</v>
       </c>
       <c r="J78" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12028;</v>
+        <v>UPDATE profile SET name = 'Orks Höhlensquig', points = 20 WHERE id =12028;</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -4420,12 +4639,15 @@
       <c r="G79">
         <v>11866</v>
       </c>
-      <c r="I79" t="s">
-        <v>1</v>
+      <c r="H79" t="s">
+        <v>508</v>
+      </c>
+      <c r="I79" s="5" t="s">
+        <v>509</v>
       </c>
       <c r="J79" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11866;</v>
+        <v>UPDATE profile SET name = 'Orks Riese', points = 200 WHERE id =11866;</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -4450,12 +4672,15 @@
       <c r="G80">
         <v>11867</v>
       </c>
-      <c r="I80" t="s">
-        <v>1</v>
+      <c r="H80" t="s">
+        <v>510</v>
+      </c>
+      <c r="I80" s="5" t="s">
+        <v>511</v>
       </c>
       <c r="J80" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11867;</v>
+        <v>UPDATE profile SET name = 'Orks Oger', points = 40 WHERE id =11867;</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -4480,12 +4705,15 @@
       <c r="G81">
         <v>11868</v>
       </c>
-      <c r="I81" t="s">
-        <v>1</v>
+      <c r="H81" t="s">
+        <v>512</v>
+      </c>
+      <c r="I81" s="5" t="s">
+        <v>514</v>
       </c>
       <c r="J81" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11868;</v>
+        <v>UPDATE profile SET name = 'Orks Flußtroll', points = 65 WHERE id =11868;</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -4510,12 +4738,15 @@
       <c r="G82">
         <v>11869</v>
       </c>
-      <c r="I82" t="s">
-        <v>1</v>
+      <c r="H82" t="s">
+        <v>513</v>
+      </c>
+      <c r="I82" s="5" t="s">
+        <v>514</v>
       </c>
       <c r="J82" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11869;</v>
+        <v>UPDATE profile SET name = 'Orks Steintroll', points = 65 WHERE id =11869;</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -4540,12 +4771,15 @@
       <c r="G83">
         <v>11870</v>
       </c>
-      <c r="I83" t="s">
-        <v>1</v>
+      <c r="H83" t="s">
+        <v>515</v>
+      </c>
+      <c r="I83" s="5" t="s">
+        <v>516</v>
       </c>
       <c r="J83" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11870;</v>
+        <v>UPDATE profile SET name = 'Orks Snotling-Base', points = 15 WHERE id =11870;</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -4570,12 +4804,15 @@
       <c r="G84">
         <v>12071</v>
       </c>
-      <c r="I84" t="s">
-        <v>1</v>
+      <c r="H84" t="s">
+        <v>491</v>
+      </c>
+      <c r="I84" s="5" t="s">
+        <v>493</v>
       </c>
       <c r="J84" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12071;</v>
+        <v>UPDATE profile SET name = 'Orks Ork Basis', points = 5.5 WHERE id =12071;</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -4600,12 +4837,15 @@
       <c r="G85">
         <v>12119</v>
       </c>
-      <c r="I85" t="s">
-        <v>1</v>
+      <c r="H85" t="s">
+        <v>174</v>
+      </c>
+      <c r="I85" s="5" t="s">
+        <v>519</v>
       </c>
       <c r="J85" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12119;</v>
+        <v>UPDATE profile SET name = 'Kleine Steinschleuder', points = 74 WHERE id =12119;</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -4630,12 +4870,15 @@
       <c r="G86">
         <v>12071</v>
       </c>
-      <c r="I86" t="s">
-        <v>1</v>
+      <c r="H86" t="s">
+        <v>491</v>
+      </c>
+      <c r="I86" s="5" t="s">
+        <v>493</v>
       </c>
       <c r="J86" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12071;</v>
+        <v>UPDATE profile SET name = 'Orks Ork Basis', points = 5.5 WHERE id =12071;</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -4660,12 +4903,15 @@
       <c r="G87">
         <v>12120</v>
       </c>
-      <c r="I87" t="s">
-        <v>1</v>
+      <c r="H87" t="s">
+        <v>176</v>
+      </c>
+      <c r="I87" s="5" t="s">
+        <v>520</v>
       </c>
       <c r="J87" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12120;</v>
+        <v>UPDATE profile SET name = 'Große Steinschleuder', points = 104 WHERE id =12120;</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -4690,12 +4936,15 @@
       <c r="G88">
         <v>12071</v>
       </c>
-      <c r="I88" t="s">
-        <v>1</v>
+      <c r="H88" t="s">
+        <v>491</v>
+      </c>
+      <c r="I88" s="5" t="s">
+        <v>493</v>
       </c>
       <c r="J88" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12071;</v>
+        <v>UPDATE profile SET name = 'Orks Ork Basis', points = 5.5 WHERE id =12071;</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -4720,12 +4969,15 @@
       <c r="G89">
         <v>12121</v>
       </c>
-      <c r="I89" t="s">
-        <v>1</v>
+      <c r="H89" t="s">
+        <v>53</v>
+      </c>
+      <c r="I89" s="5" t="s">
+        <v>521</v>
       </c>
       <c r="J89" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12121;</v>
+        <v>UPDATE profile SET name = 'Speerschleuder', points = 54 WHERE id =12121;</v>
       </c>
     </row>
     <row r="90" spans="1:10">
@@ -4750,12 +5002,15 @@
       <c r="G90">
         <v>12074</v>
       </c>
-      <c r="I90" t="s">
-        <v>1</v>
+      <c r="H90" t="s">
+        <v>515</v>
+      </c>
+      <c r="I90" s="5" t="s">
+        <v>516</v>
       </c>
       <c r="J90" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12074;</v>
+        <v>UPDATE profile SET name = 'Orks Snotling-Base', points = 15 WHERE id =12074;</v>
       </c>
     </row>
     <row r="91" spans="1:10">
@@ -4780,12 +5035,15 @@
       <c r="G91">
         <v>12122</v>
       </c>
-      <c r="I91" t="s">
-        <v>1</v>
+      <c r="H91" t="s">
+        <v>517</v>
+      </c>
+      <c r="I91" s="5" t="s">
+        <v>518</v>
       </c>
       <c r="J91" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12122;</v>
+        <v>UPDATE profile SET name = 'Orks Kurbelwagen', points = 25 WHERE id =12122;</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -4810,12 +5068,15 @@
       <c r="G92">
         <v>12075</v>
       </c>
-      <c r="I92" t="s">
-        <v>1</v>
+      <c r="H92" t="s">
+        <v>496</v>
+      </c>
+      <c r="I92" s="5" t="s">
+        <v>497</v>
       </c>
       <c r="J92" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12075;</v>
+        <v>UPDATE profile SET name = 'Orks Goblin Basis', points = 2.5 WHERE id =12075;</v>
       </c>
     </row>
     <row r="93" spans="1:10">
@@ -4840,12 +5101,15 @@
       <c r="G93">
         <v>12123</v>
       </c>
-      <c r="I93" t="s">
-        <v>1</v>
+      <c r="H93" t="s">
+        <v>522</v>
+      </c>
+      <c r="I93" s="5" t="s">
+        <v>523</v>
       </c>
       <c r="J93" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12123;</v>
+        <v>UPDATE profile SET name = 'Orks Kamikaze Katapult', points = 97.5 WHERE id =12123;</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -4870,12 +5134,15 @@
       <c r="G94">
         <v>12023</v>
       </c>
-      <c r="I94" t="s">
-        <v>1</v>
+      <c r="H94" t="s">
+        <v>490</v>
+      </c>
+      <c r="I94" s="5" t="s">
+        <v>493</v>
       </c>
       <c r="J94" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12023;</v>
+        <v>UPDATE profile SET name = 'Orks Wildschwein', points = 5.5 WHERE id =12023;</v>
       </c>
     </row>
     <row r="95" spans="1:10">
@@ -4900,12 +5167,15 @@
       <c r="G95">
         <v>12076</v>
       </c>
-      <c r="I95" t="s">
-        <v>1</v>
+      <c r="H95" t="s">
+        <v>491</v>
+      </c>
+      <c r="I95" s="5" t="s">
+        <v>493</v>
       </c>
       <c r="J95" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12076;</v>
+        <v>UPDATE profile SET name = 'Orks Ork Basis', points = 5.5 WHERE id =12076;</v>
       </c>
     </row>
     <row r="96" spans="1:10">
@@ -4930,12 +5200,15 @@
       <c r="G96">
         <v>12124</v>
       </c>
-      <c r="I96" t="s">
-        <v>1</v>
+      <c r="H96" t="s">
+        <v>56</v>
+      </c>
+      <c r="I96" s="5" t="s">
+        <v>524</v>
       </c>
       <c r="J96" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12124;</v>
+        <v>UPDATE profile SET name = 'Streitwagen', points = 50 WHERE id =12124;</v>
       </c>
     </row>
     <row r="97" spans="1:10">
@@ -4960,12 +5233,15 @@
       <c r="G97">
         <v>11841</v>
       </c>
-      <c r="I97" t="s">
-        <v>1</v>
+      <c r="H97" t="s">
+        <v>494</v>
+      </c>
+      <c r="I97" s="5" t="s">
+        <v>495</v>
       </c>
       <c r="J97" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11841;</v>
+        <v>UPDATE profile SET name = 'Orks Riesenwolf', points = 4 WHERE id =11841;</v>
       </c>
     </row>
     <row r="98" spans="1:10">
@@ -4990,12 +5266,15 @@
       <c r="G98">
         <v>11852</v>
       </c>
-      <c r="I98" t="s">
-        <v>1</v>
+      <c r="H98" t="s">
+        <v>496</v>
+      </c>
+      <c r="I98" s="5" t="s">
+        <v>497</v>
       </c>
       <c r="J98" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11852;</v>
+        <v>UPDATE profile SET name = 'Orks Goblin Basis', points = 2.5 WHERE id =11852;</v>
       </c>
     </row>
     <row r="99" spans="1:10">
@@ -5020,12 +5299,15 @@
       <c r="G99">
         <v>12125</v>
       </c>
-      <c r="I99" t="s">
-        <v>1</v>
+      <c r="H99" t="s">
+        <v>56</v>
+      </c>
+      <c r="I99" s="5" t="s">
+        <v>524</v>
       </c>
       <c r="J99" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12125;</v>
+        <v>UPDATE profile SET name = 'Streitwagen', points = 50 WHERE id =12125;</v>
       </c>
     </row>
     <row r="100" spans="1:10" s="2" customFormat="1">
@@ -5053,7 +5335,7 @@
       <c r="H100" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="I100" s="2" t="s">
+      <c r="I100" s="6" t="s">
         <v>246</v>
       </c>
     </row>
@@ -5082,7 +5364,7 @@
       <c r="H101" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="I101" s="2" t="s">
+      <c r="I101" s="6" t="s">
         <v>250</v>
       </c>
     </row>
@@ -5111,7 +5393,7 @@
       <c r="H102" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="I102" s="2" t="s">
+      <c r="I102" s="6" t="s">
         <v>230</v>
       </c>
     </row>
@@ -5140,7 +5422,7 @@
       <c r="H103" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="I103" s="2" t="s">
+      <c r="I103" s="6" t="s">
         <v>246</v>
       </c>
     </row>
@@ -5169,7 +5451,7 @@
       <c r="H104" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="I104" s="2" t="s">
+      <c r="I104" s="6" t="s">
         <v>251</v>
       </c>
     </row>
@@ -5198,7 +5480,7 @@
       <c r="H105" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="I105" s="2" t="s">
+      <c r="I105" s="6" t="s">
         <v>251</v>
       </c>
     </row>
@@ -5227,7 +5509,7 @@
       <c r="H106" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="I106" s="2" t="s">
+      <c r="I106" s="6" t="s">
         <v>251</v>
       </c>
     </row>
@@ -5256,7 +5538,7 @@
       <c r="H107" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="I107" s="2" t="s">
+      <c r="I107" s="6" t="s">
         <v>251</v>
       </c>
     </row>
@@ -5285,7 +5567,7 @@
       <c r="H108" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="I108" s="2" t="s">
+      <c r="I108" s="6" t="s">
         <v>251</v>
       </c>
     </row>
@@ -5314,7 +5596,7 @@
       <c r="H109" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="I109" s="2" t="s">
+      <c r="I109" s="6" t="s">
         <v>251</v>
       </c>
     </row>
@@ -5343,7 +5625,7 @@
       <c r="H110" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="I110" s="2" t="s">
+      <c r="I110" s="6" t="s">
         <v>251</v>
       </c>
     </row>
@@ -5372,7 +5654,7 @@
       <c r="H111" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I111" s="2" t="s">
+      <c r="I111" s="6" t="s">
         <v>191</v>
       </c>
     </row>
@@ -5401,7 +5683,7 @@
       <c r="H112" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="I112" s="2" t="s">
+      <c r="I112" s="6" t="s">
         <v>192</v>
       </c>
     </row>
@@ -5430,7 +5712,7 @@
       <c r="H113" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="I113" s="2" t="s">
+      <c r="I113" s="6" t="s">
         <v>193</v>
       </c>
     </row>
@@ -5459,7 +5741,7 @@
       <c r="H114" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="I114" s="2" t="s">
+      <c r="I114" s="6" t="s">
         <v>192</v>
       </c>
     </row>
@@ -5488,7 +5770,7 @@
       <c r="H115" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="I115" s="2" t="s">
+      <c r="I115" s="6" t="s">
         <v>194</v>
       </c>
     </row>
@@ -5517,7 +5799,7 @@
       <c r="H116" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="I116" s="2" t="s">
+      <c r="I116" s="6" t="s">
         <v>195</v>
       </c>
     </row>
@@ -5546,7 +5828,7 @@
       <c r="H117" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="I117" s="2" t="s">
+      <c r="I117" s="6" t="s">
         <v>196</v>
       </c>
     </row>
@@ -5575,12 +5857,13 @@
       <c r="H118" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="I118" s="2" t="s">
+      <c r="I118" s="6" t="s">
         <v>197</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Removed duplicate profiles of war machines
</commit_message>
<xml_diff>
--- a/resources/db/Profiles.xlsx
+++ b/resources/db/Profiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\projects\ArmyBuilder\sourcecode\resources\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272E107B-E8FC-4726-A32D-9EFB475B9A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A6B4DC-E1D6-4E37-B3FA-D2D4DAB08833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{72821A2A-92BA-4C26-854D-A2ECB76DE865}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1388" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1388" uniqueCount="529">
   <si>
     <t>General</t>
   </si>
@@ -1599,12 +1599,6 @@
     <t>25</t>
   </si>
   <si>
-    <t>74</t>
-  </si>
-  <si>
-    <t>104</t>
-  </si>
-  <si>
     <t>54</t>
   </si>
   <si>
@@ -1630,6 +1624,9 @@
   </si>
   <si>
     <t>122</t>
+  </si>
+  <si>
+    <t>80</t>
   </si>
 </sst>
 </file>
@@ -2030,8 +2027,8 @@
   <dimension ref="A1:J118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J40" sqref="J40"/>
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G85" sqref="G85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -2231,10 +2228,10 @@
         <v>11423</v>
       </c>
       <c r="H6" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="0"/>
@@ -2264,10 +2261,10 @@
         <v>11424</v>
       </c>
       <c r="H7" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" si="0"/>
@@ -3356,7 +3353,7 @@
         <v>470</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="J40" t="str">
         <f t="shared" si="0"/>
@@ -4835,17 +4832,17 @@
         <v>426</v>
       </c>
       <c r="G85">
-        <v>12119</v>
+        <v>12133</v>
       </c>
       <c r="H85" t="s">
         <v>174</v>
       </c>
       <c r="I85" s="5" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="J85" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = 'Kleine Steinschleuder', points = 74 WHERE id =12119;</v>
+        <v>UPDATE profile SET name = 'Kleine Steinschleuder', points = 50 WHERE id =12133;</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -4901,17 +4898,17 @@
         <v>428</v>
       </c>
       <c r="G87">
-        <v>12120</v>
+        <v>12134</v>
       </c>
       <c r="H87" t="s">
         <v>176</v>
       </c>
       <c r="I87" s="5" t="s">
-        <v>520</v>
+        <v>528</v>
       </c>
       <c r="J87" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = 'Große Steinschleuder', points = 104 WHERE id =12120;</v>
+        <v>UPDATE profile SET name = 'Große Steinschleuder', points = 80 WHERE id =12134;</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -4973,7 +4970,7 @@
         <v>53</v>
       </c>
       <c r="I89" s="5" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="J89" t="str">
         <f t="shared" si="1"/>
@@ -5102,10 +5099,10 @@
         <v>12123</v>
       </c>
       <c r="H93" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="I93" s="5" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="J93" t="str">
         <f t="shared" si="1"/>
@@ -5204,7 +5201,7 @@
         <v>56</v>
       </c>
       <c r="I96" s="5" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="J96" t="str">
         <f t="shared" si="1"/>
@@ -5303,7 +5300,7 @@
         <v>56</v>
       </c>
       <c r="I99" s="5" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="J99" t="str">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Updated profile points of special character models
</commit_message>
<xml_diff>
--- a/resources/db/Profiles.xlsx
+++ b/resources/db/Profiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\projects\ArmyBuilder\sourcecode\resources\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F903CF-D55B-4AAA-BE03-D16570B9D3B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65CB6B57-7E01-4AEB-AEA6-18DF509218BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{72821A2A-92BA-4C26-854D-A2ECB76DE865}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1388" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="540">
   <si>
     <t>General</t>
   </si>
@@ -1458,9 +1458,6 @@
     <t>Orks Grom der Fettsack vom Nebelberg</t>
   </si>
   <si>
-    <t>Orks Gorbad Eisenfause</t>
-  </si>
-  <si>
     <t>Orks Skarsnik Herrscher der Acht Gipfel</t>
   </si>
   <si>
@@ -1527,9 +1524,6 @@
     <t>Orks Riesenwolf</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>Orks Goblin Basis</t>
   </si>
   <si>
@@ -1548,82 +1542,124 @@
     <t>Orks Schwarzork Basis</t>
   </si>
   <si>
-    <t>8</t>
-  </si>
-  <si>
     <t>Orks Nachtgoblin Basis</t>
   </si>
   <si>
     <t>Orks Höhlensquig</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
     <t>Orks Fanatic</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>Orks Riese</t>
   </si>
   <si>
-    <t>200</t>
-  </si>
-  <si>
     <t>Orks Oger</t>
   </si>
   <si>
-    <t>40</t>
-  </si>
-  <si>
     <t>Orks Flußtroll</t>
   </si>
   <si>
     <t>Orks Steintroll</t>
   </si>
   <si>
-    <t>65</t>
-  </si>
-  <si>
     <t>Orks Snotling-Base</t>
   </si>
   <si>
-    <t>15</t>
-  </si>
-  <si>
     <t>Orks Kurbelwagen</t>
   </si>
   <si>
-    <t>25</t>
-  </si>
-  <si>
     <t>Orks Kamikaze Katapult</t>
   </si>
   <si>
     <t>97.5</t>
   </si>
   <si>
-    <t>50</t>
-  </si>
-  <si>
     <t>Orks Morglum Knochenbrecher</t>
   </si>
   <si>
-    <t>150</t>
-  </si>
-  <si>
     <t>Orks Oglock der Fürchtaliche</t>
   </si>
   <si>
-    <t>90</t>
-  </si>
-  <si>
-    <t>122</t>
-  </si>
-  <si>
-    <t>80</t>
+    <t>65.0</t>
+  </si>
+  <si>
+    <t>4.0</t>
+  </si>
+  <si>
+    <t>110.0</t>
+  </si>
+  <si>
+    <t>140.0</t>
+  </si>
+  <si>
+    <t>83.0</t>
+  </si>
+  <si>
+    <t>91.0</t>
+  </si>
+  <si>
+    <t>72.0</t>
+  </si>
+  <si>
+    <t>33.0</t>
+  </si>
+  <si>
+    <t>42.0</t>
+  </si>
+  <si>
+    <t>15.0</t>
+  </si>
+  <si>
+    <t>56.0</t>
+  </si>
+  <si>
+    <t>28.0</t>
+  </si>
+  <si>
+    <t>118.0</t>
+  </si>
+  <si>
+    <t>122.0</t>
+  </si>
+  <si>
+    <t>190.0</t>
+  </si>
+  <si>
+    <t>159.0</t>
+  </si>
+  <si>
+    <t>287.0</t>
+  </si>
+  <si>
+    <t>303.0</t>
+  </si>
+  <si>
+    <t>253.0</t>
+  </si>
+  <si>
+    <t>20.0</t>
+  </si>
+  <si>
+    <t>25.0</t>
+  </si>
+  <si>
+    <t>127</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>147</t>
+  </si>
+  <si>
+    <t>Orks Gorbad Eisenfaust</t>
   </si>
 </sst>
 </file>
@@ -2025,7 +2061,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G99" sqref="G99"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -2095,12 +2131,12 @@
       <c r="H2" t="s">
         <v>471</v>
       </c>
-      <c r="I2" s="5">
-        <v>80</v>
+      <c r="I2" s="5" t="s">
+        <v>536</v>
       </c>
       <c r="J2" t="str">
         <f t="shared" ref="J2:J65" si="0">CONCATENATE("UPDATE profile SET name = '",H2,"', points = ",I2," WHERE id =",G2,";")</f>
-        <v>UPDATE profile SET name = 'Orks Grom der Fettsack vom Nebelberg', points = 80 WHERE id =11421;</v>
+        <v>UPDATE profile SET name = 'Orks Grom der Fettsack vom Nebelberg', points = 78 WHERE id =11421;</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -2128,12 +2164,12 @@
       <c r="H3" t="s">
         <v>438</v>
       </c>
-      <c r="I3" s="5">
-        <v>65</v>
+      <c r="I3" s="5" t="s">
+        <v>513</v>
       </c>
       <c r="J3" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Niblit', points = 65 WHERE id =11791;</v>
+        <v>UPDATE profile SET name = 'Orks Niblit', points = 65.0 WHERE id =11791;</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2159,14 +2195,14 @@
         <v>11841</v>
       </c>
       <c r="H4" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>495</v>
+        <v>514</v>
       </c>
       <c r="J4" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Riesenwolf', points = 4 WHERE id =11841;</v>
+        <v>UPDATE profile SET name = 'Orks Riesenwolf', points = 4.0 WHERE id =11841;</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -2192,14 +2228,14 @@
         <v>11422</v>
       </c>
       <c r="H5" t="s">
-        <v>472</v>
-      </c>
-      <c r="I5" s="5">
-        <v>120</v>
+        <v>539</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>537</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Gorbad Eisenfause', points = 120 WHERE id =11422;</v>
+        <v>UPDATE profile SET name = 'Orks Gorbad Eisenfaust', points = 110 WHERE id =11422;</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -2225,14 +2261,14 @@
         <v>11423</v>
       </c>
       <c r="H6" t="s">
-        <v>522</v>
+        <v>511</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>523</v>
+        <v>538</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Morglum Knochenbrecher', points = 150 WHERE id =11423;</v>
+        <v>UPDATE profile SET name = 'Orks Morglum Knochenbrecher', points = 147 WHERE id =11423;</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -2258,14 +2294,14 @@
         <v>11424</v>
       </c>
       <c r="H7" t="s">
-        <v>524</v>
+        <v>512</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>525</v>
+        <v>535</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Oglock der Fürchtaliche', points = 90 WHERE id =11424;</v>
+        <v>UPDATE profile SET name = 'Orks Oglock der Fürchtaliche', points = 87 WHERE id =11424;</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -2291,14 +2327,14 @@
         <v>11425</v>
       </c>
       <c r="H8" t="s">
-        <v>473</v>
-      </c>
-      <c r="I8" s="5">
-        <v>80</v>
+        <v>472</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>536</v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Skarsnik Herrscher der Acht Gipfel', points = 80 WHERE id =11425;</v>
+        <v>UPDATE profile SET name = 'Orks Skarsnik Herrscher der Acht Gipfel', points = 78 WHERE id =11425;</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2326,12 +2362,12 @@
       <c r="H9" t="s">
         <v>439</v>
       </c>
-      <c r="I9" s="5">
-        <v>50</v>
+      <c r="I9" s="5" t="s">
+        <v>246</v>
       </c>
       <c r="J9" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Gobbla', points = 50 WHERE id =11792;</v>
+        <v>UPDATE profile SET name = 'Orks Gobbla', points = 50.0 WHERE id =11792;</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -2359,12 +2395,12 @@
       <c r="H10" t="s">
         <v>440</v>
       </c>
-      <c r="I10" s="5">
-        <v>110</v>
+      <c r="I10" s="5" t="s">
+        <v>515</v>
       </c>
       <c r="J10" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Ork Chefoberboss', points = 110 WHERE id =11426;</v>
+        <v>UPDATE profile SET name = 'Orks Ork Chefoberboss', points = 110.0 WHERE id =11426;</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2392,12 +2428,12 @@
       <c r="H11" t="s">
         <v>441</v>
       </c>
-      <c r="I11" s="5">
-        <v>140</v>
+      <c r="I11" s="5" t="s">
+        <v>516</v>
       </c>
       <c r="J11" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Schwarzork Chefoberboss', points = 140 WHERE id =11427;</v>
+        <v>UPDATE profile SET name = 'Orks Schwarzork Chefoberboss', points = 140.0 WHERE id =11427;</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -2425,12 +2461,12 @@
       <c r="H12" t="s">
         <v>442</v>
       </c>
-      <c r="I12" s="5">
-        <v>150</v>
+      <c r="I12" s="5" t="s">
+        <v>192</v>
       </c>
       <c r="J12" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Wildork Chefoberboss', points = 150 WHERE id =11428;</v>
+        <v>UPDATE profile SET name = 'Orks Wildork Chefoberboss', points = 150.0 WHERE id =11428;</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -2458,12 +2494,12 @@
       <c r="H13" t="s">
         <v>443</v>
       </c>
-      <c r="I13" s="5">
-        <v>50</v>
+      <c r="I13" s="5" t="s">
+        <v>246</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Goblin Chefoberboss', points = 50 WHERE id =11429;</v>
+        <v>UPDATE profile SET name = 'Orks Goblin Chefoberboss', points = 50.0 WHERE id =11429;</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -2491,12 +2527,12 @@
       <c r="H14" t="s">
         <v>444</v>
       </c>
-      <c r="I14" s="5">
-        <v>50</v>
+      <c r="I14" s="5" t="s">
+        <v>246</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Waldgoblin Chefoberboss', points = 50 WHERE id =11430;</v>
+        <v>UPDATE profile SET name = 'Orks Waldgoblin Chefoberboss', points = 50.0 WHERE id =11430;</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -2524,12 +2560,12 @@
       <c r="H15" t="s">
         <v>445</v>
       </c>
-      <c r="I15" s="5">
-        <v>50</v>
+      <c r="I15" s="5" t="s">
+        <v>246</v>
       </c>
       <c r="J15" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Nachtgoblin Chefoberboss', points = 50 WHERE id =11431;</v>
+        <v>UPDATE profile SET name = 'Orks Nachtgoblin Chefoberboss', points = 50.0 WHERE id =11431;</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -2557,12 +2593,12 @@
       <c r="H16" t="s">
         <v>446</v>
       </c>
-      <c r="I16" s="5">
-        <v>92</v>
+      <c r="I16" s="5" t="s">
+        <v>244</v>
       </c>
       <c r="J16" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Schwarzork Armeestandarte', points = 92 WHERE id =11432;</v>
+        <v>UPDATE profile SET name = 'Orks Schwarzork Armeestandarte', points = 92.0 WHERE id =11432;</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -2590,12 +2626,12 @@
       <c r="H17" t="s">
         <v>447</v>
       </c>
-      <c r="I17" s="5">
-        <v>83</v>
+      <c r="I17" s="5" t="s">
+        <v>517</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Ork Armeestandarte', points = 83 WHERE id =11433;</v>
+        <v>UPDATE profile SET name = 'Orks Ork Armeestandarte', points = 83.0 WHERE id =11433;</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -2623,12 +2659,12 @@
       <c r="H18" t="s">
         <v>448</v>
       </c>
-      <c r="I18" s="5">
-        <v>95</v>
+      <c r="I18" s="5" t="s">
+        <v>248</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Wildork Armeestandarte', points = 95 WHERE id =11434;</v>
+        <v>UPDATE profile SET name = 'Orks Wildork Armeestandarte', points = 95.0 WHERE id =11434;</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -2656,12 +2692,12 @@
       <c r="H19" t="s">
         <v>449</v>
       </c>
-      <c r="I19" s="5">
-        <v>65</v>
+      <c r="I19" s="5" t="s">
+        <v>513</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Goblin Armeestandarte', points = 65 WHERE id =11435;</v>
+        <v>UPDATE profile SET name = 'Orks Goblin Armeestandarte', points = 65.0 WHERE id =11435;</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -2689,12 +2725,12 @@
       <c r="H20" t="s">
         <v>450</v>
       </c>
-      <c r="I20" s="5">
-        <v>65</v>
+      <c r="I20" s="5" t="s">
+        <v>513</v>
       </c>
       <c r="J20" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Waldgoblin Armeestandarte', points = 65 WHERE id =11436;</v>
+        <v>UPDATE profile SET name = 'Orks Waldgoblin Armeestandarte', points = 65.0 WHERE id =11436;</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -2722,12 +2758,12 @@
       <c r="H21" t="s">
         <v>451</v>
       </c>
-      <c r="I21" s="5">
-        <v>65</v>
+      <c r="I21" s="5" t="s">
+        <v>513</v>
       </c>
       <c r="J21" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Nachtgoblin Armeestandarte', points = 65 WHERE id =11437;</v>
+        <v>UPDATE profile SET name = 'Orks Nachtgoblin Armeestandarte', points = 65.0 WHERE id =11437;</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -2755,12 +2791,12 @@
       <c r="H22" t="s">
         <v>452</v>
       </c>
-      <c r="I22" s="5">
-        <v>91</v>
+      <c r="I22" s="5" t="s">
+        <v>518</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Schwarzork Oberboss', points = 91 WHERE id =11438;</v>
+        <v>UPDATE profile SET name = 'Orks Schwarzork Oberboss', points = 91.0 WHERE id =11438;</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -2788,12 +2824,12 @@
       <c r="H23" t="s">
         <v>453</v>
       </c>
-      <c r="I23" s="5">
-        <v>72</v>
+      <c r="I23" s="5" t="s">
+        <v>519</v>
       </c>
       <c r="J23" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Ork Oberboss', points = 72 WHERE id =11439;</v>
+        <v>UPDATE profile SET name = 'Orks Ork Oberboss', points = 72.0 WHERE id =11439;</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -2821,12 +2857,12 @@
       <c r="H24" t="s">
         <v>454</v>
       </c>
-      <c r="I24" s="5">
-        <v>98</v>
+      <c r="I24" s="5" t="s">
+        <v>235</v>
       </c>
       <c r="J24" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Wildork Oberboss', points = 98 WHERE id =11440;</v>
+        <v>UPDATE profile SET name = 'Orks Wildork Oberboss', points = 98.0 WHERE id =11440;</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -2854,12 +2890,12 @@
       <c r="H25" t="s">
         <v>455</v>
       </c>
-      <c r="I25" s="5">
-        <v>33</v>
+      <c r="I25" s="5" t="s">
+        <v>520</v>
       </c>
       <c r="J25" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Goblin Oberboss', points = 33 WHERE id =11441;</v>
+        <v>UPDATE profile SET name = 'Orks Goblin Oberboss', points = 33.0 WHERE id =11441;</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -2887,12 +2923,12 @@
       <c r="H26" t="s">
         <v>456</v>
       </c>
-      <c r="I26" s="5">
-        <v>33</v>
+      <c r="I26" s="5" t="s">
+        <v>520</v>
       </c>
       <c r="J26" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Waldgoblin Oberboss', points = 33 WHERE id =11442;</v>
+        <v>UPDATE profile SET name = 'Orks Waldgoblin Oberboss', points = 33.0 WHERE id =11442;</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -2920,12 +2956,12 @@
       <c r="H27" t="s">
         <v>457</v>
       </c>
-      <c r="I27" s="5">
-        <v>33</v>
+      <c r="I27" s="5" t="s">
+        <v>520</v>
       </c>
       <c r="J27" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Nachtgoblin Oberboss', points = 33 WHERE id =11443;</v>
+        <v>UPDATE profile SET name = 'Orks Nachtgoblin Oberboss', points = 33.0 WHERE id =11443;</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -2953,12 +2989,12 @@
       <c r="H28" t="s">
         <v>458</v>
       </c>
-      <c r="I28" s="5">
-        <v>42</v>
+      <c r="I28" s="5" t="s">
+        <v>521</v>
       </c>
       <c r="J28" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Schwarzork Boss', points = 42 WHERE id =11444;</v>
+        <v>UPDATE profile SET name = 'Orks Schwarzork Boss', points = 42.0 WHERE id =11444;</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -2986,12 +3022,12 @@
       <c r="H29" t="s">
         <v>459</v>
       </c>
-      <c r="I29" s="5">
-        <v>33</v>
+      <c r="I29" s="5" t="s">
+        <v>520</v>
       </c>
       <c r="J29" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Ork Boss', points = 33 WHERE id =11445;</v>
+        <v>UPDATE profile SET name = 'Orks Ork Boss', points = 33.0 WHERE id =11445;</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -3019,12 +3055,12 @@
       <c r="H30" t="s">
         <v>460</v>
       </c>
-      <c r="I30" s="5">
-        <v>33</v>
+      <c r="I30" s="5" t="s">
+        <v>520</v>
       </c>
       <c r="J30" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Wildork Boss', points = 33 WHERE id =11446;</v>
+        <v>UPDATE profile SET name = 'Orks Wildork Boss', points = 33.0 WHERE id =11446;</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -3052,12 +3088,12 @@
       <c r="H31" t="s">
         <v>461</v>
       </c>
-      <c r="I31" s="5">
-        <v>15</v>
+      <c r="I31" s="5" t="s">
+        <v>522</v>
       </c>
       <c r="J31" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Goblin Boss', points = 15 WHERE id =11447;</v>
+        <v>UPDATE profile SET name = 'Orks Goblin Boss', points = 15.0 WHERE id =11447;</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -3085,12 +3121,12 @@
       <c r="H32" t="s">
         <v>462</v>
       </c>
-      <c r="I32" s="5">
-        <v>15</v>
+      <c r="I32" s="5" t="s">
+        <v>522</v>
       </c>
       <c r="J32" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Waldgoblin Boss', points = 15 WHERE id =11448;</v>
+        <v>UPDATE profile SET name = 'Orks Waldgoblin Boss', points = 15.0 WHERE id =11448;</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -3118,12 +3154,12 @@
       <c r="H33" t="s">
         <v>463</v>
       </c>
-      <c r="I33" s="5">
-        <v>15</v>
+      <c r="I33" s="5" t="s">
+        <v>522</v>
       </c>
       <c r="J33" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Nachtgoblin Boss', points = 15 WHERE id =11449;</v>
+        <v>UPDATE profile SET name = 'Orks Nachtgoblin Boss', points = 15.0 WHERE id =11449;</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -3151,12 +3187,12 @@
       <c r="H34" t="s">
         <v>464</v>
       </c>
-      <c r="I34" s="5">
-        <v>56</v>
+      <c r="I34" s="5" t="s">
+        <v>523</v>
       </c>
       <c r="J34" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Ork Schamane', points = 56 WHERE id =11450;</v>
+        <v>UPDATE profile SET name = 'Orks Ork Schamane', points = 56.0 WHERE id =11450;</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -3184,12 +3220,12 @@
       <c r="H35" t="s">
         <v>465</v>
       </c>
-      <c r="I35" s="5">
-        <v>59</v>
+      <c r="I35" s="5" t="s">
+        <v>261</v>
       </c>
       <c r="J35" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Wildork Schamane', points = 59 WHERE id =11451;</v>
+        <v>UPDATE profile SET name = 'Orks Wildork Schamane', points = 59.0 WHERE id =11451;</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -3217,12 +3253,12 @@
       <c r="H36" t="s">
         <v>466</v>
       </c>
-      <c r="I36" s="5">
-        <v>28</v>
+      <c r="I36" s="5" t="s">
+        <v>524</v>
       </c>
       <c r="J36" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Goblin Schamane', points = 28 WHERE id =11452;</v>
+        <v>UPDATE profile SET name = 'Orks Goblin Schamane', points = 28.0 WHERE id =11452;</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -3250,12 +3286,12 @@
       <c r="H37" t="s">
         <v>467</v>
       </c>
-      <c r="I37" s="5">
-        <v>28</v>
+      <c r="I37" s="5" t="s">
+        <v>524</v>
       </c>
       <c r="J37" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Nachtgoblin Schamane', points = 28 WHERE id =11453;</v>
+        <v>UPDATE profile SET name = 'Orks Nachtgoblin Schamane', points = 28.0 WHERE id =11453;</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -3283,12 +3319,12 @@
       <c r="H38" t="s">
         <v>468</v>
       </c>
-      <c r="I38" s="5">
-        <v>28</v>
+      <c r="I38" s="5" t="s">
+        <v>524</v>
       </c>
       <c r="J38" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Waldgoblin Schamane', points = 28 WHERE id =11454;</v>
+        <v>UPDATE profile SET name = 'Orks Waldgoblin Schamane', points = 28.0 WHERE id =11454;</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -3316,12 +3352,12 @@
       <c r="H39" t="s">
         <v>469</v>
       </c>
-      <c r="I39" s="5">
-        <v>118</v>
+      <c r="I39" s="5" t="s">
+        <v>525</v>
       </c>
       <c r="J39" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Ork Oberschamane', points = 118 WHERE id =11455;</v>
+        <v>UPDATE profile SET name = 'Orks Ork Oberschamane', points = 118.0 WHERE id =11455;</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -3354,7 +3390,7 @@
       </c>
       <c r="J40" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Wildork Oberschamane', points = 122 WHERE id =11456;</v>
+        <v>UPDATE profile SET name = 'Orks Wildork Oberschamane', points = 122.0 WHERE id =11456;</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -3380,14 +3416,14 @@
         <v>11457</v>
       </c>
       <c r="H41" t="s">
-        <v>474</v>
-      </c>
-      <c r="I41" s="5">
-        <v>83</v>
+        <v>473</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>517</v>
       </c>
       <c r="J41" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Goblin Oberschamane', points = 83 WHERE id =11457;</v>
+        <v>UPDATE profile SET name = 'Orks Goblin Oberschamane', points = 83.0 WHERE id =11457;</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -3413,14 +3449,14 @@
         <v>11458</v>
       </c>
       <c r="H42" t="s">
-        <v>475</v>
-      </c>
-      <c r="I42" s="5">
-        <v>83</v>
+        <v>474</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>517</v>
       </c>
       <c r="J42" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Nachtgoblin Oberschamane', points = 83 WHERE id =11458;</v>
+        <v>UPDATE profile SET name = 'Orks Nachtgoblin Oberschamane', points = 83.0 WHERE id =11458;</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -3446,14 +3482,14 @@
         <v>11459</v>
       </c>
       <c r="H43" t="s">
-        <v>476</v>
-      </c>
-      <c r="I43" s="5">
-        <v>83</v>
+        <v>475</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>517</v>
       </c>
       <c r="J43" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Waldgoblin Oberschamane', points = 83 WHERE id =11459;</v>
+        <v>UPDATE profile SET name = 'Orks Waldgoblin Oberschamane', points = 83.0 WHERE id =11459;</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -3479,14 +3515,14 @@
         <v>11460</v>
       </c>
       <c r="H44" t="s">
-        <v>477</v>
-      </c>
-      <c r="I44" s="5">
-        <v>190</v>
+        <v>476</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>527</v>
       </c>
       <c r="J44" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Ork Großschamane', points = 190 WHERE id =11460;</v>
+        <v>UPDATE profile SET name = 'Orks Ork Großschamane', points = 190.0 WHERE id =11460;</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -3512,14 +3548,14 @@
         <v>11461</v>
       </c>
       <c r="H45" t="s">
-        <v>478</v>
-      </c>
-      <c r="I45" s="5">
-        <v>219</v>
+        <v>477</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>262</v>
       </c>
       <c r="J45" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Wildork Großschamane', points = 219 WHERE id =11461;</v>
+        <v>UPDATE profile SET name = 'Orks Wildork Großschamane', points = 219.0 WHERE id =11461;</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -3545,14 +3581,14 @@
         <v>11462</v>
       </c>
       <c r="H46" t="s">
-        <v>479</v>
-      </c>
-      <c r="I46" s="5">
-        <v>159</v>
+        <v>478</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>528</v>
       </c>
       <c r="J46" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Goblin Großschamane', points = 159 WHERE id =11462;</v>
+        <v>UPDATE profile SET name = 'Orks Goblin Großschamane', points = 159.0 WHERE id =11462;</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -3578,14 +3614,14 @@
         <v>11463</v>
       </c>
       <c r="H47" t="s">
-        <v>480</v>
-      </c>
-      <c r="I47" s="5">
-        <v>159</v>
+        <v>479</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>528</v>
       </c>
       <c r="J47" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Nachtgoblin Großschamane', points = 159 WHERE id =11463;</v>
+        <v>UPDATE profile SET name = 'Orks Nachtgoblin Großschamane', points = 159.0 WHERE id =11463;</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -3611,14 +3647,14 @@
         <v>11464</v>
       </c>
       <c r="H48" t="s">
-        <v>481</v>
-      </c>
-      <c r="I48" s="5">
-        <v>159</v>
+        <v>480</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>528</v>
       </c>
       <c r="J48" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Waldgoblin Großschamane', points = 159 WHERE id =11464;</v>
+        <v>UPDATE profile SET name = 'Orks Waldgoblin Großschamane', points = 159.0 WHERE id =11464;</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -3644,14 +3680,14 @@
         <v>11465</v>
       </c>
       <c r="H49" t="s">
-        <v>482</v>
-      </c>
-      <c r="I49" s="5">
-        <v>287</v>
+        <v>481</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>529</v>
       </c>
       <c r="J49" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Ork Meisterschamane', points = 287 WHERE id =11465;</v>
+        <v>UPDATE profile SET name = 'Orks Ork Meisterschamane', points = 287.0 WHERE id =11465;</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -3677,14 +3713,14 @@
         <v>11466</v>
       </c>
       <c r="H50" t="s">
-        <v>483</v>
-      </c>
-      <c r="I50" s="5">
-        <v>303</v>
+        <v>482</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>530</v>
       </c>
       <c r="J50" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Wildork Meisterschamane', points = 303 WHERE id =11466;</v>
+        <v>UPDATE profile SET name = 'Orks Wildork Meisterschamane', points = 303.0 WHERE id =11466;</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -3710,14 +3746,14 @@
         <v>11467</v>
       </c>
       <c r="H51" t="s">
-        <v>484</v>
-      </c>
-      <c r="I51" s="5">
-        <v>253</v>
+        <v>483</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>531</v>
       </c>
       <c r="J51" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Goblin Meisterschamane', points = 253 WHERE id =11467;</v>
+        <v>UPDATE profile SET name = 'Orks Goblin Meisterschamane', points = 253.0 WHERE id =11467;</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -3743,14 +3779,14 @@
         <v>11468</v>
       </c>
       <c r="H52" t="s">
-        <v>485</v>
-      </c>
-      <c r="I52" s="5">
-        <v>253</v>
+        <v>484</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>531</v>
       </c>
       <c r="J52" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Nachtgoblin Meisterschamane', points = 253 WHERE id =11468;</v>
+        <v>UPDATE profile SET name = 'Orks Nachtgoblin Meisterschamane', points = 253.0 WHERE id =11468;</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -3776,14 +3812,14 @@
         <v>11469</v>
       </c>
       <c r="H53" t="s">
-        <v>486</v>
-      </c>
-      <c r="I53" s="5">
-        <v>253</v>
+        <v>485</v>
+      </c>
+      <c r="I53" s="5" t="s">
+        <v>531</v>
       </c>
       <c r="J53" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Waldgoblin Meisterschamane', points = 253 WHERE id =11469;</v>
+        <v>UPDATE profile SET name = 'Orks Waldgoblin Meisterschamane', points = 253.0 WHERE id =11469;</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -3809,14 +3845,14 @@
         <v>11586</v>
       </c>
       <c r="H54" t="s">
-        <v>487</v>
-      </c>
-      <c r="I54" s="5">
-        <v>90</v>
+        <v>486</v>
+      </c>
+      <c r="I54" s="5" t="s">
+        <v>535</v>
       </c>
       <c r="J54" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Gorfan Rotzahn', points = 90 WHERE id =11586;</v>
+        <v>UPDATE profile SET name = 'Orks Gorfan Rotzahn', points = 87 WHERE id =11586;</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -3842,14 +3878,14 @@
         <v>11643</v>
       </c>
       <c r="H55" t="s">
-        <v>488</v>
-      </c>
-      <c r="I55" s="5">
-        <v>130</v>
+        <v>487</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>534</v>
       </c>
       <c r="J55" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Azhag der Vernichter', points = 130 WHERE id =11643;</v>
+        <v>UPDATE profile SET name = 'Orks Azhag der Vernichter', points = 127 WHERE id =11643;</v>
       </c>
     </row>
     <row r="56" spans="1:10" s="2" customFormat="1">
@@ -3877,12 +3913,12 @@
       <c r="H56" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="I56" s="6">
-        <v>180</v>
+      <c r="I56" s="6" t="s">
+        <v>250</v>
       </c>
       <c r="J56" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Lindwurm', points = 180 WHERE id =12423;</v>
+        <v>UPDATE profile SET name = 'Lindwurm', points = 180.0 WHERE id =12423;</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -3908,10 +3944,10 @@
         <v>11850</v>
       </c>
       <c r="H57" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J57" t="str">
         <f t="shared" si="0"/>
@@ -3941,14 +3977,14 @@
         <v>12023</v>
       </c>
       <c r="H58" t="s">
-        <v>490</v>
-      </c>
-      <c r="I58" s="5">
-        <v>8</v>
+        <v>489</v>
+      </c>
+      <c r="I58" s="5" t="s">
+        <v>492</v>
       </c>
       <c r="J58" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Wildschwein', points = 8 WHERE id =12023;</v>
+        <v>UPDATE profile SET name = 'Orks Wildschwein', points = 5.5 WHERE id =12023;</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -3974,10 +4010,10 @@
         <v>11851</v>
       </c>
       <c r="H59" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="J59" t="str">
         <f t="shared" si="0"/>
@@ -4007,10 +4043,10 @@
         <v>12023</v>
       </c>
       <c r="H60" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="J60" t="str">
         <f t="shared" si="0"/>
@@ -4040,14 +4076,14 @@
         <v>11841</v>
       </c>
       <c r="H61" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>495</v>
+        <v>514</v>
       </c>
       <c r="J61" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Riesenwolf', points = 4 WHERE id =11841;</v>
+        <v>UPDATE profile SET name = 'Orks Riesenwolf', points = 4.0 WHERE id =11841;</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -4073,10 +4109,10 @@
         <v>11852</v>
       </c>
       <c r="H62" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I62" s="5" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="J62" t="str">
         <f t="shared" si="0"/>
@@ -4106,10 +4142,10 @@
         <v>11853</v>
       </c>
       <c r="H63" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="I63" s="5" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="J63" t="str">
         <f t="shared" si="0"/>
@@ -4139,10 +4175,10 @@
         <v>12026</v>
       </c>
       <c r="H64" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I64" s="5" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J64" t="str">
         <f t="shared" si="0"/>
@@ -4172,10 +4208,10 @@
         <v>11854</v>
       </c>
       <c r="H65" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="I65" s="5" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J65" t="str">
         <f t="shared" si="0"/>
@@ -4205,10 +4241,10 @@
         <v>11855</v>
       </c>
       <c r="H66" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I66" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="J66" t="str">
         <f t="shared" ref="J66:J99" si="1">CONCATENATE("UPDATE profile SET name = '",H66,"', points = ",I66," WHERE id =",G66,";")</f>
@@ -4238,10 +4274,10 @@
         <v>11856</v>
       </c>
       <c r="H67" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I67" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="J67" t="str">
         <f t="shared" si="1"/>
@@ -4271,14 +4307,14 @@
         <v>11857</v>
       </c>
       <c r="H68" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="I68" s="5" t="s">
-        <v>502</v>
+        <v>243</v>
       </c>
       <c r="J68" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = 'Orks Schwarzork Basis', points = 8 WHERE id =11857;</v>
+        <v>UPDATE profile SET name = 'Orks Schwarzork Basis', points = 8.0 WHERE id =11857;</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -4304,10 +4340,10 @@
         <v>11858</v>
       </c>
       <c r="H69" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="I69" s="5" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J69" t="str">
         <f t="shared" si="1"/>
@@ -4337,10 +4373,10 @@
         <v>11852</v>
       </c>
       <c r="H70" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I70" s="5" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="J70" t="str">
         <f t="shared" si="1"/>
@@ -4370,10 +4406,10 @@
         <v>11853</v>
       </c>
       <c r="H71" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="I71" s="5" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="J71" t="str">
         <f t="shared" si="1"/>
@@ -4403,10 +4439,10 @@
         <v>11861</v>
       </c>
       <c r="H72" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="I72" s="5" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="J72" t="str">
         <f t="shared" si="1"/>
@@ -4436,10 +4472,10 @@
         <v>11862</v>
       </c>
       <c r="H73" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="I73" s="5" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="J73" t="str">
         <f t="shared" si="1"/>
@@ -4469,14 +4505,14 @@
         <v>12027</v>
       </c>
       <c r="H74" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="I74" s="5" t="s">
-        <v>505</v>
+        <v>532</v>
       </c>
       <c r="J74" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = 'Orks Höhlensquig', points = 20 WHERE id =12027;</v>
+        <v>UPDATE profile SET name = 'Orks Höhlensquig', points = 20.0 WHERE id =12027;</v>
       </c>
     </row>
     <row r="75" spans="1:10">
@@ -4502,10 +4538,10 @@
         <v>11863</v>
       </c>
       <c r="H75" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="I75" s="5" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="J75" t="str">
         <f t="shared" si="1"/>
@@ -4535,14 +4571,14 @@
         <v>11864</v>
       </c>
       <c r="H76" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="I76" s="5" t="s">
-        <v>507</v>
+        <v>245</v>
       </c>
       <c r="J76" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = 'Orks Fanatic', points = 30 WHERE id =11864;</v>
+        <v>UPDATE profile SET name = 'Orks Fanatic', points = 30.0 WHERE id =11864;</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -4568,10 +4604,10 @@
         <v>11861</v>
       </c>
       <c r="H77" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="I77" s="5" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="J77" t="str">
         <f t="shared" si="1"/>
@@ -4601,14 +4637,14 @@
         <v>12028</v>
       </c>
       <c r="H78" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="I78" s="5" t="s">
-        <v>505</v>
+        <v>532</v>
       </c>
       <c r="J78" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = 'Orks Höhlensquig', points = 20 WHERE id =12028;</v>
+        <v>UPDATE profile SET name = 'Orks Höhlensquig', points = 20.0 WHERE id =12028;</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -4634,14 +4670,14 @@
         <v>11866</v>
       </c>
       <c r="H79" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="I79" s="5" t="s">
-        <v>509</v>
+        <v>193</v>
       </c>
       <c r="J79" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = 'Orks Riese', points = 200 WHERE id =11866;</v>
+        <v>UPDATE profile SET name = 'Orks Riese', points = 200.0 WHERE id =11866;</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -4667,14 +4703,14 @@
         <v>11867</v>
       </c>
       <c r="H80" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="I80" s="5" t="s">
-        <v>511</v>
+        <v>249</v>
       </c>
       <c r="J80" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = 'Orks Oger', points = 40 WHERE id =11867;</v>
+        <v>UPDATE profile SET name = 'Orks Oger', points = 40.0 WHERE id =11867;</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -4700,14 +4736,14 @@
         <v>11868</v>
       </c>
       <c r="H81" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
       <c r="I81" s="5" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="J81" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = 'Orks Flußtroll', points = 65 WHERE id =11868;</v>
+        <v>UPDATE profile SET name = 'Orks Flußtroll', points = 65.0 WHERE id =11868;</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -4733,14 +4769,14 @@
         <v>11869</v>
       </c>
       <c r="H82" t="s">
+        <v>506</v>
+      </c>
+      <c r="I82" s="5" t="s">
         <v>513</v>
-      </c>
-      <c r="I82" s="5" t="s">
-        <v>514</v>
       </c>
       <c r="J82" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = 'Orks Steintroll', points = 65 WHERE id =11869;</v>
+        <v>UPDATE profile SET name = 'Orks Steintroll', points = 65.0 WHERE id =11869;</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -4766,14 +4802,14 @@
         <v>11870</v>
       </c>
       <c r="H83" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="I83" s="5" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="J83" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = 'Orks Snotling-Base', points = 15 WHERE id =11870;</v>
+        <v>UPDATE profile SET name = 'Orks Snotling-Base', points = 15.0 WHERE id =11870;</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -4799,10 +4835,10 @@
         <v>12071</v>
       </c>
       <c r="H84" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I84" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="J84" t="str">
         <f t="shared" si="1"/>
@@ -4835,11 +4871,11 @@
         <v>174</v>
       </c>
       <c r="I85" s="5" t="s">
-        <v>521</v>
+        <v>246</v>
       </c>
       <c r="J85" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = 'Kleine Steinschleuder', points = 50 WHERE id =12133;</v>
+        <v>UPDATE profile SET name = 'Kleine Steinschleuder', points = 50.0 WHERE id =12133;</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -4865,10 +4901,10 @@
         <v>12071</v>
       </c>
       <c r="H86" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I86" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="J86" t="str">
         <f t="shared" si="1"/>
@@ -4901,11 +4937,11 @@
         <v>176</v>
       </c>
       <c r="I87" s="5" t="s">
-        <v>527</v>
+        <v>247</v>
       </c>
       <c r="J87" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = 'Große Steinschleuder', points = 80 WHERE id =12134;</v>
+        <v>UPDATE profile SET name = 'Große Steinschleuder', points = 80.0 WHERE id =12134;</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -4931,10 +4967,10 @@
         <v>12071</v>
       </c>
       <c r="H88" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I88" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="J88" t="str">
         <f t="shared" si="1"/>
@@ -4967,11 +5003,11 @@
         <v>53</v>
       </c>
       <c r="I89" s="5" t="s">
-        <v>507</v>
+        <v>245</v>
       </c>
       <c r="J89" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = 'Speerschleuder', points = 30 WHERE id =12132;</v>
+        <v>UPDATE profile SET name = 'Speerschleuder', points = 30.0 WHERE id =12132;</v>
       </c>
     </row>
     <row r="90" spans="1:10">
@@ -4997,14 +5033,14 @@
         <v>12074</v>
       </c>
       <c r="H90" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="I90" s="5" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="J90" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = 'Orks Snotling-Base', points = 15 WHERE id =12074;</v>
+        <v>UPDATE profile SET name = 'Orks Snotling-Base', points = 15.0 WHERE id =12074;</v>
       </c>
     </row>
     <row r="91" spans="1:10">
@@ -5030,14 +5066,14 @@
         <v>12122</v>
       </c>
       <c r="H91" t="s">
-        <v>517</v>
+        <v>508</v>
       </c>
       <c r="I91" s="5" t="s">
-        <v>518</v>
+        <v>533</v>
       </c>
       <c r="J91" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = 'Orks Kurbelwagen', points = 25 WHERE id =12122;</v>
+        <v>UPDATE profile SET name = 'Orks Kurbelwagen', points = 25.0 WHERE id =12122;</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -5063,10 +5099,10 @@
         <v>12075</v>
       </c>
       <c r="H92" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I92" s="5" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="J92" t="str">
         <f t="shared" si="1"/>
@@ -5096,10 +5132,10 @@
         <v>12123</v>
       </c>
       <c r="H93" t="s">
-        <v>519</v>
+        <v>509</v>
       </c>
       <c r="I93" s="5" t="s">
-        <v>520</v>
+        <v>510</v>
       </c>
       <c r="J93" t="str">
         <f t="shared" si="1"/>
@@ -5129,10 +5165,10 @@
         <v>12023</v>
       </c>
       <c r="H94" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I94" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="J94" t="str">
         <f t="shared" si="1"/>
@@ -5162,10 +5198,10 @@
         <v>12076</v>
       </c>
       <c r="H95" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I95" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="J95" t="str">
         <f t="shared" si="1"/>
@@ -5198,11 +5234,11 @@
         <v>56</v>
       </c>
       <c r="I96" s="5" t="s">
-        <v>521</v>
+        <v>246</v>
       </c>
       <c r="J96" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = 'Streitwagen', points = 50 WHERE id =12159;</v>
+        <v>UPDATE profile SET name = 'Streitwagen', points = 50.0 WHERE id =12159;</v>
       </c>
     </row>
     <row r="97" spans="1:10">
@@ -5228,14 +5264,14 @@
         <v>11841</v>
       </c>
       <c r="H97" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I97" s="5" t="s">
-        <v>495</v>
+        <v>514</v>
       </c>
       <c r="J97" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = 'Orks Riesenwolf', points = 4 WHERE id =11841;</v>
+        <v>UPDATE profile SET name = 'Orks Riesenwolf', points = 4.0 WHERE id =11841;</v>
       </c>
     </row>
     <row r="98" spans="1:10">
@@ -5261,10 +5297,10 @@
         <v>11852</v>
       </c>
       <c r="H98" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I98" s="5" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="J98" t="str">
         <f t="shared" si="1"/>
@@ -5297,11 +5333,11 @@
         <v>56</v>
       </c>
       <c r="I99" s="5" t="s">
-        <v>521</v>
+        <v>246</v>
       </c>
       <c r="J99" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = 'Streitwagen', points = 50 WHERE id =12159;</v>
+        <v>UPDATE profile SET name = 'Streitwagen', points = 50.0 WHERE id =12159;</v>
       </c>
     </row>
     <row r="100" spans="1:10" s="2" customFormat="1">

</xml_diff>

<commit_message>
Fixed profile points of Wildschwein
</commit_message>
<xml_diff>
--- a/resources/db/Profiles.xlsx
+++ b/resources/db/Profiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\projects\ArmyBuilder\sourcecode\resources\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65CB6B57-7E01-4AEB-AEA6-18DF509218BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D909B958-F106-4D6E-94A1-82B7320D13B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{72821A2A-92BA-4C26-854D-A2ECB76DE865}"/>
   </bookViews>
@@ -20,6 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'High Elf Profiles'!$B$1:$F$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Orcs &amp; Goblins Profiles'!$A$1:$I$118</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="541">
   <si>
     <t>General</t>
   </si>
@@ -1660,6 +1661,9 @@
   </si>
   <si>
     <t>Orks Gorbad Eisenfaust</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
 </sst>
 </file>
@@ -2057,11 +2061,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73F0926A-28CA-48B1-B472-BA874B7E1E5A}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:J118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomLeft" activeCell="I119" sqref="I119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -2106,7 +2111,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" hidden="1">
       <c r="A2">
         <v>9</v>
       </c>
@@ -2139,7 +2144,7 @@
         <v>UPDATE profile SET name = 'Orks Grom der Fettsack vom Nebelberg', points = 78 WHERE id =11421;</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" hidden="1">
       <c r="A3">
         <v>9</v>
       </c>
@@ -2172,7 +2177,7 @@
         <v>UPDATE profile SET name = 'Orks Niblit', points = 65.0 WHERE id =11791;</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" hidden="1">
       <c r="A4">
         <v>9</v>
       </c>
@@ -2205,7 +2210,7 @@
         <v>UPDATE profile SET name = 'Orks Riesenwolf', points = 4.0 WHERE id =11841;</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" hidden="1">
       <c r="A5">
         <v>9</v>
       </c>
@@ -2238,7 +2243,7 @@
         <v>UPDATE profile SET name = 'Orks Gorbad Eisenfaust', points = 110 WHERE id =11422;</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" hidden="1">
       <c r="A6">
         <v>9</v>
       </c>
@@ -2271,7 +2276,7 @@
         <v>UPDATE profile SET name = 'Orks Morglum Knochenbrecher', points = 147 WHERE id =11423;</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" hidden="1">
       <c r="A7">
         <v>9</v>
       </c>
@@ -2304,7 +2309,7 @@
         <v>UPDATE profile SET name = 'Orks Oglock der Fürchtaliche', points = 87 WHERE id =11424;</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" hidden="1">
       <c r="A8">
         <v>9</v>
       </c>
@@ -2337,7 +2342,7 @@
         <v>UPDATE profile SET name = 'Orks Skarsnik Herrscher der Acht Gipfel', points = 78 WHERE id =11425;</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" hidden="1">
       <c r="A9">
         <v>9</v>
       </c>
@@ -2370,7 +2375,7 @@
         <v>UPDATE profile SET name = 'Orks Gobbla', points = 50.0 WHERE id =11792;</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" hidden="1">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2403,7 +2408,7 @@
         <v>UPDATE profile SET name = 'Orks Ork Chefoberboss', points = 110.0 WHERE id =11426;</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" hidden="1">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2436,7 +2441,7 @@
         <v>UPDATE profile SET name = 'Orks Schwarzork Chefoberboss', points = 140.0 WHERE id =11427;</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" hidden="1">
       <c r="A12">
         <v>9</v>
       </c>
@@ -2469,7 +2474,7 @@
         <v>UPDATE profile SET name = 'Orks Wildork Chefoberboss', points = 150.0 WHERE id =11428;</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" hidden="1">
       <c r="A13">
         <v>9</v>
       </c>
@@ -2502,7 +2507,7 @@
         <v>UPDATE profile SET name = 'Orks Goblin Chefoberboss', points = 50.0 WHERE id =11429;</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" hidden="1">
       <c r="A14">
         <v>9</v>
       </c>
@@ -2535,7 +2540,7 @@
         <v>UPDATE profile SET name = 'Orks Waldgoblin Chefoberboss', points = 50.0 WHERE id =11430;</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" hidden="1">
       <c r="A15">
         <v>9</v>
       </c>
@@ -2568,7 +2573,7 @@
         <v>UPDATE profile SET name = 'Orks Nachtgoblin Chefoberboss', points = 50.0 WHERE id =11431;</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" hidden="1">
       <c r="A16">
         <v>9</v>
       </c>
@@ -2601,7 +2606,7 @@
         <v>UPDATE profile SET name = 'Orks Schwarzork Armeestandarte', points = 92.0 WHERE id =11432;</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" hidden="1">
       <c r="A17">
         <v>9</v>
       </c>
@@ -2634,7 +2639,7 @@
         <v>UPDATE profile SET name = 'Orks Ork Armeestandarte', points = 83.0 WHERE id =11433;</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" hidden="1">
       <c r="A18">
         <v>9</v>
       </c>
@@ -2667,7 +2672,7 @@
         <v>UPDATE profile SET name = 'Orks Wildork Armeestandarte', points = 95.0 WHERE id =11434;</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" hidden="1">
       <c r="A19">
         <v>9</v>
       </c>
@@ -2700,7 +2705,7 @@
         <v>UPDATE profile SET name = 'Orks Goblin Armeestandarte', points = 65.0 WHERE id =11435;</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" hidden="1">
       <c r="A20">
         <v>9</v>
       </c>
@@ -2733,7 +2738,7 @@
         <v>UPDATE profile SET name = 'Orks Waldgoblin Armeestandarte', points = 65.0 WHERE id =11436;</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" hidden="1">
       <c r="A21">
         <v>9</v>
       </c>
@@ -2766,7 +2771,7 @@
         <v>UPDATE profile SET name = 'Orks Nachtgoblin Armeestandarte', points = 65.0 WHERE id =11437;</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" hidden="1">
       <c r="A22">
         <v>9</v>
       </c>
@@ -2799,7 +2804,7 @@
         <v>UPDATE profile SET name = 'Orks Schwarzork Oberboss', points = 91.0 WHERE id =11438;</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" hidden="1">
       <c r="A23">
         <v>9</v>
       </c>
@@ -2832,7 +2837,7 @@
         <v>UPDATE profile SET name = 'Orks Ork Oberboss', points = 72.0 WHERE id =11439;</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" hidden="1">
       <c r="A24">
         <v>9</v>
       </c>
@@ -2865,7 +2870,7 @@
         <v>UPDATE profile SET name = 'Orks Wildork Oberboss', points = 98.0 WHERE id =11440;</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" hidden="1">
       <c r="A25">
         <v>9</v>
       </c>
@@ -2898,7 +2903,7 @@
         <v>UPDATE profile SET name = 'Orks Goblin Oberboss', points = 33.0 WHERE id =11441;</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" hidden="1">
       <c r="A26">
         <v>9</v>
       </c>
@@ -2931,7 +2936,7 @@
         <v>UPDATE profile SET name = 'Orks Waldgoblin Oberboss', points = 33.0 WHERE id =11442;</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" hidden="1">
       <c r="A27">
         <v>9</v>
       </c>
@@ -2964,7 +2969,7 @@
         <v>UPDATE profile SET name = 'Orks Nachtgoblin Oberboss', points = 33.0 WHERE id =11443;</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" hidden="1">
       <c r="A28">
         <v>9</v>
       </c>
@@ -2997,7 +3002,7 @@
         <v>UPDATE profile SET name = 'Orks Schwarzork Boss', points = 42.0 WHERE id =11444;</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" hidden="1">
       <c r="A29">
         <v>9</v>
       </c>
@@ -3030,7 +3035,7 @@
         <v>UPDATE profile SET name = 'Orks Ork Boss', points = 33.0 WHERE id =11445;</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" hidden="1">
       <c r="A30">
         <v>9</v>
       </c>
@@ -3063,7 +3068,7 @@
         <v>UPDATE profile SET name = 'Orks Wildork Boss', points = 33.0 WHERE id =11446;</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" hidden="1">
       <c r="A31">
         <v>9</v>
       </c>
@@ -3096,7 +3101,7 @@
         <v>UPDATE profile SET name = 'Orks Goblin Boss', points = 15.0 WHERE id =11447;</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" hidden="1">
       <c r="A32">
         <v>9</v>
       </c>
@@ -3129,7 +3134,7 @@
         <v>UPDATE profile SET name = 'Orks Waldgoblin Boss', points = 15.0 WHERE id =11448;</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" hidden="1">
       <c r="A33">
         <v>9</v>
       </c>
@@ -3162,7 +3167,7 @@
         <v>UPDATE profile SET name = 'Orks Nachtgoblin Boss', points = 15.0 WHERE id =11449;</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" hidden="1">
       <c r="A34">
         <v>9</v>
       </c>
@@ -3195,7 +3200,7 @@
         <v>UPDATE profile SET name = 'Orks Ork Schamane', points = 56.0 WHERE id =11450;</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" hidden="1">
       <c r="A35">
         <v>9</v>
       </c>
@@ -3228,7 +3233,7 @@
         <v>UPDATE profile SET name = 'Orks Wildork Schamane', points = 59.0 WHERE id =11451;</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" hidden="1">
       <c r="A36">
         <v>9</v>
       </c>
@@ -3261,7 +3266,7 @@
         <v>UPDATE profile SET name = 'Orks Goblin Schamane', points = 28.0 WHERE id =11452;</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" hidden="1">
       <c r="A37">
         <v>9</v>
       </c>
@@ -3294,7 +3299,7 @@
         <v>UPDATE profile SET name = 'Orks Nachtgoblin Schamane', points = 28.0 WHERE id =11453;</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" hidden="1">
       <c r="A38">
         <v>9</v>
       </c>
@@ -3327,7 +3332,7 @@
         <v>UPDATE profile SET name = 'Orks Waldgoblin Schamane', points = 28.0 WHERE id =11454;</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" hidden="1">
       <c r="A39">
         <v>9</v>
       </c>
@@ -3360,7 +3365,7 @@
         <v>UPDATE profile SET name = 'Orks Ork Oberschamane', points = 118.0 WHERE id =11455;</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" hidden="1">
       <c r="A40">
         <v>9</v>
       </c>
@@ -3393,7 +3398,7 @@
         <v>UPDATE profile SET name = 'Orks Wildork Oberschamane', points = 122.0 WHERE id =11456;</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" hidden="1">
       <c r="A41">
         <v>9</v>
       </c>
@@ -3426,7 +3431,7 @@
         <v>UPDATE profile SET name = 'Orks Goblin Oberschamane', points = 83.0 WHERE id =11457;</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" hidden="1">
       <c r="A42">
         <v>9</v>
       </c>
@@ -3459,7 +3464,7 @@
         <v>UPDATE profile SET name = 'Orks Nachtgoblin Oberschamane', points = 83.0 WHERE id =11458;</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" hidden="1">
       <c r="A43">
         <v>9</v>
       </c>
@@ -3492,7 +3497,7 @@
         <v>UPDATE profile SET name = 'Orks Waldgoblin Oberschamane', points = 83.0 WHERE id =11459;</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" hidden="1">
       <c r="A44">
         <v>9</v>
       </c>
@@ -3525,7 +3530,7 @@
         <v>UPDATE profile SET name = 'Orks Ork Großschamane', points = 190.0 WHERE id =11460;</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" hidden="1">
       <c r="A45">
         <v>9</v>
       </c>
@@ -3558,7 +3563,7 @@
         <v>UPDATE profile SET name = 'Orks Wildork Großschamane', points = 219.0 WHERE id =11461;</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" hidden="1">
       <c r="A46">
         <v>9</v>
       </c>
@@ -3591,7 +3596,7 @@
         <v>UPDATE profile SET name = 'Orks Goblin Großschamane', points = 159.0 WHERE id =11462;</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" hidden="1">
       <c r="A47">
         <v>9</v>
       </c>
@@ -3624,7 +3629,7 @@
         <v>UPDATE profile SET name = 'Orks Nachtgoblin Großschamane', points = 159.0 WHERE id =11463;</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" hidden="1">
       <c r="A48">
         <v>9</v>
       </c>
@@ -3657,7 +3662,7 @@
         <v>UPDATE profile SET name = 'Orks Waldgoblin Großschamane', points = 159.0 WHERE id =11464;</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" hidden="1">
       <c r="A49">
         <v>9</v>
       </c>
@@ -3690,7 +3695,7 @@
         <v>UPDATE profile SET name = 'Orks Ork Meisterschamane', points = 287.0 WHERE id =11465;</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" hidden="1">
       <c r="A50">
         <v>9</v>
       </c>
@@ -3723,7 +3728,7 @@
         <v>UPDATE profile SET name = 'Orks Wildork Meisterschamane', points = 303.0 WHERE id =11466;</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" hidden="1">
       <c r="A51">
         <v>9</v>
       </c>
@@ -3756,7 +3761,7 @@
         <v>UPDATE profile SET name = 'Orks Goblin Meisterschamane', points = 253.0 WHERE id =11467;</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" hidden="1">
       <c r="A52">
         <v>9</v>
       </c>
@@ -3789,7 +3794,7 @@
         <v>UPDATE profile SET name = 'Orks Nachtgoblin Meisterschamane', points = 253.0 WHERE id =11468;</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" hidden="1">
       <c r="A53">
         <v>9</v>
       </c>
@@ -3822,7 +3827,7 @@
         <v>UPDATE profile SET name = 'Orks Waldgoblin Meisterschamane', points = 253.0 WHERE id =11469;</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" hidden="1">
       <c r="A54">
         <v>9</v>
       </c>
@@ -3855,7 +3860,7 @@
         <v>UPDATE profile SET name = 'Orks Gorfan Rotzahn', points = 87 WHERE id =11586;</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" hidden="1">
       <c r="A55">
         <v>9</v>
       </c>
@@ -3888,7 +3893,7 @@
         <v>UPDATE profile SET name = 'Orks Azhag der Vernichter', points = 127 WHERE id =11643;</v>
       </c>
     </row>
-    <row r="56" spans="1:10" s="2" customFormat="1">
+    <row r="56" spans="1:10" s="2" customFormat="1" hidden="1">
       <c r="A56" s="2">
         <v>9</v>
       </c>
@@ -3921,7 +3926,7 @@
         <v>UPDATE profile SET name = 'Lindwurm', points = 180.0 WHERE id =12423;</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" hidden="1">
       <c r="A57">
         <v>9</v>
       </c>
@@ -3980,14 +3985,14 @@
         <v>489</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>492</v>
+        <v>540</v>
       </c>
       <c r="J58" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Wildschwein', points = 5.5 WHERE id =12023;</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10">
+        <v>UPDATE profile SET name = 'Orks Wildschwein', points = 8 WHERE id =12023;</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" hidden="1">
       <c r="A59">
         <v>9</v>
       </c>
@@ -4046,14 +4051,14 @@
         <v>489</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>492</v>
+        <v>540</v>
       </c>
       <c r="J60" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = 'Orks Wildschwein', points = 5.5 WHERE id =12023;</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10">
+        <v>UPDATE profile SET name = 'Orks Wildschwein', points = 8 WHERE id =12023;</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" hidden="1">
       <c r="A61">
         <v>9</v>
       </c>
@@ -4086,7 +4091,7 @@
         <v>UPDATE profile SET name = 'Orks Riesenwolf', points = 4.0 WHERE id =11841;</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" hidden="1">
       <c r="A62">
         <v>9</v>
       </c>
@@ -4119,7 +4124,7 @@
         <v>UPDATE profile SET name = 'Orks Goblin Basis', points = 2.5 WHERE id =11852;</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" hidden="1">
       <c r="A63">
         <v>9</v>
       </c>
@@ -4152,7 +4157,7 @@
         <v>UPDATE profile SET name = 'Orks Waldgoblin Basis', points = 2.5 WHERE id =11853;</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" hidden="1">
       <c r="A64">
         <v>9</v>
       </c>
@@ -4185,7 +4190,7 @@
         <v>UPDATE profile SET name = 'Orks Riesenspinne', points = 6.5 WHERE id =12026;</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" hidden="1">
       <c r="A65">
         <v>9</v>
       </c>
@@ -4218,7 +4223,7 @@
         <v>UPDATE profile SET name = 'Orks Grobgitz Basis', points = 6.5 WHERE id =11854;</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" hidden="1">
       <c r="A66">
         <v>9</v>
       </c>
@@ -4251,7 +4256,7 @@
         <v>UPDATE profile SET name = 'Orks Ork Basis', points = 5.5 WHERE id =11855;</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" hidden="1">
       <c r="A67">
         <v>9</v>
       </c>
@@ -4284,7 +4289,7 @@
         <v>UPDATE profile SET name = 'Orks Ork Basis', points = 5.5 WHERE id =11856;</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" hidden="1">
       <c r="A68">
         <v>9</v>
       </c>
@@ -4317,7 +4322,7 @@
         <v>UPDATE profile SET name = 'Orks Schwarzork Basis', points = 8.0 WHERE id =11857;</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" hidden="1">
       <c r="A69">
         <v>9</v>
       </c>
@@ -4350,7 +4355,7 @@
         <v>UPDATE profile SET name = 'Orks Wildork Basis', points = 6.5 WHERE id =11858;</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" hidden="1">
       <c r="A70">
         <v>9</v>
       </c>
@@ -4383,7 +4388,7 @@
         <v>UPDATE profile SET name = 'Orks Goblin Basis', points = 2.5 WHERE id =11852;</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" hidden="1">
       <c r="A71">
         <v>9</v>
       </c>
@@ -4416,7 +4421,7 @@
         <v>UPDATE profile SET name = 'Orks Waldgoblin Basis', points = 2.5 WHERE id =11853;</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" hidden="1">
       <c r="A72">
         <v>9</v>
       </c>
@@ -4449,7 +4454,7 @@
         <v>UPDATE profile SET name = 'Orks Nachtgoblin Basis', points = 2.5 WHERE id =11861;</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" hidden="1">
       <c r="A73">
         <v>9</v>
       </c>
@@ -4482,7 +4487,7 @@
         <v>UPDATE profile SET name = 'Orks Nachtgoblin Basis', points = 2.5 WHERE id =11862;</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" hidden="1">
       <c r="A74">
         <v>9</v>
       </c>
@@ -4515,7 +4520,7 @@
         <v>UPDATE profile SET name = 'Orks Höhlensquig', points = 20.0 WHERE id =12027;</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" hidden="1">
       <c r="A75">
         <v>9</v>
       </c>
@@ -4548,7 +4553,7 @@
         <v>UPDATE profile SET name = 'Orks Nachtgoblin Basis', points = 2.5 WHERE id =11863;</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" hidden="1">
       <c r="A76">
         <v>9</v>
       </c>
@@ -4581,7 +4586,7 @@
         <v>UPDATE profile SET name = 'Orks Fanatic', points = 30.0 WHERE id =11864;</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" hidden="1">
       <c r="A77">
         <v>9</v>
       </c>
@@ -4614,7 +4619,7 @@
         <v>UPDATE profile SET name = 'Orks Nachtgoblin Basis', points = 2.5 WHERE id =11861;</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" hidden="1">
       <c r="A78">
         <v>9</v>
       </c>
@@ -4647,7 +4652,7 @@
         <v>UPDATE profile SET name = 'Orks Höhlensquig', points = 20.0 WHERE id =12028;</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" hidden="1">
       <c r="A79">
         <v>9</v>
       </c>
@@ -4680,7 +4685,7 @@
         <v>UPDATE profile SET name = 'Orks Riese', points = 200.0 WHERE id =11866;</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" hidden="1">
       <c r="A80">
         <v>9</v>
       </c>
@@ -4713,7 +4718,7 @@
         <v>UPDATE profile SET name = 'Orks Oger', points = 40.0 WHERE id =11867;</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" hidden="1">
       <c r="A81">
         <v>9</v>
       </c>
@@ -4746,7 +4751,7 @@
         <v>UPDATE profile SET name = 'Orks Flußtroll', points = 65.0 WHERE id =11868;</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" hidden="1">
       <c r="A82">
         <v>9</v>
       </c>
@@ -4779,7 +4784,7 @@
         <v>UPDATE profile SET name = 'Orks Steintroll', points = 65.0 WHERE id =11869;</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" hidden="1">
       <c r="A83">
         <v>9</v>
       </c>
@@ -4812,7 +4817,7 @@
         <v>UPDATE profile SET name = 'Orks Snotling-Base', points = 15.0 WHERE id =11870;</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" hidden="1">
       <c r="A84">
         <v>9</v>
       </c>
@@ -4845,7 +4850,7 @@
         <v>UPDATE profile SET name = 'Orks Ork Basis', points = 5.5 WHERE id =12071;</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" hidden="1">
       <c r="A85">
         <v>9</v>
       </c>
@@ -4878,7 +4883,7 @@
         <v>UPDATE profile SET name = 'Kleine Steinschleuder', points = 50.0 WHERE id =12133;</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" hidden="1">
       <c r="A86">
         <v>9</v>
       </c>
@@ -4911,7 +4916,7 @@
         <v>UPDATE profile SET name = 'Orks Ork Basis', points = 5.5 WHERE id =12071;</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" hidden="1">
       <c r="A87">
         <v>9</v>
       </c>
@@ -4944,7 +4949,7 @@
         <v>UPDATE profile SET name = 'Große Steinschleuder', points = 80.0 WHERE id =12134;</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" hidden="1">
       <c r="A88">
         <v>9</v>
       </c>
@@ -4977,7 +4982,7 @@
         <v>UPDATE profile SET name = 'Orks Ork Basis', points = 5.5 WHERE id =12071;</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" hidden="1">
       <c r="A89">
         <v>9</v>
       </c>
@@ -5010,7 +5015,7 @@
         <v>UPDATE profile SET name = 'Speerschleuder', points = 30.0 WHERE id =12132;</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" hidden="1">
       <c r="A90">
         <v>9</v>
       </c>
@@ -5043,7 +5048,7 @@
         <v>UPDATE profile SET name = 'Orks Snotling-Base', points = 15.0 WHERE id =12074;</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" hidden="1">
       <c r="A91">
         <v>9</v>
       </c>
@@ -5076,7 +5081,7 @@
         <v>UPDATE profile SET name = 'Orks Kurbelwagen', points = 25.0 WHERE id =12122;</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" hidden="1">
       <c r="A92">
         <v>9</v>
       </c>
@@ -5109,7 +5114,7 @@
         <v>UPDATE profile SET name = 'Orks Goblin Basis', points = 2.5 WHERE id =12075;</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" hidden="1">
       <c r="A93">
         <v>9</v>
       </c>
@@ -5168,14 +5173,14 @@
         <v>489</v>
       </c>
       <c r="I94" s="5" t="s">
-        <v>492</v>
+        <v>540</v>
       </c>
       <c r="J94" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = 'Orks Wildschwein', points = 5.5 WHERE id =12023;</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10">
+        <v>UPDATE profile SET name = 'Orks Wildschwein', points = 8 WHERE id =12023;</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" hidden="1">
       <c r="A95">
         <v>9</v>
       </c>
@@ -5208,7 +5213,7 @@
         <v>UPDATE profile SET name = 'Orks Ork Basis', points = 5.5 WHERE id =12076;</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" hidden="1">
       <c r="A96">
         <v>9</v>
       </c>
@@ -5241,7 +5246,7 @@
         <v>UPDATE profile SET name = 'Streitwagen', points = 50.0 WHERE id =12159;</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" hidden="1">
       <c r="A97">
         <v>9</v>
       </c>
@@ -5274,7 +5279,7 @@
         <v>UPDATE profile SET name = 'Orks Riesenwolf', points = 4.0 WHERE id =11841;</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" hidden="1">
       <c r="A98">
         <v>9</v>
       </c>
@@ -5307,7 +5312,7 @@
         <v>UPDATE profile SET name = 'Orks Goblin Basis', points = 2.5 WHERE id =11852;</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" hidden="1">
       <c r="A99">
         <v>9</v>
       </c>
@@ -5340,7 +5345,7 @@
         <v>UPDATE profile SET name = 'Streitwagen', points = 50.0 WHERE id =12159;</v>
       </c>
     </row>
-    <row r="100" spans="1:10" s="2" customFormat="1">
+    <row r="100" spans="1:10" s="2" customFormat="1" hidden="1">
       <c r="A100" s="2">
         <v>9</v>
       </c>
@@ -5369,7 +5374,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="101" spans="1:10" s="2" customFormat="1">
+    <row r="101" spans="1:10" s="2" customFormat="1" hidden="1">
       <c r="A101" s="2">
         <v>9</v>
       </c>
@@ -5398,7 +5403,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="102" spans="1:10" s="2" customFormat="1">
+    <row r="102" spans="1:10" s="2" customFormat="1" hidden="1">
       <c r="A102" s="2">
         <v>9</v>
       </c>
@@ -5427,7 +5432,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="103" spans="1:10" s="2" customFormat="1">
+    <row r="103" spans="1:10" s="2" customFormat="1" hidden="1">
       <c r="A103" s="2">
         <v>9</v>
       </c>
@@ -5456,7 +5461,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="104" spans="1:10" s="2" customFormat="1">
+    <row r="104" spans="1:10" s="2" customFormat="1" hidden="1">
       <c r="A104" s="2">
         <v>9</v>
       </c>
@@ -5485,7 +5490,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="105" spans="1:10" s="2" customFormat="1">
+    <row r="105" spans="1:10" s="2" customFormat="1" hidden="1">
       <c r="A105" s="2">
         <v>9</v>
       </c>
@@ -5514,7 +5519,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="106" spans="1:10" s="2" customFormat="1">
+    <row r="106" spans="1:10" s="2" customFormat="1" hidden="1">
       <c r="A106" s="2">
         <v>9</v>
       </c>
@@ -5543,7 +5548,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="107" spans="1:10" s="2" customFormat="1">
+    <row r="107" spans="1:10" s="2" customFormat="1" hidden="1">
       <c r="A107" s="2">
         <v>9</v>
       </c>
@@ -5572,7 +5577,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="108" spans="1:10" s="2" customFormat="1">
+    <row r="108" spans="1:10" s="2" customFormat="1" hidden="1">
       <c r="A108" s="2">
         <v>9</v>
       </c>
@@ -5601,7 +5606,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="109" spans="1:10" s="2" customFormat="1">
+    <row r="109" spans="1:10" s="2" customFormat="1" hidden="1">
       <c r="A109" s="2">
         <v>9</v>
       </c>
@@ -5630,7 +5635,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="110" spans="1:10" s="2" customFormat="1">
+    <row r="110" spans="1:10" s="2" customFormat="1" hidden="1">
       <c r="A110" s="2">
         <v>9</v>
       </c>
@@ -5659,7 +5664,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="111" spans="1:10" s="2" customFormat="1">
+    <row r="111" spans="1:10" s="2" customFormat="1" hidden="1">
       <c r="A111" s="2">
         <v>9</v>
       </c>
@@ -5688,7 +5693,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="112" spans="1:10" s="2" customFormat="1">
+    <row r="112" spans="1:10" s="2" customFormat="1" hidden="1">
       <c r="A112" s="2">
         <v>9</v>
       </c>
@@ -5717,7 +5722,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="113" spans="1:9" s="2" customFormat="1">
+    <row r="113" spans="1:9" s="2" customFormat="1" hidden="1">
       <c r="A113" s="2">
         <v>9</v>
       </c>
@@ -5746,7 +5751,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="114" spans="1:9" s="2" customFormat="1">
+    <row r="114" spans="1:9" s="2" customFormat="1" hidden="1">
       <c r="A114" s="2">
         <v>9</v>
       </c>
@@ -5775,7 +5780,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="115" spans="1:9" s="2" customFormat="1">
+    <row r="115" spans="1:9" s="2" customFormat="1" hidden="1">
       <c r="A115" s="2">
         <v>9</v>
       </c>
@@ -5804,7 +5809,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="116" spans="1:9" s="2" customFormat="1">
+    <row r="116" spans="1:9" s="2" customFormat="1" hidden="1">
       <c r="A116" s="2">
         <v>9</v>
       </c>
@@ -5833,7 +5838,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="117" spans="1:9" s="2" customFormat="1">
+    <row r="117" spans="1:9" s="2" customFormat="1" hidden="1">
       <c r="A117" s="2">
         <v>9</v>
       </c>
@@ -5862,7 +5867,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="118" spans="1:9" s="2" customFormat="1">
+    <row r="118" spans="1:9" s="2" customFormat="1" hidden="1">
       <c r="A118" s="2">
         <v>9</v>
       </c>
@@ -5892,6 +5897,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I118" xr:uid="{73F0926A-28CA-48B1-B472-BA874B7E1E5A}">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="Orks Wildschwein"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Edited profiles of empire
</commit_message>
<xml_diff>
--- a/resources/db/Profiles.xlsx
+++ b/resources/db/Profiles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IN57KC\data\Projekte\csharp\ArmyBuilder\resources\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\projects\ArmyBuilder\sourcecode\resources\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDEB7E77-5668-46D3-BEEA-2658FD261B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{615C4764-397C-41DB-992F-12A4A7F362B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{72821A2A-92BA-4C26-854D-A2ECB76DE865}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{72821A2A-92BA-4C26-854D-A2ECB76DE865}"/>
   </bookViews>
   <sheets>
     <sheet name="Empire Profiles" sheetId="10" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1827" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1883" uniqueCount="639">
   <si>
     <t>General</t>
   </si>
@@ -1839,13 +1839,133 @@
   </si>
   <si>
     <t>100</t>
+  </si>
+  <si>
+    <t>Imperium Armeestandarte</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>Imperium Held</t>
+  </si>
+  <si>
+    <t>Imperium Champion</t>
+  </si>
+  <si>
+    <t>Imperium Zauberer</t>
+  </si>
+  <si>
+    <t>Imperium Oberzauberer</t>
+  </si>
+  <si>
+    <t>Imperium Großzauberer</t>
+  </si>
+  <si>
+    <t>Imperium Meisterzauberer</t>
+  </si>
+  <si>
+    <t>Imperium Halbling Champion</t>
+  </si>
+  <si>
+    <t>Imperium Halbling Held</t>
+  </si>
+  <si>
+    <t>Imperium Halbling General</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>118</t>
+  </si>
+  <si>
+    <t>190</t>
+  </si>
+  <si>
+    <t>287</t>
+  </si>
+  <si>
+    <t>Imperium Karl Franz</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>Imperium Kriegspferd</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Imperium Elite</t>
+  </si>
+  <si>
+    <t>Imperium Basis</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Imperium Schwertkämpfer</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Imperium Flagelant</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Imperium Halbling</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>Imperium Zwerg</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>114</t>
+  </si>
+  <si>
+    <t>39.5</t>
+  </si>
+  <si>
+    <t>Imperium Reiter</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>70</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2238,25 +2358,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0E7169B-97C9-4864-9863-F346617492A7}">
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="28.5">
       <c r="A1" s="3" t="s">
         <v>110</v>
       </c>
@@ -2285,7 +2405,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>8</v>
       </c>
@@ -2318,7 +2438,7 @@
         <v>UPDATE profile SET name = 'Imperium General', points = 100 WHERE id =11487;</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>8</v>
       </c>
@@ -2340,15 +2460,18 @@
       <c r="G3">
         <v>11488</v>
       </c>
+      <c r="H3" t="s">
+        <v>599</v>
+      </c>
       <c r="I3" s="5" t="s">
-        <v>1</v>
+        <v>600</v>
       </c>
       <c r="J3" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11488;</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Armeestandarte', points = 80 WHERE id =11488;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>8</v>
       </c>
@@ -2370,15 +2493,18 @@
       <c r="G4">
         <v>11489</v>
       </c>
+      <c r="H4" t="s">
+        <v>601</v>
+      </c>
       <c r="I4" s="5" t="s">
-        <v>1</v>
+        <v>610</v>
       </c>
       <c r="J4" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11489;</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Held', points = 65 WHERE id =11489;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>8</v>
       </c>
@@ -2400,15 +2526,18 @@
       <c r="G5">
         <v>11490</v>
       </c>
+      <c r="H5" t="s">
+        <v>602</v>
+      </c>
       <c r="I5" s="5" t="s">
-        <v>1</v>
+        <v>611</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11490;</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Champion', points = 30 WHERE id =11490;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>8</v>
       </c>
@@ -2430,15 +2559,18 @@
       <c r="G6">
         <v>11491</v>
       </c>
+      <c r="H6" t="s">
+        <v>603</v>
+      </c>
       <c r="I6" s="5" t="s">
-        <v>1</v>
+        <v>612</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11491;</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Zauberer', points = 56 WHERE id =11491;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>8</v>
       </c>
@@ -2460,15 +2592,18 @@
       <c r="G7">
         <v>11492</v>
       </c>
+      <c r="H7" t="s">
+        <v>604</v>
+      </c>
       <c r="I7" s="5" t="s">
-        <v>1</v>
+        <v>613</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11492;</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Oberzauberer', points = 118 WHERE id =11492;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>8</v>
       </c>
@@ -2490,15 +2625,18 @@
       <c r="G8">
         <v>11493</v>
       </c>
+      <c r="H8" t="s">
+        <v>605</v>
+      </c>
       <c r="I8" s="5" t="s">
-        <v>1</v>
+        <v>614</v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11493;</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Großzauberer', points = 190 WHERE id =11493;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2520,15 +2658,18 @@
       <c r="G9">
         <v>11494</v>
       </c>
+      <c r="H9" t="s">
+        <v>606</v>
+      </c>
       <c r="I9" s="5" t="s">
-        <v>1</v>
+        <v>615</v>
       </c>
       <c r="J9" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11494;</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Meisterzauberer', points = 287 WHERE id =11494;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2550,15 +2691,18 @@
       <c r="G10">
         <v>11495</v>
       </c>
+      <c r="H10" t="s">
+        <v>616</v>
+      </c>
       <c r="I10" s="5" t="s">
-        <v>1</v>
+        <v>537</v>
       </c>
       <c r="J10" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11495;</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Karl Franz', points = 110 WHERE id =11495;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>8</v>
       </c>
@@ -2580,15 +2724,18 @@
       <c r="G11">
         <v>11795</v>
       </c>
+      <c r="H11" t="s">
+        <v>65</v>
+      </c>
       <c r="I11" s="5" t="s">
-        <v>1</v>
+        <v>617</v>
       </c>
       <c r="J11" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11795;</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Greif', points = 150 WHERE id =11795;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>8</v>
       </c>
@@ -2618,7 +2765,7 @@
         <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11496;</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>8</v>
       </c>
@@ -2648,7 +2795,7 @@
         <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11497;</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>8</v>
       </c>
@@ -2670,15 +2817,18 @@
       <c r="G14">
         <v>11796</v>
       </c>
+      <c r="H14" t="s">
+        <v>618</v>
+      </c>
       <c r="I14" s="5" t="s">
-        <v>1</v>
+        <v>619</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11796;</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Kriegspferd', points = 3 WHERE id =11796;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>8</v>
       </c>
@@ -2708,7 +2858,7 @@
         <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11498;</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>8</v>
       </c>
@@ -2738,7 +2888,7 @@
         <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11842;</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>8</v>
       </c>
@@ -2760,15 +2910,18 @@
       <c r="G17">
         <v>12156</v>
       </c>
+      <c r="H17" t="s">
+        <v>618</v>
+      </c>
       <c r="I17" s="5" t="s">
-        <v>1</v>
+        <v>619</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12156;</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Kriegspferd', points = 3 WHERE id =12156;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>8</v>
       </c>
@@ -2798,7 +2951,7 @@
         <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11499;</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>8</v>
       </c>
@@ -2828,7 +2981,7 @@
         <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11500;</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>8</v>
       </c>
@@ -2850,15 +3003,18 @@
       <c r="G20">
         <v>11796</v>
       </c>
+      <c r="H20" t="s">
+        <v>618</v>
+      </c>
       <c r="I20" s="5" t="s">
-        <v>1</v>
+        <v>619</v>
       </c>
       <c r="J20" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11796;</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Kriegspferd', points = 3 WHERE id =11796;</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>8</v>
       </c>
@@ -2888,7 +3044,7 @@
         <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11502;</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>8</v>
       </c>
@@ -2910,15 +3066,18 @@
       <c r="G22">
         <v>11799</v>
       </c>
+      <c r="H22" t="s">
+        <v>618</v>
+      </c>
       <c r="I22" s="5" t="s">
-        <v>1</v>
+        <v>619</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11799;</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Kriegspferd', points = 3 WHERE id =11799;</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>8</v>
       </c>
@@ -2948,7 +3107,7 @@
         <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11503;</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>8</v>
       </c>
@@ -2970,15 +3129,18 @@
       <c r="G24">
         <v>12156</v>
       </c>
+      <c r="H24" t="s">
+        <v>618</v>
+      </c>
       <c r="I24" s="5" t="s">
-        <v>1</v>
+        <v>619</v>
       </c>
       <c r="J24" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12156;</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Kriegspferd', points = 3 WHERE id =12156;</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>8</v>
       </c>
@@ -3008,7 +3170,7 @@
         <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11504;</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>8</v>
       </c>
@@ -3030,15 +3192,18 @@
       <c r="G26">
         <v>12156</v>
       </c>
+      <c r="H26" t="s">
+        <v>618</v>
+      </c>
       <c r="I26" s="5" t="s">
-        <v>1</v>
+        <v>619</v>
       </c>
       <c r="J26" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12156;</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Kriegspferd', points = 3 WHERE id =12156;</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>8</v>
       </c>
@@ -3068,7 +3233,7 @@
         <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11505;</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>8</v>
       </c>
@@ -3090,15 +3255,18 @@
       <c r="G28">
         <v>11796</v>
       </c>
+      <c r="H28" t="s">
+        <v>618</v>
+      </c>
       <c r="I28" s="5" t="s">
-        <v>1</v>
+        <v>619</v>
       </c>
       <c r="J28" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11796;</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Kriegspferd', points = 3 WHERE id =11796;</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>8</v>
       </c>
@@ -3128,7 +3296,7 @@
         <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11640;</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>8</v>
       </c>
@@ -3150,15 +3318,18 @@
       <c r="G30">
         <v>11799</v>
       </c>
+      <c r="H30" t="s">
+        <v>618</v>
+      </c>
       <c r="I30" s="5" t="s">
-        <v>1</v>
+        <v>619</v>
       </c>
       <c r="J30" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11799;</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Kriegspferd', points = 3 WHERE id =11799;</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>8</v>
       </c>
@@ -3180,15 +3351,18 @@
       <c r="G31">
         <v>11718</v>
       </c>
+      <c r="H31" t="s">
+        <v>607</v>
+      </c>
       <c r="I31" s="5" t="s">
-        <v>1</v>
+        <v>636</v>
       </c>
       <c r="J31" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11718;</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Halbling Champion', points = 21 WHERE id =11718;</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>8</v>
       </c>
@@ -3210,15 +3384,18 @@
       <c r="G32">
         <v>11719</v>
       </c>
+      <c r="H32" t="s">
+        <v>608</v>
+      </c>
       <c r="I32" s="5" t="s">
-        <v>1</v>
+        <v>637</v>
       </c>
       <c r="J32" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11719;</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Halbling Held', points = 46 WHERE id =11719;</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33">
         <v>8</v>
       </c>
@@ -3240,15 +3417,18 @@
       <c r="G33">
         <v>11720</v>
       </c>
+      <c r="H33" t="s">
+        <v>609</v>
+      </c>
       <c r="I33" s="5" t="s">
-        <v>1</v>
+        <v>638</v>
       </c>
       <c r="J33" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11720;</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Halbling General', points = 70 WHERE id =11720;</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34">
         <v>8</v>
       </c>
@@ -3270,15 +3450,18 @@
       <c r="G34">
         <v>11871</v>
       </c>
+      <c r="H34" t="s">
+        <v>620</v>
+      </c>
       <c r="I34" s="5" t="s">
-        <v>1</v>
+        <v>540</v>
       </c>
       <c r="J34" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11871;</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Elite', points = 8 WHERE id =11871;</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35">
         <v>8</v>
       </c>
@@ -3300,15 +3483,18 @@
       <c r="G35">
         <v>12156</v>
       </c>
+      <c r="H35" t="s">
+        <v>618</v>
+      </c>
       <c r="I35" s="5" t="s">
-        <v>1</v>
+        <v>619</v>
       </c>
       <c r="J35" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12156;</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Kriegspferd', points = 3 WHERE id =12156;</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36">
         <v>8</v>
       </c>
@@ -3330,15 +3516,18 @@
       <c r="G36">
         <v>11799</v>
       </c>
+      <c r="H36" t="s">
+        <v>618</v>
+      </c>
       <c r="I36" s="5" t="s">
-        <v>1</v>
+        <v>619</v>
       </c>
       <c r="J36" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11799;</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Kriegspferd', points = 3 WHERE id =11799;</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37">
         <v>8</v>
       </c>
@@ -3360,15 +3549,18 @@
       <c r="G37">
         <v>11872</v>
       </c>
+      <c r="H37" t="s">
+        <v>620</v>
+      </c>
       <c r="I37" s="5" t="s">
-        <v>1</v>
+        <v>540</v>
       </c>
       <c r="J37" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11872;</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Elite', points = 8 WHERE id =11872;</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38">
         <v>8</v>
       </c>
@@ -3390,15 +3582,18 @@
       <c r="G38">
         <v>11799</v>
       </c>
+      <c r="H38" t="s">
+        <v>618</v>
+      </c>
       <c r="I38" s="5" t="s">
-        <v>1</v>
+        <v>619</v>
       </c>
       <c r="J38" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11799;</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Kriegspferd', points = 3 WHERE id =11799;</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39">
         <v>8</v>
       </c>
@@ -3420,15 +3615,18 @@
       <c r="G39">
         <v>11873</v>
       </c>
+      <c r="H39" t="s">
+        <v>620</v>
+      </c>
       <c r="I39" s="5" t="s">
-        <v>1</v>
+        <v>540</v>
       </c>
       <c r="J39" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11873;</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Elite', points = 8 WHERE id =11873;</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40">
         <v>8</v>
       </c>
@@ -3450,15 +3648,18 @@
       <c r="G40">
         <v>11799</v>
       </c>
+      <c r="H40" t="s">
+        <v>618</v>
+      </c>
       <c r="I40" s="5" t="s">
-        <v>1</v>
+        <v>619</v>
       </c>
       <c r="J40" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11799;</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Kriegspferd', points = 3 WHERE id =11799;</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41">
         <v>8</v>
       </c>
@@ -3480,15 +3681,18 @@
       <c r="G41">
         <v>11874</v>
       </c>
+      <c r="H41" t="s">
+        <v>620</v>
+      </c>
       <c r="I41" s="5" t="s">
-        <v>1</v>
+        <v>540</v>
       </c>
       <c r="J41" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11874;</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Elite', points = 8 WHERE id =11874;</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42">
         <v>8</v>
       </c>
@@ -3510,15 +3714,18 @@
       <c r="G42">
         <v>11875</v>
       </c>
+      <c r="H42" t="s">
+        <v>634</v>
+      </c>
       <c r="I42" s="5" t="s">
-        <v>1</v>
+        <v>635</v>
       </c>
       <c r="J42" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11875;</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Reiter', points = 7 WHERE id =11875;</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43">
         <v>8</v>
       </c>
@@ -3540,15 +3747,18 @@
       <c r="G43">
         <v>11876</v>
       </c>
+      <c r="H43" t="s">
+        <v>634</v>
+      </c>
       <c r="I43" s="5" t="s">
-        <v>1</v>
+        <v>635</v>
       </c>
       <c r="J43" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11876;</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Reiter', points = 7 WHERE id =11876;</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44">
         <v>8</v>
       </c>
@@ -3570,15 +3780,18 @@
       <c r="G44">
         <v>11877</v>
       </c>
+      <c r="H44" t="s">
+        <v>621</v>
+      </c>
       <c r="I44" s="5" t="s">
-        <v>1</v>
+        <v>622</v>
       </c>
       <c r="J44" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11877;</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Basis', points = 5 WHERE id =11877;</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45">
         <v>8</v>
       </c>
@@ -3600,15 +3813,18 @@
       <c r="G45">
         <v>11878</v>
       </c>
+      <c r="H45" t="s">
+        <v>620</v>
+      </c>
       <c r="I45" s="5" t="s">
-        <v>1</v>
+        <v>540</v>
       </c>
       <c r="J45" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11878;</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Elite', points = 8 WHERE id =11878;</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46">
         <v>8</v>
       </c>
@@ -3630,15 +3846,18 @@
       <c r="G46">
         <v>11879</v>
       </c>
+      <c r="H46" t="s">
+        <v>621</v>
+      </c>
       <c r="I46" s="5" t="s">
-        <v>1</v>
+        <v>622</v>
       </c>
       <c r="J46" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11879;</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Basis', points = 5 WHERE id =11879;</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47">
         <v>8</v>
       </c>
@@ -3660,15 +3879,18 @@
       <c r="G47">
         <v>11880</v>
       </c>
+      <c r="H47" t="s">
+        <v>621</v>
+      </c>
       <c r="I47" s="5" t="s">
-        <v>1</v>
+        <v>622</v>
       </c>
       <c r="J47" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11880;</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Basis', points = 5 WHERE id =11880;</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48">
         <v>8</v>
       </c>
@@ -3690,15 +3912,18 @@
       <c r="G48">
         <v>11881</v>
       </c>
+      <c r="H48" t="s">
+        <v>623</v>
+      </c>
       <c r="I48" s="5" t="s">
-        <v>1</v>
+        <v>624</v>
       </c>
       <c r="J48" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11881;</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Schwertkämpfer', points = 6 WHERE id =11881;</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49">
         <v>8</v>
       </c>
@@ -3720,15 +3945,18 @@
       <c r="G49">
         <v>11882</v>
       </c>
+      <c r="H49" t="s">
+        <v>621</v>
+      </c>
       <c r="I49" s="5" t="s">
-        <v>1</v>
+        <v>622</v>
       </c>
       <c r="J49" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11882;</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Basis', points = 5 WHERE id =11882;</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50">
         <v>8</v>
       </c>
@@ -3750,15 +3978,18 @@
       <c r="G50">
         <v>11883</v>
       </c>
+      <c r="H50" t="s">
+        <v>621</v>
+      </c>
       <c r="I50" s="5" t="s">
-        <v>1</v>
+        <v>622</v>
       </c>
       <c r="J50" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11883;</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Basis', points = 5 WHERE id =11883;</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51">
         <v>8</v>
       </c>
@@ -3780,15 +4011,18 @@
       <c r="G51">
         <v>11796</v>
       </c>
+      <c r="H51" t="s">
+        <v>618</v>
+      </c>
       <c r="I51" s="5" t="s">
-        <v>1</v>
+        <v>619</v>
       </c>
       <c r="J51" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11796;</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Kriegspferd', points = 3 WHERE id =11796;</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52">
         <v>8</v>
       </c>
@@ -3810,15 +4044,18 @@
       <c r="G52">
         <v>11884</v>
       </c>
+      <c r="H52" t="s">
+        <v>623</v>
+      </c>
       <c r="I52" s="5" t="s">
-        <v>1</v>
+        <v>624</v>
       </c>
       <c r="J52" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11884;</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Schwertkämpfer', points = 6 WHERE id =11884;</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53">
         <v>8</v>
       </c>
@@ -3840,15 +4077,18 @@
       <c r="G53">
         <v>11885</v>
       </c>
+      <c r="H53" t="s">
+        <v>634</v>
+      </c>
       <c r="I53" s="5" t="s">
-        <v>1</v>
+        <v>635</v>
       </c>
       <c r="J53" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11885;</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Reiter', points = 7 WHERE id =11885;</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54">
         <v>8</v>
       </c>
@@ -3870,15 +4110,18 @@
       <c r="G54">
         <v>11886</v>
       </c>
+      <c r="H54" t="s">
+        <v>625</v>
+      </c>
       <c r="I54" s="5" t="s">
-        <v>1</v>
+        <v>626</v>
       </c>
       <c r="J54" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11886;</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Flagelant', points = 9 WHERE id =11886;</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55">
         <v>8</v>
       </c>
@@ -3900,15 +4143,18 @@
       <c r="G55">
         <v>11887</v>
       </c>
+      <c r="H55" t="s">
+        <v>629</v>
+      </c>
       <c r="I55" s="5" t="s">
-        <v>1</v>
+        <v>540</v>
       </c>
       <c r="J55" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11887;</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Zwerg', points = 8 WHERE id =11887;</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56">
         <v>8</v>
       </c>
@@ -3930,15 +4176,18 @@
       <c r="G56">
         <v>11888</v>
       </c>
+      <c r="H56" t="s">
+        <v>627</v>
+      </c>
       <c r="I56" s="5" t="s">
-        <v>1</v>
+        <v>628</v>
       </c>
       <c r="J56" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11888;</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Halbling', points = 3.5 WHERE id =11888;</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57">
         <v>8</v>
       </c>
@@ -3971,7 +4220,7 @@
         <v>UPDATE profile SET name = 'Orks Oger', points = 40.0 WHERE id =11867;</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10">
       <c r="A58">
         <v>8</v>
       </c>
@@ -3993,15 +4242,18 @@
       <c r="G58">
         <v>11962</v>
       </c>
+      <c r="H58" t="s">
+        <v>621</v>
+      </c>
       <c r="I58" s="5" t="s">
-        <v>1</v>
+        <v>622</v>
       </c>
       <c r="J58" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11962;</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Basis', points = 5 WHERE id =11962;</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59">
         <v>8</v>
       </c>
@@ -4023,15 +4275,18 @@
       <c r="G59">
         <v>12078</v>
       </c>
+      <c r="H59" t="s">
+        <v>621</v>
+      </c>
       <c r="I59" s="5" t="s">
-        <v>1</v>
+        <v>622</v>
       </c>
       <c r="J59" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12078;</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Basis', points = 5 WHERE id =12078;</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60">
         <v>8</v>
       </c>
@@ -4053,15 +4308,18 @@
       <c r="G60">
         <v>12126</v>
       </c>
+      <c r="H60" t="s">
+        <v>589</v>
+      </c>
       <c r="I60" s="5" t="s">
-        <v>1</v>
+        <v>630</v>
       </c>
       <c r="J60" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12126;</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Mörser', points = 85 WHERE id =12126;</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
       <c r="A61">
         <v>8</v>
       </c>
@@ -4083,15 +4341,18 @@
       <c r="G61">
         <v>12078</v>
       </c>
+      <c r="H61" t="s">
+        <v>621</v>
+      </c>
       <c r="I61" s="5" t="s">
-        <v>1</v>
+        <v>622</v>
       </c>
       <c r="J61" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12078;</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Basis', points = 5 WHERE id =12078;</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
       <c r="A62">
         <v>8</v>
       </c>
@@ -4113,15 +4374,18 @@
       <c r="G62">
         <v>12127</v>
       </c>
+      <c r="H62" t="s">
+        <v>590</v>
+      </c>
       <c r="I62" s="5" t="s">
-        <v>1</v>
+        <v>630</v>
       </c>
       <c r="J62" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12127;</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Großkanone', points = 85 WHERE id =12127;</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
       <c r="A63">
         <v>8</v>
       </c>
@@ -4143,15 +4407,18 @@
       <c r="G63">
         <v>12080</v>
       </c>
+      <c r="H63" t="s">
+        <v>591</v>
+      </c>
       <c r="I63" s="5" t="s">
-        <v>1</v>
+        <v>631</v>
       </c>
       <c r="J63" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12080;</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Dampfpanzer', points = 200 WHERE id =12080;</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
       <c r="A64">
         <v>8</v>
       </c>
@@ -4173,15 +4440,18 @@
       <c r="G64">
         <v>12078</v>
       </c>
+      <c r="H64" t="s">
+        <v>621</v>
+      </c>
       <c r="I64" s="5" t="s">
-        <v>1</v>
+        <v>622</v>
       </c>
       <c r="J64" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12078;</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Basis', points = 5 WHERE id =12078;</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
       <c r="A65">
         <v>8</v>
       </c>
@@ -4203,15 +4473,18 @@
       <c r="G65">
         <v>12128</v>
       </c>
+      <c r="H65" t="s">
+        <v>592</v>
+      </c>
       <c r="I65" s="5" t="s">
-        <v>1</v>
+        <v>632</v>
       </c>
       <c r="J65" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12128;</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Kriegswagen', points = 114 WHERE id =12128;</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
       <c r="A66">
         <v>8</v>
       </c>
@@ -4233,15 +4506,18 @@
       <c r="G66">
         <v>12156</v>
       </c>
+      <c r="H66" t="s">
+        <v>618</v>
+      </c>
       <c r="I66" s="5" t="s">
-        <v>1</v>
+        <v>619</v>
       </c>
       <c r="J66" t="str">
         <f t="shared" ref="J66:J70" si="1">CONCATENATE("UPDATE profile SET name = '",H66,"', points = ",I66," WHERE id =",G66,";")</f>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12156;</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Kriegspferd', points = 3 WHERE id =12156;</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
       <c r="A67">
         <v>8</v>
       </c>
@@ -4263,15 +4539,18 @@
       <c r="G67">
         <v>12078</v>
       </c>
+      <c r="H67" t="s">
+        <v>621</v>
+      </c>
       <c r="I67" s="5" t="s">
-        <v>1</v>
+        <v>622</v>
       </c>
       <c r="J67" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12078;</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Basis', points = 5 WHERE id =12078;</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
       <c r="A68">
         <v>8</v>
       </c>
@@ -4293,15 +4572,18 @@
       <c r="G68">
         <v>12129</v>
       </c>
+      <c r="H68" t="s">
+        <v>594</v>
+      </c>
       <c r="I68" s="5" t="s">
-        <v>1</v>
+        <v>630</v>
       </c>
       <c r="J68" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12129;</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Salvenkanone', points = 85 WHERE id =12129;</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
       <c r="A69">
         <v>8</v>
       </c>
@@ -4323,15 +4605,18 @@
       <c r="G69">
         <v>11888</v>
       </c>
+      <c r="H69" t="s">
+        <v>627</v>
+      </c>
       <c r="I69" s="5" t="s">
-        <v>1</v>
+        <v>628</v>
       </c>
       <c r="J69" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11888;</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Imperium Halbling', points = 3.5 WHERE id =11888;</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
       <c r="A70">
         <v>8</v>
       </c>
@@ -4353,15 +4638,18 @@
       <c r="G70">
         <v>12130</v>
       </c>
+      <c r="H70" t="s">
+        <v>596</v>
+      </c>
       <c r="I70" s="5" t="s">
-        <v>1</v>
+        <v>633</v>
       </c>
       <c r="J70" t="str">
         <f t="shared" si="1"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =12130;</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+        <v>UPDATE profile SET name = 'Suppenkatapult', points = 39.5 WHERE id =12130;</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
       <c r="A71">
         <v>8</v>
       </c>
@@ -4390,7 +4678,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10">
       <c r="A72">
         <v>8</v>
       </c>
@@ -4419,7 +4707,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10">
       <c r="A73">
         <v>8</v>
       </c>
@@ -4448,7 +4736,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10">
       <c r="A74">
         <v>8</v>
       </c>
@@ -4477,7 +4765,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10">
       <c r="A75">
         <v>8</v>
       </c>
@@ -4506,7 +4794,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10">
       <c r="A76">
         <v>8</v>
       </c>
@@ -4535,7 +4823,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10">
       <c r="A77">
         <v>8</v>
       </c>
@@ -4564,7 +4852,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10">
       <c r="A78">
         <v>8</v>
       </c>
@@ -4593,7 +4881,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10">
       <c r="A79">
         <v>8</v>
       </c>
@@ -4622,7 +4910,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10">
       <c r="A80">
         <v>8</v>
       </c>
@@ -4651,7 +4939,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9">
       <c r="A81">
         <v>8</v>
       </c>
@@ -4680,7 +4968,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9">
       <c r="A82">
         <v>8</v>
       </c>
@@ -4709,7 +4997,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9">
       <c r="A83">
         <v>8</v>
       </c>
@@ -4738,7 +5026,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9">
       <c r="A84">
         <v>8</v>
       </c>
@@ -4767,7 +5055,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9">
       <c r="A85">
         <v>8</v>
       </c>
@@ -4796,7 +5084,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9">
       <c r="A86">
         <v>8</v>
       </c>
@@ -4825,7 +5113,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9">
       <c r="A87">
         <v>8</v>
       </c>
@@ -4854,7 +5142,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9">
       <c r="A88">
         <v>8</v>
       </c>
@@ -4883,7 +5171,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9">
       <c r="A89">
         <v>8</v>
       </c>
@@ -4912,7 +5200,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9">
       <c r="A90">
         <v>8</v>
       </c>
@@ -4955,20 +5243,20 @@
       <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.75" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="A1" s="3" t="s">
         <v>110</v>
       </c>
@@ -4997,7 +5285,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>9</v>
       </c>
@@ -5030,7 +5318,7 @@
         <v>UPDATE profile SET name = 'Orks Grom der Fettsack vom Nebelberg', points = 78 WHERE id =11421;</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>9</v>
       </c>
@@ -5063,7 +5351,7 @@
         <v>UPDATE profile SET name = 'Orks Niblit', points = 65.0 WHERE id =11791;</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>9</v>
       </c>
@@ -5096,7 +5384,7 @@
         <v>UPDATE profile SET name = 'Orks Riesenwolf', points = 4.0 WHERE id =11841;</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>9</v>
       </c>
@@ -5129,7 +5417,7 @@
         <v>UPDATE profile SET name = 'Orks Gorbad Eisenfaust', points = 110 WHERE id =11422;</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>9</v>
       </c>
@@ -5162,7 +5450,7 @@
         <v>UPDATE profile SET name = 'Orks Morglum Knochenbrecher', points = 147 WHERE id =11423;</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>9</v>
       </c>
@@ -5195,7 +5483,7 @@
         <v>UPDATE profile SET name = 'Orks Oglock der Fürchtaliche', points = 87 WHERE id =11424;</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>9</v>
       </c>
@@ -5228,7 +5516,7 @@
         <v>UPDATE profile SET name = 'Orks Skarsnik Herrscher der Acht Gipfel', points = 78 WHERE id =11425;</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>9</v>
       </c>
@@ -5261,7 +5549,7 @@
         <v>UPDATE profile SET name = 'Orks Gobbla', points = 50.0 WHERE id =11792;</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5294,7 +5582,7 @@
         <v>UPDATE profile SET name = 'Orks Ork Chefoberboss', points = 110.0 WHERE id =11426;</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>9</v>
       </c>
@@ -5327,7 +5615,7 @@
         <v>UPDATE profile SET name = 'Orks Schwarzork Chefoberboss', points = 140.0 WHERE id =11427;</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>9</v>
       </c>
@@ -5360,7 +5648,7 @@
         <v>UPDATE profile SET name = 'Orks Wildork Chefoberboss', points = 150.0 WHERE id =11428;</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>9</v>
       </c>
@@ -5393,7 +5681,7 @@
         <v>UPDATE profile SET name = 'Orks Goblin Chefoberboss', points = 50.0 WHERE id =11429;</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>9</v>
       </c>
@@ -5426,7 +5714,7 @@
         <v>UPDATE profile SET name = 'Orks Waldgoblin Chefoberboss', points = 50.0 WHERE id =11430;</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>9</v>
       </c>
@@ -5459,7 +5747,7 @@
         <v>UPDATE profile SET name = 'Orks Nachtgoblin Chefoberboss', points = 50.0 WHERE id =11431;</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>9</v>
       </c>
@@ -5492,7 +5780,7 @@
         <v>UPDATE profile SET name = 'Orks Schwarzork Armeestandarte', points = 92.0 WHERE id =11432;</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>9</v>
       </c>
@@ -5525,7 +5813,7 @@
         <v>UPDATE profile SET name = 'Orks Ork Armeestandarte', points = 83.0 WHERE id =11433;</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>9</v>
       </c>
@@ -5558,7 +5846,7 @@
         <v>UPDATE profile SET name = 'Orks Wildork Armeestandarte', points = 95.0 WHERE id =11434;</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>9</v>
       </c>
@@ -5591,7 +5879,7 @@
         <v>UPDATE profile SET name = 'Orks Goblin Armeestandarte', points = 65.0 WHERE id =11435;</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>9</v>
       </c>
@@ -5624,7 +5912,7 @@
         <v>UPDATE profile SET name = 'Orks Waldgoblin Armeestandarte', points = 65.0 WHERE id =11436;</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>9</v>
       </c>
@@ -5657,7 +5945,7 @@
         <v>UPDATE profile SET name = 'Orks Nachtgoblin Armeestandarte', points = 65.0 WHERE id =11437;</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>9</v>
       </c>
@@ -5690,7 +5978,7 @@
         <v>UPDATE profile SET name = 'Orks Schwarzork Oberboss', points = 91.0 WHERE id =11438;</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>9</v>
       </c>
@@ -5723,7 +6011,7 @@
         <v>UPDATE profile SET name = 'Orks Ork Oberboss', points = 72.0 WHERE id =11439;</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>9</v>
       </c>
@@ -5756,7 +6044,7 @@
         <v>UPDATE profile SET name = 'Orks Wildork Oberboss', points = 98.0 WHERE id =11440;</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>9</v>
       </c>
@@ -5789,7 +6077,7 @@
         <v>UPDATE profile SET name = 'Orks Goblin Oberboss', points = 33.0 WHERE id =11441;</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>9</v>
       </c>
@@ -5822,7 +6110,7 @@
         <v>UPDATE profile SET name = 'Orks Waldgoblin Oberboss', points = 33.0 WHERE id =11442;</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>9</v>
       </c>
@@ -5855,7 +6143,7 @@
         <v>UPDATE profile SET name = 'Orks Nachtgoblin Oberboss', points = 33.0 WHERE id =11443;</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>9</v>
       </c>
@@ -5888,7 +6176,7 @@
         <v>UPDATE profile SET name = 'Orks Schwarzork Boss', points = 42.0 WHERE id =11444;</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>9</v>
       </c>
@@ -5921,7 +6209,7 @@
         <v>UPDATE profile SET name = 'Orks Ork Boss', points = 33.0 WHERE id =11445;</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>9</v>
       </c>
@@ -5954,7 +6242,7 @@
         <v>UPDATE profile SET name = 'Orks Wildork Boss', points = 33.0 WHERE id =11446;</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>9</v>
       </c>
@@ -5987,7 +6275,7 @@
         <v>UPDATE profile SET name = 'Orks Goblin Boss', points = 15.0 WHERE id =11447;</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>9</v>
       </c>
@@ -6020,7 +6308,7 @@
         <v>UPDATE profile SET name = 'Orks Waldgoblin Boss', points = 15.0 WHERE id =11448;</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10">
       <c r="A33">
         <v>9</v>
       </c>
@@ -6053,7 +6341,7 @@
         <v>UPDATE profile SET name = 'Orks Nachtgoblin Boss', points = 15.0 WHERE id =11449;</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10">
       <c r="A34">
         <v>9</v>
       </c>
@@ -6086,7 +6374,7 @@
         <v>UPDATE profile SET name = 'Orks Ork Schamane', points = 56.0 WHERE id =11450;</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10">
       <c r="A35">
         <v>9</v>
       </c>
@@ -6119,7 +6407,7 @@
         <v>UPDATE profile SET name = 'Orks Wildork Schamane', points = 59.0 WHERE id =11451;</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10">
       <c r="A36">
         <v>9</v>
       </c>
@@ -6152,7 +6440,7 @@
         <v>UPDATE profile SET name = 'Orks Goblin Schamane', points = 28.0 WHERE id =11452;</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10">
       <c r="A37">
         <v>9</v>
       </c>
@@ -6185,7 +6473,7 @@
         <v>UPDATE profile SET name = 'Orks Nachtgoblin Schamane', points = 28.0 WHERE id =11453;</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10">
       <c r="A38">
         <v>9</v>
       </c>
@@ -6218,7 +6506,7 @@
         <v>UPDATE profile SET name = 'Orks Waldgoblin Schamane', points = 28.0 WHERE id =11454;</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10">
       <c r="A39">
         <v>9</v>
       </c>
@@ -6251,7 +6539,7 @@
         <v>UPDATE profile SET name = 'Orks Ork Oberschamane', points = 118.0 WHERE id =11455;</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10">
       <c r="A40">
         <v>9</v>
       </c>
@@ -6284,7 +6572,7 @@
         <v>UPDATE profile SET name = 'Orks Wildork Oberschamane', points = 122.0 WHERE id =11456;</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10">
       <c r="A41">
         <v>9</v>
       </c>
@@ -6317,7 +6605,7 @@
         <v>UPDATE profile SET name = 'Orks Goblin Oberschamane', points = 83.0 WHERE id =11457;</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10">
       <c r="A42">
         <v>9</v>
       </c>
@@ -6350,7 +6638,7 @@
         <v>UPDATE profile SET name = 'Orks Nachtgoblin Oberschamane', points = 83.0 WHERE id =11458;</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10">
       <c r="A43">
         <v>9</v>
       </c>
@@ -6383,7 +6671,7 @@
         <v>UPDATE profile SET name = 'Orks Waldgoblin Oberschamane', points = 83.0 WHERE id =11459;</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10">
       <c r="A44">
         <v>9</v>
       </c>
@@ -6416,7 +6704,7 @@
         <v>UPDATE profile SET name = 'Orks Ork Großschamane', points = 190.0 WHERE id =11460;</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10">
       <c r="A45">
         <v>9</v>
       </c>
@@ -6449,7 +6737,7 @@
         <v>UPDATE profile SET name = 'Orks Wildork Großschamane', points = 219.0 WHERE id =11461;</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10">
       <c r="A46">
         <v>9</v>
       </c>
@@ -6482,7 +6770,7 @@
         <v>UPDATE profile SET name = 'Orks Goblin Großschamane', points = 159.0 WHERE id =11462;</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10">
       <c r="A47">
         <v>9</v>
       </c>
@@ -6515,7 +6803,7 @@
         <v>UPDATE profile SET name = 'Orks Nachtgoblin Großschamane', points = 159.0 WHERE id =11463;</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10">
       <c r="A48">
         <v>9</v>
       </c>
@@ -6548,7 +6836,7 @@
         <v>UPDATE profile SET name = 'Orks Waldgoblin Großschamane', points = 159.0 WHERE id =11464;</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10">
       <c r="A49">
         <v>9</v>
       </c>
@@ -6581,7 +6869,7 @@
         <v>UPDATE profile SET name = 'Orks Ork Meisterschamane', points = 287.0 WHERE id =11465;</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10">
       <c r="A50">
         <v>9</v>
       </c>
@@ -6614,7 +6902,7 @@
         <v>UPDATE profile SET name = 'Orks Wildork Meisterschamane', points = 303.0 WHERE id =11466;</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10">
       <c r="A51">
         <v>9</v>
       </c>
@@ -6647,7 +6935,7 @@
         <v>UPDATE profile SET name = 'Orks Goblin Meisterschamane', points = 253.0 WHERE id =11467;</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10">
       <c r="A52">
         <v>9</v>
       </c>
@@ -6680,7 +6968,7 @@
         <v>UPDATE profile SET name = 'Orks Nachtgoblin Meisterschamane', points = 253.0 WHERE id =11468;</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10">
       <c r="A53">
         <v>9</v>
       </c>
@@ -6713,7 +7001,7 @@
         <v>UPDATE profile SET name = 'Orks Waldgoblin Meisterschamane', points = 253.0 WHERE id =11469;</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10">
       <c r="A54">
         <v>9</v>
       </c>
@@ -6746,7 +7034,7 @@
         <v>UPDATE profile SET name = 'Orks Gorfan Rotzahn', points = 87 WHERE id =11586;</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10">
       <c r="A55">
         <v>9</v>
       </c>
@@ -6779,7 +7067,7 @@
         <v>UPDATE profile SET name = 'Orks Azhag der Vernichter', points = 127 WHERE id =11643;</v>
       </c>
     </row>
-    <row r="56" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" s="2" customFormat="1">
       <c r="A56" s="2">
         <v>9</v>
       </c>
@@ -6812,7 +7100,7 @@
         <v>UPDATE profile SET name = 'Lindwurm', points = 180.0 WHERE id =12423;</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10">
       <c r="A57">
         <v>9</v>
       </c>
@@ -6845,7 +7133,7 @@
         <v>UPDATE profile SET name = 'Orks Wildork Basis', points = 6.5 WHERE id =11850;</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10">
       <c r="A58">
         <v>9</v>
       </c>
@@ -6878,7 +7166,7 @@
         <v>UPDATE profile SET name = 'Orks Wildschwein', points = 8 WHERE id =12023;</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10">
       <c r="A59">
         <v>9</v>
       </c>
@@ -6911,7 +7199,7 @@
         <v>UPDATE profile SET name = 'Orks Ork Basis', points = 5.5 WHERE id =11851;</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10">
       <c r="A60">
         <v>9</v>
       </c>
@@ -6944,7 +7232,7 @@
         <v>UPDATE profile SET name = 'Orks Wildschwein', points = 8 WHERE id =12023;</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10">
       <c r="A61">
         <v>9</v>
       </c>
@@ -6977,7 +7265,7 @@
         <v>UPDATE profile SET name = 'Orks Riesenwolf', points = 4.0 WHERE id =11841;</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10">
       <c r="A62">
         <v>9</v>
       </c>
@@ -7010,7 +7298,7 @@
         <v>UPDATE profile SET name = 'Orks Goblin Basis', points = 2.5 WHERE id =11852;</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10">
       <c r="A63">
         <v>9</v>
       </c>
@@ -7043,7 +7331,7 @@
         <v>UPDATE profile SET name = 'Orks Waldgoblin Basis', points = 2.5 WHERE id =11853;</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10">
       <c r="A64">
         <v>9</v>
       </c>
@@ -7076,7 +7364,7 @@
         <v>UPDATE profile SET name = 'Orks Riesenspinne', points = 6.5 WHERE id =12026;</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10">
       <c r="A65">
         <v>9</v>
       </c>
@@ -7109,7 +7397,7 @@
         <v>UPDATE profile SET name = 'Orks Grobgitz Basis', points = 6.5 WHERE id =11854;</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10">
       <c r="A66">
         <v>9</v>
       </c>
@@ -7142,7 +7430,7 @@
         <v>UPDATE profile SET name = 'Orks Ork Basis', points = 5.5 WHERE id =11855;</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10">
       <c r="A67">
         <v>9</v>
       </c>
@@ -7175,7 +7463,7 @@
         <v>UPDATE profile SET name = 'Orks Ork Basis', points = 5.5 WHERE id =11856;</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10">
       <c r="A68">
         <v>9</v>
       </c>
@@ -7208,7 +7496,7 @@
         <v>UPDATE profile SET name = 'Orks Schwarzork Basis', points = 8.0 WHERE id =11857;</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10">
       <c r="A69">
         <v>9</v>
       </c>
@@ -7241,7 +7529,7 @@
         <v>UPDATE profile SET name = 'Orks Wildork Basis', points = 6.5 WHERE id =11858;</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10">
       <c r="A70">
         <v>9</v>
       </c>
@@ -7274,7 +7562,7 @@
         <v>UPDATE profile SET name = 'Orks Goblin Basis', points = 2.5 WHERE id =11852;</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10">
       <c r="A71">
         <v>9</v>
       </c>
@@ -7307,7 +7595,7 @@
         <v>UPDATE profile SET name = 'Orks Waldgoblin Basis', points = 2.5 WHERE id =11853;</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10">
       <c r="A72">
         <v>9</v>
       </c>
@@ -7340,7 +7628,7 @@
         <v>UPDATE profile SET name = 'Orks Nachtgoblin Basis', points = 2.5 WHERE id =11861;</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10">
       <c r="A73">
         <v>9</v>
       </c>
@@ -7373,7 +7661,7 @@
         <v>UPDATE profile SET name = 'Orks Nachtgoblin Basis', points = 2.5 WHERE id =11862;</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10">
       <c r="A74">
         <v>9</v>
       </c>
@@ -7406,7 +7694,7 @@
         <v>UPDATE profile SET name = 'Orks Höhlensquig', points = 20.0 WHERE id =12027;</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10">
       <c r="A75">
         <v>9</v>
       </c>
@@ -7439,7 +7727,7 @@
         <v>UPDATE profile SET name = 'Orks Nachtgoblin Basis', points = 2.5 WHERE id =11863;</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10">
       <c r="A76">
         <v>9</v>
       </c>
@@ -7472,7 +7760,7 @@
         <v>UPDATE profile SET name = 'Orks Fanatic', points = 30.0 WHERE id =11864;</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10">
       <c r="A77">
         <v>9</v>
       </c>
@@ -7505,7 +7793,7 @@
         <v>UPDATE profile SET name = 'Orks Nachtgoblin Basis', points = 2.5 WHERE id =11861;</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10">
       <c r="A78">
         <v>9</v>
       </c>
@@ -7538,7 +7826,7 @@
         <v>UPDATE profile SET name = 'Orks Höhlensquig', points = 20.0 WHERE id =12028;</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10">
       <c r="A79">
         <v>9</v>
       </c>
@@ -7571,7 +7859,7 @@
         <v>UPDATE profile SET name = 'Orks Riese', points = 200.0 WHERE id =11866;</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10">
       <c r="A80">
         <v>9</v>
       </c>
@@ -7604,7 +7892,7 @@
         <v>UPDATE profile SET name = 'Orks Oger', points = 40.0 WHERE id =11867;</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10">
       <c r="A81">
         <v>9</v>
       </c>
@@ -7637,7 +7925,7 @@
         <v>UPDATE profile SET name = 'Orks Flußtroll', points = 65.0 WHERE id =11868;</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10">
       <c r="A82">
         <v>9</v>
       </c>
@@ -7670,7 +7958,7 @@
         <v>UPDATE profile SET name = 'Orks Steintroll', points = 65.0 WHERE id =11869;</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10">
       <c r="A83">
         <v>9</v>
       </c>
@@ -7703,7 +7991,7 @@
         <v>UPDATE profile SET name = 'Orks Snotling-Base', points = 15.0 WHERE id =11870;</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10">
       <c r="A84">
         <v>9</v>
       </c>
@@ -7736,7 +8024,7 @@
         <v>UPDATE profile SET name = 'Orks Ork Basis', points = 5.5 WHERE id =12071;</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10">
       <c r="A85">
         <v>9</v>
       </c>
@@ -7769,7 +8057,7 @@
         <v>UPDATE profile SET name = 'Kleine Steinschleuder', points = 50.0 WHERE id =12133;</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10">
       <c r="A86">
         <v>9</v>
       </c>
@@ -7802,7 +8090,7 @@
         <v>UPDATE profile SET name = 'Orks Ork Basis', points = 5.5 WHERE id =12071;</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10">
       <c r="A87">
         <v>9</v>
       </c>
@@ -7835,7 +8123,7 @@
         <v>UPDATE profile SET name = 'Große Steinschleuder', points = 80.0 WHERE id =12134;</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10">
       <c r="A88">
         <v>9</v>
       </c>
@@ -7868,7 +8156,7 @@
         <v>UPDATE profile SET name = 'Orks Ork Basis', points = 5.5 WHERE id =12071;</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10">
       <c r="A89">
         <v>9</v>
       </c>
@@ -7901,7 +8189,7 @@
         <v>UPDATE profile SET name = 'Speerschleuder', points = 30.0 WHERE id =12132;</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10">
       <c r="A90">
         <v>9</v>
       </c>
@@ -7934,7 +8222,7 @@
         <v>UPDATE profile SET name = 'Orks Snotling-Base', points = 15.0 WHERE id =12074;</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10">
       <c r="A91">
         <v>9</v>
       </c>
@@ -7967,7 +8255,7 @@
         <v>UPDATE profile SET name = 'Orks Kurbelwagen', points = 25.0 WHERE id =12122;</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10">
       <c r="A92">
         <v>9</v>
       </c>
@@ -8000,7 +8288,7 @@
         <v>UPDATE profile SET name = 'Orks Goblin Basis', points = 2.5 WHERE id =12075;</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10">
       <c r="A93">
         <v>9</v>
       </c>
@@ -8033,7 +8321,7 @@
         <v>UPDATE profile SET name = 'Orks Kamikaze Katapult', points = 97.5 WHERE id =12123;</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10">
       <c r="A94">
         <v>9</v>
       </c>
@@ -8066,7 +8354,7 @@
         <v>UPDATE profile SET name = 'Orks Wildschwein', points = 8 WHERE id =12023;</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10">
       <c r="A95">
         <v>9</v>
       </c>
@@ -8099,7 +8387,7 @@
         <v>UPDATE profile SET name = 'Orks Ork Basis', points = 5.5 WHERE id =12076;</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:10">
       <c r="A96">
         <v>9</v>
       </c>
@@ -8132,7 +8420,7 @@
         <v>UPDATE profile SET name = 'Streitwagen', points = 50.0 WHERE id =12159;</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10">
       <c r="A97">
         <v>9</v>
       </c>
@@ -8165,7 +8453,7 @@
         <v>UPDATE profile SET name = 'Orks Riesenwolf', points = 4.0 WHERE id =11841;</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10">
       <c r="A98">
         <v>9</v>
       </c>
@@ -8198,7 +8486,7 @@
         <v>UPDATE profile SET name = 'Orks Goblin Basis', points = 2.5 WHERE id =11852;</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10">
       <c r="A99">
         <v>9</v>
       </c>
@@ -8231,7 +8519,7 @@
         <v>UPDATE profile SET name = 'Streitwagen', points = 50.0 WHERE id =12159;</v>
       </c>
     </row>
-    <row r="100" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:10" s="2" customFormat="1">
       <c r="A100" s="2">
         <v>9</v>
       </c>
@@ -8260,7 +8548,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="101" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:10" s="2" customFormat="1">
       <c r="A101" s="2">
         <v>9</v>
       </c>
@@ -8289,7 +8577,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="102" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:10" s="2" customFormat="1">
       <c r="A102" s="2">
         <v>9</v>
       </c>
@@ -8318,7 +8606,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="103" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:10" s="2" customFormat="1">
       <c r="A103" s="2">
         <v>9</v>
       </c>
@@ -8347,7 +8635,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="104" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:10" s="2" customFormat="1">
       <c r="A104" s="2">
         <v>9</v>
       </c>
@@ -8376,7 +8664,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="105" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:10" s="2" customFormat="1">
       <c r="A105" s="2">
         <v>9</v>
       </c>
@@ -8405,7 +8693,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="106" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:10" s="2" customFormat="1">
       <c r="A106" s="2">
         <v>9</v>
       </c>
@@ -8434,7 +8722,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="107" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:10" s="2" customFormat="1">
       <c r="A107" s="2">
         <v>9</v>
       </c>
@@ -8463,7 +8751,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="108" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:10" s="2" customFormat="1">
       <c r="A108" s="2">
         <v>9</v>
       </c>
@@ -8492,7 +8780,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="109" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:10" s="2" customFormat="1">
       <c r="A109" s="2">
         <v>9</v>
       </c>
@@ -8521,7 +8809,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="110" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:10" s="2" customFormat="1">
       <c r="A110" s="2">
         <v>9</v>
       </c>
@@ -8550,7 +8838,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="111" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:10" s="2" customFormat="1">
       <c r="A111" s="2">
         <v>9</v>
       </c>
@@ -8579,7 +8867,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="112" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:10" s="2" customFormat="1">
       <c r="A112" s="2">
         <v>9</v>
       </c>
@@ -8608,7 +8896,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="113" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" s="2" customFormat="1">
       <c r="A113" s="2">
         <v>9</v>
       </c>
@@ -8637,7 +8925,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="114" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" s="2" customFormat="1">
       <c r="A114" s="2">
         <v>9</v>
       </c>
@@ -8666,7 +8954,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="115" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" s="2" customFormat="1">
       <c r="A115" s="2">
         <v>9</v>
       </c>
@@ -8695,7 +8983,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="116" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" s="2" customFormat="1">
       <c r="A116" s="2">
         <v>9</v>
       </c>
@@ -8724,7 +9012,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="117" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" s="2" customFormat="1">
       <c r="A117" s="2">
         <v>9</v>
       </c>
@@ -8753,7 +9041,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="118" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" s="2" customFormat="1">
       <c r="A118" s="2">
         <v>9</v>
       </c>
@@ -8798,18 +9086,18 @@
       <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="A1" s="3" t="s">
         <v>110</v>
       </c>
@@ -8838,7 +9126,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>14</v>
       </c>
@@ -8871,7 +9159,7 @@
         <v>UPDATE profile SET name = 'Zwerge König Kazador', points = 174.0 WHERE id =11470;</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>14</v>
       </c>
@@ -8904,7 +9192,7 @@
         <v>UPDATE profile SET name = 'Zwerge Ungrim Eisenfaust', points = 210.0 WHERE id =11471;</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>14</v>
       </c>
@@ -8937,7 +9225,7 @@
         <v>UPDATE profile SET name = 'Zwerge Kragg', points = 309.0 WHERE id =11472;</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>14</v>
       </c>
@@ -8970,7 +9258,7 @@
         <v>UPDATE profile SET name = 'Zwerge Gotrek', points = 225.0 WHERE id =11473;</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>14</v>
       </c>
@@ -9003,7 +9291,7 @@
         <v>UPDATE profile SET name = 'Zwerge Felix', points = 77.0 WHERE id =11793;</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>14</v>
       </c>
@@ -9036,7 +9324,7 @@
         <v>UPDATE profile SET name = 'Zwerge Thorgrim Grollbart', points = 160.0 WHERE id =11474;</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>14</v>
       </c>
@@ -9069,7 +9357,7 @@
         <v>UPDATE profile SET name = 'Zwerge Thronträger', points = 35.0 WHERE id =11794;</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>14</v>
       </c>
@@ -9102,7 +9390,7 @@
         <v>UPDATE profile SET name = 'Zwerge Josef Bugman', points = 111.0 WHERE id =11475;</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>14</v>
       </c>
@@ -9135,7 +9423,7 @@
         <v>UPDATE profile SET name = 'Zwerge Burlock Damminson', points = 130.0 WHERE id =11476;</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>14</v>
       </c>
@@ -9168,7 +9456,7 @@
         <v>UPDATE profile SET name = 'Zwerge General', points = 160.0 WHERE id =11697;</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>14</v>
       </c>
@@ -9201,7 +9489,7 @@
         <v>UPDATE profile SET name = 'Zwerge Armeestandarte', points = 98.0 WHERE id =11478;</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>14</v>
       </c>
@@ -9234,7 +9522,7 @@
         <v>UPDATE profile SET name = 'Zwerge Held', points = 104.0 WHERE id =11701;</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>14</v>
       </c>
@@ -9267,7 +9555,7 @@
         <v>UPDATE profile SET name = 'Zwerge Champion', points = 48.0 WHERE id =11704;</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>14</v>
       </c>
@@ -9300,7 +9588,7 @@
         <v>UPDATE profile SET name = 'Zwerge Riesenslayer', points = 63.0 WHERE id =11481;</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>14</v>
       </c>
@@ -9333,7 +9621,7 @@
         <v>UPDATE profile SET name = 'Zwerge Drachenslayer', points = 136.0 WHERE id =11482;</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>14</v>
       </c>
@@ -9366,7 +9654,7 @@
         <v>UPDATE profile SET name = 'Zwerge Dämonenslayer', points = 210.0 WHERE id =11483;</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>14</v>
       </c>
@@ -9399,7 +9687,7 @@
         <v>UPDATE profile SET name = 'Zwerge Runenschmied', points = 78.0 WHERE id =11484;</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>14</v>
       </c>
@@ -9432,7 +9720,7 @@
         <v>UPDATE profile SET name = 'Zwerge Runenmeister', points = 187.0 WHERE id =11485;</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>14</v>
       </c>
@@ -9465,7 +9753,7 @@
         <v>UPDATE profile SET name = 'Zwerge Runengroßmeister', points = 306.0 WHERE id =11486;</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>14</v>
       </c>
@@ -9498,7 +9786,7 @@
         <v>UPDATE profile SET name = 'Zwerge Krudd der Rebell', points = 69.0 WHERE id =11644;</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>14</v>
       </c>
@@ -9531,7 +9819,7 @@
         <v>UPDATE profile SET name = 'Zwerge Grung Grollbringer', points = 187.0 WHERE id =11645;</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>14</v>
       </c>
@@ -9564,7 +9852,7 @@
         <v>UPDATE profile SET name = 'Zwerge Skag der Verstohlene', points = 107.0 WHERE id =11646;</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>14</v>
       </c>
@@ -9597,7 +9885,7 @@
         <v>UPDATE profile SET name = 'Zwerge Drong der Harte', points = 121.0 WHERE id =11647;</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>14</v>
       </c>
@@ -9630,7 +9918,7 @@
         <v>UPDATE profile SET name = 'Zwerge Helgar Langzopf', points = 158.0 WHERE id =11648;</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>14</v>
       </c>
@@ -9663,7 +9951,7 @@
         <v>UPDATE profile SET name = 'Zwerge Loki Weissbart', points = 113.0 WHERE id =11649;</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>14</v>
       </c>
@@ -9696,7 +9984,7 @@
         <v>UPDATE profile SET name = 'Zwerge Grombrindal der White Dwarf', points = 180.0 WHERE id =11650;</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>14</v>
       </c>
@@ -9729,7 +10017,7 @@
         <v>UPDATE profile SET name = 'Zwerge Elite', points = 11.0 WHERE id =11890;</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>14</v>
       </c>
@@ -9762,7 +10050,7 @@
         <v>UPDATE profile SET name = 'Zwerge Elite', points = 11.0 WHERE id =11891;</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>14</v>
       </c>
@@ -9795,7 +10083,7 @@
         <v>UPDATE profile SET name = 'Zwerge Elite', points = 11.0 WHERE id =11892;</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>14</v>
       </c>
@@ -9828,7 +10116,7 @@
         <v>UPDATE profile SET name = 'Zwerge Basis', points = 8.0 WHERE id =11893;</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>14</v>
       </c>
@@ -9861,7 +10149,7 @@
         <v>UPDATE profile SET name = 'Zwerge Basis', points = 8.0 WHERE id =11894;</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10">
       <c r="A33">
         <v>14</v>
       </c>
@@ -9894,7 +10182,7 @@
         <v>UPDATE profile SET name = 'Zwerge Basis', points = 8.0 WHERE id =11895;</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10">
       <c r="A34">
         <v>14</v>
       </c>
@@ -9927,7 +10215,7 @@
         <v>UPDATE profile SET name = 'Zwerge Basis', points = 8.0 WHERE id =11896;</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10">
       <c r="A35">
         <v>14</v>
       </c>
@@ -9960,7 +10248,7 @@
         <v>UPDATE profile SET name = 'Zwerge Slayer', points = 11.0 WHERE id =11897;</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10">
       <c r="A36">
         <v>14</v>
       </c>
@@ -9993,7 +10281,7 @@
         <v>UPDATE profile SET name = 'Zwerge Basis', points = 8.0 WHERE id =12084;</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10">
       <c r="A37">
         <v>14</v>
       </c>
@@ -10026,7 +10314,7 @@
         <v>UPDATE profile SET name = 'Gyrokopter', points = 92.0 WHERE id =12131;</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10">
       <c r="A38">
         <v>14</v>
       </c>
@@ -10059,7 +10347,7 @@
         <v>UPDATE profile SET name = 'Zwerge Basis', points = 8.0 WHERE id =12085;</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10">
       <c r="A39">
         <v>14</v>
       </c>
@@ -10092,7 +10380,7 @@
         <v>UPDATE profile SET name = 'Speerschleuder', points = 30.0 WHERE id =12132;</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10">
       <c r="A40">
         <v>14</v>
       </c>
@@ -10125,7 +10413,7 @@
         <v>UPDATE profile SET name = 'Zwerge Basis', points = 8.0 WHERE id =12085;</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10">
       <c r="A41">
         <v>14</v>
       </c>
@@ -10158,7 +10446,7 @@
         <v>UPDATE profile SET name = 'Kleine Steinschleuder', points = 50.0 WHERE id =12133;</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10">
       <c r="A42">
         <v>14</v>
       </c>
@@ -10191,7 +10479,7 @@
         <v>UPDATE profile SET name = 'Zwerge Basis', points = 8.0 WHERE id =12085;</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10">
       <c r="A43">
         <v>14</v>
       </c>
@@ -10224,7 +10512,7 @@
         <v>UPDATE profile SET name = 'Große Steinschleuder', points = 80.0 WHERE id =12134;</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10">
       <c r="A44">
         <v>14</v>
       </c>
@@ -10257,7 +10545,7 @@
         <v>UPDATE profile SET name = 'Zwerge Basis', points = 8.0 WHERE id =12085;</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10">
       <c r="A45">
         <v>14</v>
       </c>
@@ -10290,7 +10578,7 @@
         <v>UPDATE profile SET name = 'Flammenkanone', points = 95.0 WHERE id =12135;</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10">
       <c r="A46">
         <v>14</v>
       </c>
@@ -10323,7 +10611,7 @@
         <v>UPDATE profile SET name = 'Zwerge Basis', points = 8.0 WHERE id =12085;</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10">
       <c r="A47">
         <v>14</v>
       </c>
@@ -10356,7 +10644,7 @@
         <v>UPDATE profile SET name = 'Orgelkanone', points = 40.0 WHERE id =12136;</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10">
       <c r="A48">
         <v>14</v>
       </c>
@@ -10389,7 +10677,7 @@
         <v>UPDATE profile SET name = 'Zwerge Basis', points = 8.0 WHERE id =12085;</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10">
       <c r="A49">
         <v>14</v>
       </c>
@@ -10422,7 +10710,7 @@
         <v>UPDATE profile SET name = 'Kanone', points = 80.0 WHERE id =12137;</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10">
       <c r="A50">
         <v>14</v>
       </c>
@@ -10455,7 +10743,7 @@
         <v>UPDATE profile SET name = 'Lindwurm', points = 180.0 WHERE id =12423;</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10">
       <c r="A51">
         <v>14</v>
       </c>
@@ -10488,7 +10776,7 @@
         <v>UPDATE profile SET name = 'Hydra', points = 225.0 WHERE id =12421;</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10">
       <c r="A52">
         <v>14</v>
       </c>
@@ -10521,7 +10809,7 @@
         <v>UPDATE profile SET name = 'Riesenskorpion', points = 50.0 WHERE id =12314;</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10">
       <c r="A53">
         <v>14</v>
       </c>
@@ -10554,7 +10842,7 @@
         <v>UPDATE profile SET name = 'Rattenschwarm', points = 100.0 WHERE id =12320;</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10">
       <c r="A54">
         <v>14</v>
       </c>
@@ -10587,7 +10875,7 @@
         <v>UPDATE profile SET name = 'Froschschwarm', points = 100.0 WHERE id =12315;</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10">
       <c r="A55">
         <v>14</v>
       </c>
@@ -10620,7 +10908,7 @@
         <v>UPDATE profile SET name = 'Eidechsenschwarm', points = 100.0 WHERE id =12316;</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10">
       <c r="A56">
         <v>14</v>
       </c>
@@ -10653,7 +10941,7 @@
         <v>UPDATE profile SET name = 'Fledermausschwarm', points = 100.0 WHERE id =12321;</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10">
       <c r="A57">
         <v>14</v>
       </c>
@@ -10686,7 +10974,7 @@
         <v>UPDATE profile SET name = 'Schlangenschwarm', points = 100.0 WHERE id =12410;</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10">
       <c r="A58">
         <v>14</v>
       </c>
@@ -10719,7 +11007,7 @@
         <v>UPDATE profile SET name = 'Insekten-/Spinnenschwarm', points = 100.0 WHERE id =12411;</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10">
       <c r="A59">
         <v>14</v>
       </c>
@@ -10752,7 +11040,7 @@
         <v>UPDATE profile SET name = 'Skorpionschwarm', points = 100.0 WHERE id =12412;</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10">
       <c r="A60">
         <v>14</v>
       </c>
@@ -10785,7 +11073,7 @@
         <v>UPDATE profile SET name = 'Gigantenspinne', points = 50.0 WHERE id =12311;</v>
       </c>
     </row>
-    <row r="61" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" s="1" customFormat="1">
       <c r="A61" s="1">
         <v>14</v>
       </c>
@@ -10814,7 +11102,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="62" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" s="1" customFormat="1">
       <c r="A62" s="1">
         <v>14</v>
       </c>
@@ -10843,7 +11131,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="63" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" s="1" customFormat="1">
       <c r="A63" s="1">
         <v>14</v>
       </c>
@@ -10872,7 +11160,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="64" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" s="1" customFormat="1">
       <c r="A64" s="1">
         <v>14</v>
       </c>
@@ -10901,7 +11189,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="65" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" s="1" customFormat="1">
       <c r="A65" s="1">
         <v>14</v>
       </c>
@@ -10930,7 +11218,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="66" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" s="1" customFormat="1">
       <c r="A66" s="1">
         <v>14</v>
       </c>
@@ -10959,7 +11247,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="67" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" s="1" customFormat="1">
       <c r="A67" s="1">
         <v>14</v>
       </c>
@@ -10988,7 +11276,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="68" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" s="1" customFormat="1">
       <c r="A68" s="1">
         <v>14</v>
       </c>
@@ -11031,14 +11319,14 @@
       <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
     <col min="4" max="4" width="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="A1" s="3" t="s">
         <v>110</v>
       </c>
@@ -11067,7 +11355,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>5</v>
       </c>
@@ -11100,7 +11388,7 @@
         <v>UPDATE profile SET name = 'Elfen General', points = 160.0 WHERE id =11506;</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>5</v>
       </c>
@@ -11133,7 +11421,7 @@
         <v>UPDATE profile SET name = 'Elfen Champion', points = 48 WHERE id =11509;</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>5</v>
       </c>
@@ -11166,7 +11454,7 @@
         <v>UPDATE profile SET name = 'Elfen Held', points = 104.0 WHERE id =11508;</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>5</v>
       </c>
@@ -11199,7 +11487,7 @@
         <v>UPDATE profile SET name = 'Dunkelelfen Hexenheldin', points = 132 WHERE id =11571;</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>5</v>
       </c>
@@ -11232,7 +11520,7 @@
         <v>UPDATE profile SET name = 'Elfen Champion', points = 48.0 WHERE id =11509;</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>5</v>
       </c>
@@ -11265,7 +11553,7 @@
         <v>UPDATE profile SET name = 'Dunkelelfen Hexenchampion', points = 62 WHERE id =11573;</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>5</v>
       </c>
@@ -11298,7 +11586,7 @@
         <v>UPDATE profile SET name = 'Elfen Zauberer', points = 59.0 WHERE id =11510;</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>5</v>
       </c>
@@ -11331,7 +11619,7 @@
         <v>UPDATE profile SET name = 'Elfen Oberzauberer', points = 121.0 WHERE id =11511;</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>5</v>
       </c>
@@ -11364,7 +11652,7 @@
         <v>UPDATE profile SET name = 'Elfen Großzauberer', points = 219.0 WHERE id =11512;</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>5</v>
       </c>
@@ -11397,7 +11685,7 @@
         <v>UPDATE profile SET name = 'Elfen Meisterzauberer', points = 328.0 WHERE id =11513;</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>5</v>
       </c>
@@ -11430,7 +11718,7 @@
         <v>UPDATE profile SET name = 'Dunkelelfen Malekith', points = 350 WHERE id =11578;</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>5</v>
       </c>
@@ -11463,7 +11751,7 @@
         <v>UPDATE profile SET name = 'Dunkelelfen Kampfechse', points = 10 WHERE id =11810;</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>5</v>
       </c>
@@ -11496,7 +11784,7 @@
         <v>UPDATE profile SET name = 'Dunkelelfen Schwarzer Streitwagen', points = 70 WHERE id =11844;</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>5</v>
       </c>
@@ -11529,7 +11817,7 @@
         <v>UPDATE profile SET name = 'Dunkelelfen Rakarth', points = 134 WHERE id =11579;</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>5</v>
       </c>
@@ -11562,7 +11850,7 @@
         <v>UPDATE profile SET name = 'Dunkelelfen Schwarzer Drache', points = 450 WHERE id =11811;</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>5</v>
       </c>
@@ -11595,7 +11883,7 @@
         <v>UPDATE profile SET name = 'Dunkelelfen Morati', points = 327 WHERE id =11580;</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>5</v>
       </c>
@@ -11628,7 +11916,7 @@
         <v>UPDATE profile SET name = 'Dunkelelfen Schwarzer Pegasus', points = 50 WHERE id =12166;</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>5</v>
       </c>
@@ -11661,7 +11949,7 @@
         <v>UPDATE profile SET name = 'Dunkelelfen Kouran', points = 105 WHERE id =11581;</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>5</v>
       </c>
@@ -11694,7 +11982,7 @@
         <v>UPDATE profile SET name = 'Dunkelelfen Helleborn', points = 207 WHERE id =11582;</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>5</v>
       </c>
@@ -11727,7 +12015,7 @@
         <v>UPDATE profile SET name = 'Dunkelelfen Mantikor', points = 200 WHERE id =12335;</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>5</v>
       </c>
@@ -11760,7 +12048,7 @@
         <v>UPDATE profile SET name = 'Dunkelelfen Tullaris', points = 120 WHERE id =11583;</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>5</v>
       </c>
@@ -11793,7 +12081,7 @@
         <v>UPDATE profile SET name = 'Dunkelelfen Schattenklinge', points = 115 WHERE id =11584;</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>5</v>
       </c>
@@ -11826,7 +12114,7 @@
         <v>UPDATE profile SET name = 'Dunkelelfen Assassin', points = 56 WHERE id =11636;</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>5</v>
       </c>
@@ -11859,7 +12147,7 @@
         <v>UPDATE profile SET name = 'Elfen Elite', points = 10 WHERE id =11929;</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>5</v>
       </c>
@@ -11892,7 +12180,7 @@
         <v>UPDATE profile SET name = 'Dunkelelfen Kampfechse', points = 10 WHERE id =12041;</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>5</v>
       </c>
@@ -11925,7 +12213,7 @@
         <v>UPDATE profile SET name = 'Elfen Basis', points = 8 WHERE id =11930;</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>5</v>
       </c>
@@ -11958,7 +12246,7 @@
         <v>UPDATE profile SET name = 'Dunkelelfenroß', points = 3 WHERE id =12042;</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>5</v>
       </c>
@@ -11991,7 +12279,7 @@
         <v>UPDATE profile SET name = 'Elfen Elite', points = 10 WHERE id =11931;</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>5</v>
       </c>
@@ -12024,7 +12312,7 @@
         <v>UPDATE profile SET name = 'Elfen Elite', points = 10 WHERE id =11932;</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>5</v>
       </c>
@@ -12057,7 +12345,7 @@
         <v>UPDATE profile SET name = 'Elfen Basis', points = 8 WHERE id =11933;</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>5</v>
       </c>
@@ -12090,7 +12378,7 @@
         <v>UPDATE profile SET name = 'Elfen Basis', points = 8 WHERE id =11934;</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10">
       <c r="A33">
         <v>5</v>
       </c>
@@ -12123,7 +12411,7 @@
         <v>UPDATE profile SET name = 'Elfen Basis', points = 8 WHERE id =11935;</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10">
       <c r="A34">
         <v>5</v>
       </c>
@@ -12156,7 +12444,7 @@
         <v>UPDATE profile SET name = 'Elfen Basis', points = 8 WHERE id =11936;</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10">
       <c r="A35">
         <v>5</v>
       </c>
@@ -12189,7 +12477,7 @@
         <v>UPDATE profile SET name = 'Dunkelelfen Kundschafter', points = 10 WHERE id =11937;</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10">
       <c r="A36">
         <v>5</v>
       </c>
@@ -12222,7 +12510,7 @@
         <v>UPDATE profile SET name = 'Elfen Basis', points = 8 WHERE id =11938;</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10">
       <c r="A37">
         <v>5</v>
       </c>
@@ -12255,7 +12543,7 @@
         <v>UPDATE profile SET name = 'Elfen Basis', points = 8.0 WHERE id =11906;</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10">
       <c r="A38">
         <v>5</v>
       </c>
@@ -12288,7 +12576,7 @@
         <v>UPDATE profile SET name = 'Dunkelelfen Harpie', points = 15 WHERE id =12309;</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10">
       <c r="A39">
         <v>5</v>
       </c>
@@ -12321,7 +12609,7 @@
         <v>UPDATE profile SET name = 'Dunkelelfen Hexenchampion', points = 10 WHERE id =12107;</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10">
       <c r="A40">
         <v>5</v>
       </c>
@@ -12354,7 +12642,7 @@
         <v>UPDATE profile SET name = 'Elfen Basis', points = 8 WHERE id =12145;</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10">
       <c r="A41">
         <v>5</v>
       </c>
@@ -12387,7 +12675,7 @@
         <v>UPDATE profile SET name = 'Elfen Basis', points = 0.0 WHERE id =12108;</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10">
       <c r="A42">
         <v>5</v>
       </c>
@@ -12420,7 +12708,7 @@
         <v>UPDATE profile SET name = 'Repetier-Speerschleuder', points = 80 WHERE id =12146;</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10">
       <c r="A43">
         <v>5</v>
       </c>
@@ -12453,7 +12741,7 @@
         <v>UPDATE profile SET name = 'Schwarzer Pegasus', points = 50 WHERE id =12166;</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10">
       <c r="A44">
         <v>5</v>
       </c>
@@ -12486,7 +12774,7 @@
         <v>UPDATE profile SET name = 'Kriegshydra', points = 225 WHERE id =12168;</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10">
       <c r="A45" s="2">
         <v>5</v>
       </c>
@@ -12515,7 +12803,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10">
       <c r="A46" s="2">
         <v>5</v>
       </c>
@@ -12544,7 +12832,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10">
       <c r="A47" s="2">
         <v>5</v>
       </c>
@@ -12573,7 +12861,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10">
       <c r="A48" s="2">
         <v>5</v>
       </c>
@@ -12602,7 +12890,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9">
       <c r="A49" s="2">
         <v>5</v>
       </c>
@@ -12631,7 +12919,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9">
       <c r="A50" s="2">
         <v>5</v>
       </c>
@@ -12660,7 +12948,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9">
       <c r="A51" s="2">
         <v>5</v>
       </c>
@@ -12689,7 +12977,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9">
       <c r="A52" s="2">
         <v>5</v>
       </c>
@@ -12718,7 +13006,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9">
       <c r="A53" s="2">
         <v>5</v>
       </c>
@@ -12747,7 +13035,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9">
       <c r="A54" s="2">
         <v>5</v>
       </c>
@@ -12776,7 +13064,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9">
       <c r="A55" s="2">
         <v>5</v>
       </c>
@@ -12805,7 +13093,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9">
       <c r="A56" s="2">
         <v>5</v>
       </c>
@@ -12834,7 +13122,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9">
       <c r="A57" s="2">
         <v>5</v>
       </c>
@@ -12863,7 +13151,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9">
       <c r="A58" s="2">
         <v>5</v>
       </c>
@@ -12892,7 +13180,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9">
       <c r="A59" s="2">
         <v>5</v>
       </c>
@@ -12921,7 +13209,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9">
       <c r="A60" s="2">
         <v>5</v>
       </c>
@@ -12950,7 +13238,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9">
       <c r="A61" s="2">
         <v>5</v>
       </c>
@@ -12979,7 +13267,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9">
       <c r="A62" s="2">
         <v>5</v>
       </c>
@@ -13022,14 +13310,14 @@
       <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="45.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.88671875" customWidth="1"/>
+    <col min="2" max="2" width="45.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>112</v>
       </c>
@@ -13049,7 +13337,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>11693</v>
       </c>
@@ -13073,7 +13361,7 @@
         <v>UPDATE profile SET name = 'Immerkönigin' WHERE id = '11693';</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>11692</v>
       </c>
@@ -13097,7 +13385,7 @@
         <v>UPDATE profile SET name = 'General' WHERE id = '11692';</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>11507</v>
       </c>
@@ -13121,7 +13409,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Champion' WHERE id = '11507';</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>12243</v>
       </c>
@@ -13145,7 +13433,7 @@
         <v>UPDATE profile SET name = 'Basilisk' WHERE id = '12415';</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>11694</v>
       </c>
@@ -13169,7 +13457,7 @@
         <v>UPDATE profile SET name = 'Belannaer' WHERE id = '11694';</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>11906</v>
       </c>
@@ -13193,7 +13481,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '11906';</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>12591</v>
       </c>
@@ -13217,7 +13505,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12591';</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>12472</v>
       </c>
@@ -13241,7 +13529,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12472';</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>11696</v>
       </c>
@@ -13265,7 +13553,7 @@
         <v>UPDATE profile SET name = 'Caradryan' WHERE id = '11696';</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>11509</v>
       </c>
@@ -13289,7 +13577,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Champion' WHERE id = '11509';</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>12236</v>
       </c>
@@ -13313,7 +13601,7 @@
         <v>UPDATE profile SET name = 'Chimäre' WHERE id = '12414';</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>12286</v>
       </c>
@@ -13337,7 +13625,7 @@
         <v>UPDATE profile SET name = 'Drache' WHERE id = '12416';</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>11900</v>
       </c>
@@ -13361,7 +13649,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '11900';</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>12585</v>
       </c>
@@ -13385,7 +13673,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '12585';</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>12466</v>
       </c>
@@ -13409,7 +13697,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '12466';</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>12163</v>
       </c>
@@ -13433,7 +13721,7 @@
         <v>UPDATE profile SET name = 'Einhorn' WHERE id = '12163';</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>11898</v>
       </c>
@@ -13457,7 +13745,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '11898';</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7">
       <c r="A19">
         <v>12583</v>
       </c>
@@ -13481,7 +13769,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12583';</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7">
       <c r="A20">
         <v>12464</v>
       </c>
@@ -13505,7 +13793,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12464';</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7">
       <c r="A21">
         <v>11516</v>
       </c>
@@ -13529,7 +13817,7 @@
         <v>UPDATE profile SET name = 'Greif' WHERE id = '11516';</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7">
       <c r="A22">
         <v>11516</v>
       </c>
@@ -13553,7 +13841,7 @@
         <v>UPDATE profile SET name = 'Hochelfen General' WHERE id = '11804';</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7">
       <c r="A23">
         <v>11506</v>
       </c>
@@ -13577,7 +13865,7 @@
         <v>UPDATE profile SET name = 'Hochelfen General' WHERE id = '11506';</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7">
       <c r="A24">
         <v>12269</v>
       </c>
@@ -13601,7 +13889,7 @@
         <v>UPDATE profile SET name = 'Greif' WHERE id = '12419';</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7">
       <c r="A25">
         <v>12294</v>
       </c>
@@ -13625,7 +13913,7 @@
         <v>UPDATE profile SET name = 'Großer Drache' WHERE id = '12417';</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7">
       <c r="A26">
         <v>11512</v>
       </c>
@@ -13649,7 +13937,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Großzauberer' WHERE id = '11512';</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7">
       <c r="A27">
         <v>11508</v>
       </c>
@@ -13673,7 +13961,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Held' WHERE id = '11508';</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7">
       <c r="A28">
         <v>12278</v>
       </c>
@@ -13697,7 +13985,7 @@
         <v>UPDATE profile SET name = 'Hippogreif' WHERE id = '12420';</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7">
       <c r="A29">
         <v>11980</v>
       </c>
@@ -13721,7 +14009,7 @@
         <v>UPDATE profile SET name = 'Jungferngarde' WHERE id = '11980';</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7">
       <c r="A30">
         <v>12637</v>
       </c>
@@ -13745,7 +14033,7 @@
         <v>UPDATE profile SET name = 'Jungferngarde' WHERE id = '12637';</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7">
       <c r="A31">
         <v>12518</v>
       </c>
@@ -13769,7 +14057,7 @@
         <v>UPDATE profile SET name = 'Jungferngarde' WHERE id = '12518';</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7">
       <c r="A32">
         <v>12302</v>
       </c>
@@ -13793,7 +14081,7 @@
         <v>UPDATE profile SET name = 'Kaiserdrache' WHERE id = '12418';</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7">
       <c r="A33">
         <v>11695</v>
       </c>
@@ -13817,7 +14105,7 @@
         <v>UPDATE profile SET name = 'Korhil' WHERE id = '11695';</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7">
       <c r="A34">
         <v>12250</v>
       </c>
@@ -13841,7 +14129,7 @@
         <v>UPDATE profile SET name = 'Mantikor' WHERE id = '12422';</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7">
       <c r="A35">
         <v>11513</v>
       </c>
@@ -13865,7 +14153,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Meisterzauberer' WHERE id = '11513';</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7">
       <c r="A36">
         <v>11511</v>
       </c>
@@ -13889,7 +14177,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Oberzauberer' WHERE id = '11511';</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7">
       <c r="A37">
         <v>12167</v>
       </c>
@@ -13913,7 +14201,7 @@
         <v>UPDATE profile SET name = 'Pegasus' WHERE id = '12336';</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7">
       <c r="A38">
         <v>11902</v>
       </c>
@@ -13937,7 +14225,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '11902';</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7">
       <c r="A39">
         <v>12587</v>
       </c>
@@ -13961,7 +14249,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '12587';</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7">
       <c r="A40">
         <v>12468</v>
       </c>
@@ -13985,7 +14273,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '12468';</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7">
       <c r="A41">
         <v>11517</v>
       </c>
@@ -14009,7 +14297,7 @@
         <v>UPDATE profile SET name = 'Prinz Imrik' WHERE id = '11517';</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7">
       <c r="A42">
         <v>12091</v>
       </c>
@@ -14033,7 +14321,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12091';</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7">
       <c r="A43">
         <v>12091</v>
       </c>
@@ -14057,7 +14345,7 @@
         <v>UPDATE profile SET name = 'Speerschleuder' WHERE id = '12138';</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7">
       <c r="A44">
         <v>12162</v>
       </c>
@@ -14081,7 +14369,7 @@
         <v>UPDATE profile SET name = 'Riesenadler' WHERE id = '12162';</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7">
       <c r="A45">
         <v>11907</v>
       </c>
@@ -14105,7 +14393,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '11907';</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7">
       <c r="A46">
         <v>12592</v>
       </c>
@@ -14129,7 +14417,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12592';</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7">
       <c r="A47">
         <v>12473</v>
       </c>
@@ -14153,7 +14441,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12473';</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7">
       <c r="A48">
         <v>11901</v>
       </c>
@@ -14177,7 +14465,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '11901';</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7">
       <c r="A49">
         <v>12586</v>
       </c>
@@ -14201,7 +14489,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '12586';</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7">
       <c r="A50">
         <v>12467</v>
       </c>
@@ -14225,7 +14513,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '12467';</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7">
       <c r="A51">
         <v>11905</v>
       </c>
@@ -14249,7 +14537,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '11905';</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7">
       <c r="A52">
         <v>12590</v>
       </c>
@@ -14273,7 +14561,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12590';</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7">
       <c r="A53">
         <v>12471</v>
       </c>
@@ -14297,7 +14585,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12471';</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7">
       <c r="A54">
         <v>11899</v>
       </c>
@@ -14321,7 +14609,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '11899';</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7">
       <c r="A55">
         <v>12584</v>
       </c>
@@ -14345,7 +14633,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '12584';</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7">
       <c r="A56">
         <v>12465</v>
       </c>
@@ -14369,7 +14657,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '12465';</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7">
       <c r="A57">
         <v>11904</v>
       </c>
@@ -14393,7 +14681,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '11904';</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7">
       <c r="A58">
         <v>12589</v>
       </c>
@@ -14417,7 +14705,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12589';</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7">
       <c r="A59">
         <v>12470</v>
       </c>
@@ -14441,7 +14729,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12470';</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7">
       <c r="A60">
         <v>11515</v>
       </c>
@@ -14465,7 +14753,7 @@
         <v>UPDATE profile SET name = 'Teclis' WHERE id = '11515';</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7">
       <c r="A61">
         <v>12113</v>
       </c>
@@ -14489,7 +14777,7 @@
         <v>UPDATE profile SET name = 'Streitwagen' WHERE id = '12159';</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7">
       <c r="A62">
         <v>12113</v>
       </c>
@@ -14513,7 +14801,7 @@
         <v>UPDATE profile SET name = 'Streitwagen' WHERE id = '12113';</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7">
       <c r="A63">
         <v>12118</v>
       </c>
@@ -14537,7 +14825,7 @@
         <v>UPDATE profile SET name = 'Streitwagen' WHERE id = '12160';</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7">
       <c r="A64">
         <v>12118</v>
       </c>
@@ -14561,7 +14849,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12113';</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7">
       <c r="A65">
         <v>11514</v>
       </c>
@@ -14585,7 +14873,7 @@
         <v>UPDATE profile SET name = 'Malhandir' WHERE id = '11803';</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7">
       <c r="A66">
         <v>11514</v>
       </c>
@@ -14609,7 +14897,7 @@
         <v>UPDATE profile SET name = 'Tyrion' WHERE id = '11514';</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7">
       <c r="A67">
         <v>11903</v>
       </c>
@@ -14633,7 +14921,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '11903';</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7">
       <c r="A68">
         <v>12588</v>
       </c>
@@ -14657,7 +14945,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '12588';</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7">
       <c r="A69">
         <v>12469</v>
       </c>
@@ -14681,7 +14969,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Elite' WHERE id = '12469';</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7">
       <c r="A70">
         <v>11510</v>
       </c>
@@ -14705,7 +14993,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Zauberer' WHERE id = '11510';</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7">
       <c r="A71">
         <v>11997</v>
       </c>
@@ -14729,7 +15017,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '11997';</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7">
       <c r="A72">
         <v>12652</v>
       </c>
@@ -14753,7 +15041,7 @@
         <v>UPDATE profile SET name = 'Hochelfen Basis' WHERE id = '12652';</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7">
       <c r="A73">
         <v>12533</v>
       </c>

</xml_diff>

<commit_message>
Updated profiles of Empire army list
</commit_message>
<xml_diff>
--- a/resources/db/Profiles.xlsx
+++ b/resources/db/Profiles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\projects\ArmyBuilder\sourcecode\resources\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{615C4764-397C-41DB-992F-12A4A7F362B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9900C29B-A2FF-42F3-8BBF-C85EA592122F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{72821A2A-92BA-4C26-854D-A2ECB76DE865}"/>
+    <workbookView xWindow="1560" yWindow="330" windowWidth="7725" windowHeight="15150" xr2:uid="{72821A2A-92BA-4C26-854D-A2ECB76DE865}"/>
   </bookViews>
   <sheets>
     <sheet name="Empire Profiles" sheetId="10" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1883" uniqueCount="639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1894" uniqueCount="653">
   <si>
     <t>General</t>
   </si>
@@ -1959,6 +1959,48 @@
   </si>
   <si>
     <t>70</t>
+  </si>
+  <si>
+    <t>Imperium Magnus</t>
+  </si>
+  <si>
+    <t>Imperium Ludwig Schwarzhelm</t>
+  </si>
+  <si>
+    <t>Imperium Volkmar</t>
+  </si>
+  <si>
+    <t>Imperium Kriegsaltar</t>
+  </si>
+  <si>
+    <t>Imperium Heiliger Patriarch</t>
+  </si>
+  <si>
+    <t>Imperium Kurt Helburg</t>
+  </si>
+  <si>
+    <t>Imperium Aldebrand Ludenhof</t>
+  </si>
+  <si>
+    <t>Imperium Valmir von Raukov</t>
+  </si>
+  <si>
+    <t>Imperium Marius Leitdorf</t>
+  </si>
+  <si>
+    <t>Imperium Boris Wüterich</t>
+  </si>
+  <si>
+    <t>210</t>
+  </si>
+  <si>
+    <t>290</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>Imperium Tzarnia</t>
   </si>
 </sst>
 </file>
@@ -2359,8 +2401,8 @@
   <dimension ref="A1:J90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I34" sqref="I34"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -2757,12 +2799,15 @@
       <c r="G12">
         <v>11496</v>
       </c>
+      <c r="H12" t="s">
+        <v>639</v>
+      </c>
       <c r="I12" s="5" t="s">
-        <v>1</v>
+        <v>649</v>
       </c>
       <c r="J12" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11496;</v>
+        <v>UPDATE profile SET name = 'Imperium Magnus', points = 210 WHERE id =11496;</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -2787,12 +2832,15 @@
       <c r="G13">
         <v>11497</v>
       </c>
+      <c r="H13" t="s">
+        <v>640</v>
+      </c>
       <c r="I13" s="5" t="s">
-        <v>1</v>
+        <v>638</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11497;</v>
+        <v>UPDATE profile SET name = 'Imperium Ludwig Schwarzhelm', points = 70 WHERE id =11497;</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -2850,12 +2898,15 @@
       <c r="G15">
         <v>11498</v>
       </c>
+      <c r="H15" t="s">
+        <v>641</v>
+      </c>
       <c r="I15" s="5" t="s">
-        <v>1</v>
+        <v>617</v>
       </c>
       <c r="J15" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11498;</v>
+        <v>UPDATE profile SET name = 'Imperium Volkmar', points = 150 WHERE id =11498;</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -2880,12 +2931,15 @@
       <c r="G16">
         <v>11842</v>
       </c>
+      <c r="H16" t="s">
+        <v>642</v>
+      </c>
       <c r="I16" s="5" t="s">
-        <v>1</v>
+        <v>598</v>
       </c>
       <c r="J16" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11842;</v>
+        <v>UPDATE profile SET name = 'Imperium Kriegsaltar', points = 100 WHERE id =11842;</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -2943,12 +2997,15 @@
       <c r="G18">
         <v>11499</v>
       </c>
+      <c r="H18" t="s">
+        <v>643</v>
+      </c>
       <c r="I18" s="5" t="s">
-        <v>1</v>
+        <v>650</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11499;</v>
+        <v>UPDATE profile SET name = 'Imperium Heiliger Patriarch', points = 290 WHERE id =11499;</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -2973,12 +3030,15 @@
       <c r="G19">
         <v>11500</v>
       </c>
+      <c r="H19" t="s">
+        <v>644</v>
+      </c>
       <c r="I19" s="5" t="s">
-        <v>1</v>
+        <v>537</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11500;</v>
+        <v>UPDATE profile SET name = 'Imperium Kurt Helburg', points = 110 WHERE id =11500;</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -3036,12 +3096,15 @@
       <c r="G21">
         <v>11502</v>
       </c>
+      <c r="H21" t="s">
+        <v>645</v>
+      </c>
       <c r="I21" s="5" t="s">
-        <v>1</v>
+        <v>651</v>
       </c>
       <c r="J21" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11502;</v>
+        <v>UPDATE profile SET name = 'Imperium Aldebrand Ludenhof', points = 90 WHERE id =11502;</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -3099,12 +3162,15 @@
       <c r="G23">
         <v>11503</v>
       </c>
+      <c r="H23" t="s">
+        <v>646</v>
+      </c>
       <c r="I23" s="5" t="s">
-        <v>1</v>
+        <v>651</v>
       </c>
       <c r="J23" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11503;</v>
+        <v>UPDATE profile SET name = 'Imperium Valmir von Raukov', points = 90 WHERE id =11503;</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -3162,12 +3228,15 @@
       <c r="G25">
         <v>11504</v>
       </c>
+      <c r="H25" t="s">
+        <v>647</v>
+      </c>
       <c r="I25" s="5" t="s">
-        <v>1</v>
+        <v>537</v>
       </c>
       <c r="J25" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11504;</v>
+        <v>UPDATE profile SET name = 'Imperium Marius Leitdorf', points = 110 WHERE id =11504;</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -3225,12 +3294,15 @@
       <c r="G27">
         <v>11505</v>
       </c>
+      <c r="H27" t="s">
+        <v>652</v>
+      </c>
       <c r="I27" s="5" t="s">
-        <v>1</v>
+        <v>631</v>
       </c>
       <c r="J27" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11505;</v>
+        <v>UPDATE profile SET name = 'Imperium Tzarnia', points = 200 WHERE id =11505;</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -3288,12 +3360,15 @@
       <c r="G29">
         <v>11640</v>
       </c>
+      <c r="H29" t="s">
+        <v>648</v>
+      </c>
       <c r="I29" s="5" t="s">
-        <v>1</v>
+        <v>651</v>
       </c>
       <c r="J29" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE profile SET name = '', points = 0.0 WHERE id =11640;</v>
+        <v>UPDATE profile SET name = 'Imperium Boris Wüterich', points = 90 WHERE id =11640;</v>
       </c>
     </row>
     <row r="30" spans="1:10">

</xml_diff>